<commit_message>
Update pearl log notes for 2021-03-23 testing
</commit_message>
<xml_diff>
--- a/pearl_logs/PEARL_MOOS_testing_notes.xlsx
+++ b/pearl_logs/PEARL_MOOS_testing_notes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maha/moos-ivp-pearl/pearl_logs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45842B30-B207-194D-A7F6-ADF062FDFED5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC35CBCB-A42D-9B42-A7BC-A51A05565F0E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6780" yWindow="460" windowWidth="18820" windowHeight="15540" xr2:uid="{CE7898E4-CB96-184C-9C00-2CBDA86B470B}"/>
+    <workbookView xWindow="12800" yWindow="460" windowWidth="12800" windowHeight="15540" xr2:uid="{CE7898E4-CB96-184C-9C00-2CBDA86B470B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="83">
   <si>
     <t>Date</t>
   </si>
@@ -138,6 +138,192 @@
   </si>
   <si>
     <t>next Yaw to 1.0, sent to waypoint and then returned home but kept spinning round</t>
+  </si>
+  <si>
+    <t>Waypoint - Star</t>
+  </si>
+  <si>
+    <t>Yaw_Kp</t>
+  </si>
+  <si>
+    <t>Yaw_Ki</t>
+  </si>
+  <si>
+    <t>Yaw_Kd</t>
+  </si>
+  <si>
+    <t>Speed_Kp</t>
+  </si>
+  <si>
+    <t>Speed_Ki</t>
+  </si>
+  <si>
+    <t>Did a three loops, issue with the IMU heading as recorded or used by MOOS?</t>
+  </si>
+  <si>
+    <t>Again did loops… If IMU heading is trash, can try to estimate based on GPS waypoints to construct your actual velocity vector and allows you to get your heading (works even if you don't have a dedicated compass or IMU)</t>
+  </si>
+  <si>
+    <t>Tighter loops</t>
+  </si>
+  <si>
+    <t>Still looping. Maybe something wrong with the heading</t>
+  </si>
+  <si>
+    <t>Re-running experiment 4 with new printouts for heading. IMU Heading values definitely off when in MOOS mode, but seem ok when did manual RC override</t>
+  </si>
+  <si>
+    <t>Try re-running slow moving but maybe successful mission from yesterday
+- did one loop at the start… some issue with IMU reading from Arduino lagging?</t>
+  </si>
+  <si>
+    <t>Try another spin, through MOOS, 50% thrust, delay a bit more - maybe 10 seconds</t>
+  </si>
+  <si>
+    <t>GPS now for heading, tried manual square mission</t>
+  </si>
+  <si>
+    <t>GPS now used for heading, simple striahgt line - to waypoint and then returned - did pretty good, some curved pattern but no loops!</t>
+  </si>
+  <si>
+    <t>Speed (m/s)</t>
+  </si>
+  <si>
+    <t>- overshot a little on the heading - probably because we only have proportional control
+- we bumped into her about 3:27pm
+- no damped at all
+- overshoot of heading is almost 90 degrees (wants 81 but goes to 170 and back) - quite severe</t>
+  </si>
+  <si>
+    <t>- did a bit better, so we won't remove Kp in future from yaw</t>
+  </si>
+  <si>
+    <t>- kept Yaw Kp same because responsiveness looks good, now add in derivative gain
+- we don't really care how fast she goes so OK that Speed Ki not used
+- she couldn't really settle in turns</t>
+  </si>
+  <si>
+    <t>- looked better, got to her waypoint, still need some damping out with yaw Kd</t>
+  </si>
+  <si>
+    <t>- oscillated to about 20 degrees away from desired heading?
+- made it to waypoint</t>
+  </si>
+  <si>
+    <t>- still oscillated, more than before? Maybe bump up D more</t>
+  </si>
+  <si>
+    <t>- a bit better</t>
+  </si>
+  <si>
+    <t>- now trying to add in some integral control
+- no oscillations!</t>
+  </si>
+  <si>
+    <t>- did really well before, now just trying more "symmetric" Ki and Kp for Yaw
+- oscillated just slightly in beginning but did really well! Happy with these. Now try patterns?</t>
+  </si>
+  <si>
+    <t>- had not commented out desired track info, restarting next without track leads
+- she's not ready yet with PID gains to follow track well</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- now leads commented out - wait was for wrong pattern </t>
+  </si>
+  <si>
+    <t>- NOW leads commented out for STAR pattern
+- still some slight oscillation. Ok to leave gains as they are now, but they are not completely optimized yet</t>
+  </si>
+  <si>
+    <t>- let's try more derivative and integral gain, oscillated a lot, too much P?</t>
+  </si>
+  <si>
+    <t>- did pretty well! Keep these gains and try star again</t>
+  </si>
+  <si>
+    <t>- did well on straight legs, on the 180 turns she had issues and overshot, so may need some more D but let's look at theoretical model first</t>
+  </si>
+  <si>
+    <t>LOG_PEARL_SIMPLE_23_3_2021_____09_55_00</t>
+  </si>
+  <si>
+    <t>LOG_PEARL_SIMPLE_23_3_2021_____10_10_47</t>
+  </si>
+  <si>
+    <t>LOG_PEARL_SIMPLE_23_3_2021_____10_17_52</t>
+  </si>
+  <si>
+    <t>LOG_PEARL_SIMPLE_23_3_2021_____10_24_30</t>
+  </si>
+  <si>
+    <t>LOG_PEARL_SIMPLE_23_3_2021_____10_35_18</t>
+  </si>
+  <si>
+    <t>LOG_PEARL_SIMPLE_23_3_2021_____10_49_35</t>
+  </si>
+  <si>
+    <t>LOG_PEARL_SIMPLE_23_3_2021_____10_58_13</t>
+  </si>
+  <si>
+    <t>LOG_PEARL_SIMPLE_23_3_2021_____11_17_21</t>
+  </si>
+  <si>
+    <t>Bump up derivative gain a bit more
+Tried doing some RC control to spin, estimate the delay to be 5 seconds
+slow turn took about 1 minute ended around 11:07 AM
+next turn - try a bit faster, also 5 seconds delay
+tried the fast spin again, 6.8 seconds</t>
+  </si>
+  <si>
+    <t>LOG_PEARL_SIMPLE_23_3_2021_____11_24_57</t>
+  </si>
+  <si>
+    <t>LOG_PEARL_SIMPLE_23_3_2021_____11_37_55</t>
+  </si>
+  <si>
+    <t>LOG_PEARL_SIMPLE_23_3_2021_____15_25_19</t>
+  </si>
+  <si>
+    <t>LOG_PEARL_SIMPLE_23_3_2021_____15_32_32</t>
+  </si>
+  <si>
+    <t>LOG_PEARL_SIMPLE_23_3_2021_____15_36_26</t>
+  </si>
+  <si>
+    <t>LOG_PEARL_SIMPLE_23_3_2021_____15_39_06</t>
+  </si>
+  <si>
+    <t>LOG_PEARL_SIMPLE_23_3_2021_____15_42_12</t>
+  </si>
+  <si>
+    <t>LOG_PEARL_SIMPLE_23_3_2021_____15_47_16</t>
+  </si>
+  <si>
+    <t>LOG_PEARL_SIMPLE_23_3_2021_____15_51_34</t>
+  </si>
+  <si>
+    <t>LOG_PEARL_SIMPLE_23_3_2021_____15_55_01</t>
+  </si>
+  <si>
+    <t>LOG_PEARL_SIMPLE_23_3_2021_____16_00_03</t>
+  </si>
+  <si>
+    <t>LOG_PEARL_WAYPOINT_23_3_2021_____16_09_17</t>
+  </si>
+  <si>
+    <t>LOG_PEARL_WAYPOINT_23_3_2021_____16_14_09</t>
+  </si>
+  <si>
+    <t>LOG_PEARL_WAYPOINT_23_3_2021_____16_16_26</t>
+  </si>
+  <si>
+    <t>LOG_PEARL_SQUARE_23_3_2021_____16_33_09</t>
+  </si>
+  <si>
+    <t>LOG_PEARL_WAYPOINT_23_3_2021_____16_47_05</t>
+  </si>
+  <si>
+    <t>LOG_PEARL_SQUARE_23_3_2021_____16_37_43</t>
   </si>
 </sst>
 </file>
@@ -181,7 +367,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -192,6 +378,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -506,10 +693,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C322D9A-DAA8-F94B-8299-5D36BBA36BB2}">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:K35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" topLeftCell="C21" workbookViewId="0">
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -517,10 +704,16 @@
     <col min="2" max="2" width="16.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="25.83203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="55.83203125" customWidth="1"/>
-    <col min="5" max="5" width="80.1640625" customWidth="1"/>
+    <col min="5" max="5" width="7.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.83203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.83203125" customWidth="1"/>
+    <col min="11" max="11" width="80.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -534,10 +727,28 @@
         <v>1</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" ht="34" x14ac:dyDescent="0.2">
       <c r="A2" s="5">
         <v>44277</v>
       </c>
@@ -550,11 +761,29 @@
       <c r="D2" t="s">
         <v>23</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2">
+        <v>0.1</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>1</v>
+      </c>
+      <c r="I2">
+        <v>1</v>
+      </c>
+      <c r="J2">
+        <v>0.3</v>
+      </c>
+      <c r="K2" s="2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="5">
         <v>44277</v>
       </c>
@@ -567,11 +796,29 @@
       <c r="D3" t="s">
         <v>21</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
+      </c>
+      <c r="I3">
+        <v>1</v>
+      </c>
+      <c r="J3">
+        <v>0.3</v>
+      </c>
+      <c r="K3" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="85" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" ht="85" x14ac:dyDescent="0.2">
       <c r="A4" s="5">
         <v>44277</v>
       </c>
@@ -584,11 +831,29 @@
       <c r="D4" t="s">
         <v>20</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="E4">
+        <v>0.5</v>
+      </c>
+      <c r="F4">
+        <v>0.5</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>1</v>
+      </c>
+      <c r="I4">
+        <v>1</v>
+      </c>
+      <c r="J4">
+        <v>0.3</v>
+      </c>
+      <c r="K4" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="68" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" ht="68" x14ac:dyDescent="0.2">
       <c r="A5" s="5">
         <v>44277</v>
       </c>
@@ -601,11 +866,29 @@
       <c r="D5" t="s">
         <v>19</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="E5">
+        <v>0.2</v>
+      </c>
+      <c r="F5">
+        <v>0.2</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>0.2</v>
+      </c>
+      <c r="I5">
+        <v>0.2</v>
+      </c>
+      <c r="J5">
+        <v>0.3</v>
+      </c>
+      <c r="K5" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="272" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" ht="272" x14ac:dyDescent="0.2">
       <c r="A6" s="5">
         <v>44277</v>
       </c>
@@ -618,11 +901,14 @@
       <c r="D6" t="s">
         <v>18</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="J6">
+        <v>0.3</v>
+      </c>
+      <c r="K6" s="4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="102" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" ht="102" x14ac:dyDescent="0.2">
       <c r="A7" s="5">
         <v>44277</v>
       </c>
@@ -635,11 +921,29 @@
       <c r="D7" t="s">
         <v>17</v>
       </c>
-      <c r="E7" s="4" t="s">
+      <c r="E7">
+        <v>0.25</v>
+      </c>
+      <c r="F7">
+        <v>0.2</v>
+      </c>
+      <c r="G7">
+        <v>0.1</v>
+      </c>
+      <c r="H7">
+        <v>0.2</v>
+      </c>
+      <c r="I7">
+        <v>0.2</v>
+      </c>
+      <c r="J7">
+        <v>0.3</v>
+      </c>
+      <c r="K7" s="4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" ht="34" x14ac:dyDescent="0.2">
       <c r="A8" s="5">
         <v>44277</v>
       </c>
@@ -652,11 +956,29 @@
       <c r="D8" t="s">
         <v>16</v>
       </c>
-      <c r="E8" s="4" t="s">
+      <c r="E8">
+        <v>0.4</v>
+      </c>
+      <c r="F8">
+        <v>0.2</v>
+      </c>
+      <c r="G8">
+        <v>0.1</v>
+      </c>
+      <c r="H8">
+        <v>0.6</v>
+      </c>
+      <c r="I8">
+        <v>0.2</v>
+      </c>
+      <c r="J8">
+        <v>0.3</v>
+      </c>
+      <c r="K8" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="136" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" ht="136" x14ac:dyDescent="0.2">
       <c r="A9" s="5">
         <v>44277</v>
       </c>
@@ -669,11 +991,29 @@
       <c r="D9" t="s">
         <v>15</v>
       </c>
-      <c r="E9" s="4" t="s">
+      <c r="E9">
+        <v>0.3</v>
+      </c>
+      <c r="F9">
+        <v>0.2</v>
+      </c>
+      <c r="G9">
+        <v>0.1</v>
+      </c>
+      <c r="H9">
+        <v>0.5</v>
+      </c>
+      <c r="I9">
+        <v>0.2</v>
+      </c>
+      <c r="J9">
+        <v>0.3</v>
+      </c>
+      <c r="K9" s="4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" ht="51" x14ac:dyDescent="0.2">
       <c r="A10" s="5">
         <v>44277</v>
       </c>
@@ -686,8 +1026,901 @@
       <c r="D10" t="s">
         <v>14</v>
       </c>
-      <c r="E10" s="2" t="s">
+      <c r="E10">
+        <v>0.3</v>
+      </c>
+      <c r="F10">
+        <v>0.2</v>
+      </c>
+      <c r="G10">
+        <v>0.1</v>
+      </c>
+      <c r="H10">
+        <v>0.5</v>
+      </c>
+      <c r="I10">
+        <v>0.2</v>
+      </c>
+      <c r="J10">
+        <v>0.3</v>
+      </c>
+      <c r="K10" s="2" t="s">
         <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A11" s="5">
+        <v>44278</v>
+      </c>
+      <c r="B11" s="3">
+        <v>0.41319444444444442</v>
+      </c>
+      <c r="C11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D11" t="s">
+        <v>57</v>
+      </c>
+      <c r="E11">
+        <v>0.25</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>0.25</v>
+      </c>
+      <c r="H11">
+        <v>0.5</v>
+      </c>
+      <c r="I11">
+        <v>0.75</v>
+      </c>
+      <c r="J11">
+        <v>0.3</v>
+      </c>
+      <c r="K11" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A12" s="5">
+        <v>44278</v>
+      </c>
+      <c r="B12" s="3">
+        <v>0.4236111111111111</v>
+      </c>
+      <c r="C12" t="s">
+        <v>6</v>
+      </c>
+      <c r="D12" t="s">
+        <v>58</v>
+      </c>
+      <c r="E12">
+        <v>0.25</v>
+      </c>
+      <c r="F12">
+        <v>0.25</v>
+      </c>
+      <c r="G12">
+        <v>0.5</v>
+      </c>
+      <c r="H12">
+        <v>0.75</v>
+      </c>
+      <c r="I12">
+        <v>1</v>
+      </c>
+      <c r="J12">
+        <v>0.3</v>
+      </c>
+      <c r="K12" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A13" s="5">
+        <v>44278</v>
+      </c>
+      <c r="B13" s="3">
+        <v>0.4284722222222222</v>
+      </c>
+      <c r="C13" t="s">
+        <v>6</v>
+      </c>
+      <c r="D13" t="s">
+        <v>59</v>
+      </c>
+      <c r="E13">
+        <v>0.25</v>
+      </c>
+      <c r="F13">
+        <v>0.5</v>
+      </c>
+      <c r="G13">
+        <v>0.75</v>
+      </c>
+      <c r="H13">
+        <v>1</v>
+      </c>
+      <c r="I13">
+        <v>0</v>
+      </c>
+      <c r="J13">
+        <v>0.3</v>
+      </c>
+      <c r="K13" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A14" s="5">
+        <v>44278</v>
+      </c>
+      <c r="B14" s="3">
+        <v>0.43333333333333335</v>
+      </c>
+      <c r="C14" t="s">
+        <v>6</v>
+      </c>
+      <c r="D14" t="s">
+        <v>60</v>
+      </c>
+      <c r="E14">
+        <v>0.25</v>
+      </c>
+      <c r="F14">
+        <v>1</v>
+      </c>
+      <c r="G14">
+        <v>0</v>
+      </c>
+      <c r="H14">
+        <v>0.25</v>
+      </c>
+      <c r="I14">
+        <v>0.5</v>
+      </c>
+      <c r="J14">
+        <v>0.3</v>
+      </c>
+      <c r="K14" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A15" s="5">
+        <v>44278</v>
+      </c>
+      <c r="B15" s="3">
+        <v>0.44097222222222227</v>
+      </c>
+      <c r="C15" t="s">
+        <v>6</v>
+      </c>
+      <c r="D15" t="s">
+        <v>61</v>
+      </c>
+      <c r="E15">
+        <v>0.25</v>
+      </c>
+      <c r="F15">
+        <v>1</v>
+      </c>
+      <c r="G15">
+        <v>0</v>
+      </c>
+      <c r="H15">
+        <v>0.25</v>
+      </c>
+      <c r="I15">
+        <v>0.5</v>
+      </c>
+      <c r="J15">
+        <v>0.3</v>
+      </c>
+      <c r="K15" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="34" x14ac:dyDescent="0.2">
+      <c r="A16" s="5">
+        <v>44278</v>
+      </c>
+      <c r="B16" s="3">
+        <v>0.45</v>
+      </c>
+      <c r="C16" t="s">
+        <v>6</v>
+      </c>
+      <c r="D16" t="s">
+        <v>62</v>
+      </c>
+      <c r="E16">
+        <v>0.25</v>
+      </c>
+      <c r="F16">
+        <v>0.2</v>
+      </c>
+      <c r="G16">
+        <v>0.1</v>
+      </c>
+      <c r="H16">
+        <v>0.5</v>
+      </c>
+      <c r="I16">
+        <v>0.2</v>
+      </c>
+      <c r="J16">
+        <v>0.3</v>
+      </c>
+      <c r="K16" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" ht="85" x14ac:dyDescent="0.2">
+      <c r="A17" s="5">
+        <v>44278</v>
+      </c>
+      <c r="B17" s="3">
+        <v>0.45624999999999999</v>
+      </c>
+      <c r="C17" t="s">
+        <v>6</v>
+      </c>
+      <c r="D17" t="s">
+        <v>63</v>
+      </c>
+      <c r="E17">
+        <v>0.25</v>
+      </c>
+      <c r="F17">
+        <v>0.2</v>
+      </c>
+      <c r="G17">
+        <v>0.2</v>
+      </c>
+      <c r="H17">
+        <v>0.5</v>
+      </c>
+      <c r="I17">
+        <v>0.2</v>
+      </c>
+      <c r="J17">
+        <v>0.3</v>
+      </c>
+      <c r="K17" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A18" s="5">
+        <v>44278</v>
+      </c>
+      <c r="B18" s="3">
+        <v>0.47013888888888888</v>
+      </c>
+      <c r="C18" t="s">
+        <v>6</v>
+      </c>
+      <c r="D18" t="s">
+        <v>64</v>
+      </c>
+      <c r="E18">
+        <v>0.25</v>
+      </c>
+      <c r="F18">
+        <v>0.2</v>
+      </c>
+      <c r="G18">
+        <v>0.1</v>
+      </c>
+      <c r="H18">
+        <v>0.5</v>
+      </c>
+      <c r="I18">
+        <v>0.2</v>
+      </c>
+      <c r="J18">
+        <v>0.3</v>
+      </c>
+      <c r="K18" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="A19" s="5">
+        <v>44278</v>
+      </c>
+      <c r="B19" s="3">
+        <v>0.47500000000000003</v>
+      </c>
+      <c r="C19" t="s">
+        <v>6</v>
+      </c>
+      <c r="D19" t="s">
+        <v>66</v>
+      </c>
+      <c r="E19">
+        <v>0.25</v>
+      </c>
+      <c r="F19">
+        <v>0.2</v>
+      </c>
+      <c r="G19">
+        <v>0.1</v>
+      </c>
+      <c r="H19">
+        <v>0.5</v>
+      </c>
+      <c r="I19">
+        <v>0.2</v>
+      </c>
+      <c r="J19">
+        <v>0.3</v>
+      </c>
+      <c r="K19" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A20" s="5">
+        <v>44278</v>
+      </c>
+      <c r="B20" s="3">
+        <v>0.48402777777777778</v>
+      </c>
+      <c r="C20" t="s">
+        <v>6</v>
+      </c>
+      <c r="D20" t="s">
+        <v>67</v>
+      </c>
+      <c r="E20">
+        <v>0.25</v>
+      </c>
+      <c r="F20">
+        <v>0.2</v>
+      </c>
+      <c r="G20">
+        <v>0.1</v>
+      </c>
+      <c r="H20">
+        <v>0.5</v>
+      </c>
+      <c r="I20">
+        <v>0.2</v>
+      </c>
+      <c r="J20">
+        <v>0.3</v>
+      </c>
+      <c r="K20" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" ht="66" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="5">
+        <v>44278</v>
+      </c>
+      <c r="B21" s="3">
+        <v>0.64166666666666672</v>
+      </c>
+      <c r="C21" t="s">
+        <v>6</v>
+      </c>
+      <c r="D21" t="s">
+        <v>68</v>
+      </c>
+      <c r="E21">
+        <v>1</v>
+      </c>
+      <c r="F21">
+        <v>0</v>
+      </c>
+      <c r="G21">
+        <v>0</v>
+      </c>
+      <c r="H21">
+        <v>1</v>
+      </c>
+      <c r="I21">
+        <v>0</v>
+      </c>
+      <c r="J21">
+        <v>0.5</v>
+      </c>
+      <c r="K21" s="4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A22" s="5">
+        <v>44278</v>
+      </c>
+      <c r="B22" s="3">
+        <v>0.64722222222222225</v>
+      </c>
+      <c r="C22" t="s">
+        <v>6</v>
+      </c>
+      <c r="D22" t="s">
+        <v>69</v>
+      </c>
+      <c r="E22">
+        <v>0.75</v>
+      </c>
+      <c r="F22">
+        <v>0</v>
+      </c>
+      <c r="G22">
+        <v>0</v>
+      </c>
+      <c r="H22">
+        <v>1</v>
+      </c>
+      <c r="I22">
+        <v>0</v>
+      </c>
+      <c r="J22">
+        <v>0.5</v>
+      </c>
+      <c r="K22" s="6" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" ht="51" x14ac:dyDescent="0.2">
+      <c r="A23" s="5">
+        <v>44278</v>
+      </c>
+      <c r="B23" s="3">
+        <v>0.65</v>
+      </c>
+      <c r="C23" t="s">
+        <v>6</v>
+      </c>
+      <c r="D23" t="s">
+        <v>70</v>
+      </c>
+      <c r="E23">
+        <v>0.75</v>
+      </c>
+      <c r="F23">
+        <v>0</v>
+      </c>
+      <c r="G23">
+        <v>0.25</v>
+      </c>
+      <c r="H23">
+        <v>1</v>
+      </c>
+      <c r="I23">
+        <v>0</v>
+      </c>
+      <c r="J23">
+        <v>0.5</v>
+      </c>
+      <c r="K23" s="4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A24" s="5">
+        <v>44278</v>
+      </c>
+      <c r="B24" s="3">
+        <v>0.65138888888888891</v>
+      </c>
+      <c r="C24" t="s">
+        <v>6</v>
+      </c>
+      <c r="D24" t="s">
+        <v>71</v>
+      </c>
+      <c r="E24">
+        <v>0.75</v>
+      </c>
+      <c r="F24">
+        <v>0</v>
+      </c>
+      <c r="G24">
+        <v>0.5</v>
+      </c>
+      <c r="H24">
+        <v>1</v>
+      </c>
+      <c r="I24">
+        <v>0</v>
+      </c>
+      <c r="J24">
+        <v>0.5</v>
+      </c>
+      <c r="K24" s="6" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" ht="34" x14ac:dyDescent="0.2">
+      <c r="A25" s="5">
+        <v>44278</v>
+      </c>
+      <c r="B25" s="3">
+        <v>0.65347222222222223</v>
+      </c>
+      <c r="C25" t="s">
+        <v>6</v>
+      </c>
+      <c r="D25" t="s">
+        <v>72</v>
+      </c>
+      <c r="E25">
+        <v>0.75</v>
+      </c>
+      <c r="F25">
+        <v>0</v>
+      </c>
+      <c r="G25">
+        <v>0.75</v>
+      </c>
+      <c r="H25">
+        <v>1</v>
+      </c>
+      <c r="I25">
+        <v>0</v>
+      </c>
+      <c r="J25">
+        <v>0.5</v>
+      </c>
+      <c r="K25" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A26" s="5">
+        <v>44278</v>
+      </c>
+      <c r="B26" s="3">
+        <v>0.65763888888888888</v>
+      </c>
+      <c r="C26" t="s">
+        <v>6</v>
+      </c>
+      <c r="D26" t="s">
+        <v>73</v>
+      </c>
+      <c r="E26">
+        <v>0.75</v>
+      </c>
+      <c r="F26">
+        <v>0</v>
+      </c>
+      <c r="G26">
+        <v>1</v>
+      </c>
+      <c r="H26">
+        <v>1</v>
+      </c>
+      <c r="I26">
+        <v>0</v>
+      </c>
+      <c r="J26">
+        <v>0.5</v>
+      </c>
+      <c r="K26" s="6" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="A27" s="5">
+        <v>44278</v>
+      </c>
+      <c r="B27" s="3">
+        <v>0.66041666666666665</v>
+      </c>
+      <c r="C27" t="s">
+        <v>6</v>
+      </c>
+      <c r="D27" t="s">
+        <v>74</v>
+      </c>
+      <c r="E27">
+        <v>0.75</v>
+      </c>
+      <c r="F27">
+        <v>0</v>
+      </c>
+      <c r="G27">
+        <v>1.5</v>
+      </c>
+      <c r="H27">
+        <v>1</v>
+      </c>
+      <c r="I27">
+        <v>0</v>
+      </c>
+      <c r="J27">
+        <v>0.5</v>
+      </c>
+      <c r="K27" s="4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" ht="34" x14ac:dyDescent="0.2">
+      <c r="A28" s="5">
+        <v>44278</v>
+      </c>
+      <c r="B28" s="3">
+        <v>0.66249999999999998</v>
+      </c>
+      <c r="C28" t="s">
+        <v>6</v>
+      </c>
+      <c r="D28" t="s">
+        <v>75</v>
+      </c>
+      <c r="E28">
+        <v>0.75</v>
+      </c>
+      <c r="F28">
+        <v>0.5</v>
+      </c>
+      <c r="G28">
+        <v>1.5</v>
+      </c>
+      <c r="H28">
+        <v>1</v>
+      </c>
+      <c r="I28">
+        <v>0</v>
+      </c>
+      <c r="J28">
+        <v>0.5</v>
+      </c>
+      <c r="K28" s="4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" ht="34" x14ac:dyDescent="0.2">
+      <c r="A29" s="5">
+        <v>44278</v>
+      </c>
+      <c r="B29" s="3">
+        <v>0.66597222222222219</v>
+      </c>
+      <c r="C29" t="s">
+        <v>6</v>
+      </c>
+      <c r="D29" t="s">
+        <v>76</v>
+      </c>
+      <c r="E29">
+        <v>0.75</v>
+      </c>
+      <c r="F29">
+        <v>0.75</v>
+      </c>
+      <c r="G29">
+        <v>1.5</v>
+      </c>
+      <c r="H29">
+        <v>1</v>
+      </c>
+      <c r="I29">
+        <v>0</v>
+      </c>
+      <c r="J29">
+        <v>0.5</v>
+      </c>
+      <c r="K29" s="4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" ht="34" x14ac:dyDescent="0.2">
+      <c r="A30" s="5">
+        <v>44278</v>
+      </c>
+      <c r="B30" s="3">
+        <v>0.67152777777777783</v>
+      </c>
+      <c r="C30" t="s">
+        <v>26</v>
+      </c>
+      <c r="D30" t="s">
+        <v>77</v>
+      </c>
+      <c r="E30">
+        <v>0.75</v>
+      </c>
+      <c r="F30">
+        <v>0.75</v>
+      </c>
+      <c r="G30">
+        <v>1.5</v>
+      </c>
+      <c r="H30">
+        <v>1</v>
+      </c>
+      <c r="I30">
+        <v>0</v>
+      </c>
+      <c r="J30">
+        <v>0.5</v>
+      </c>
+      <c r="K30" s="4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="A31" s="5">
+        <v>44278</v>
+      </c>
+      <c r="B31" s="3">
+        <v>0.67569444444444438</v>
+      </c>
+      <c r="C31" t="s">
+        <v>26</v>
+      </c>
+      <c r="D31" t="s">
+        <v>78</v>
+      </c>
+      <c r="E31">
+        <v>0.75</v>
+      </c>
+      <c r="F31">
+        <v>0.75</v>
+      </c>
+      <c r="G31">
+        <v>1.5</v>
+      </c>
+      <c r="H31">
+        <v>1</v>
+      </c>
+      <c r="I31">
+        <v>0</v>
+      </c>
+      <c r="J31">
+        <v>0.5</v>
+      </c>
+      <c r="K31" s="4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" ht="51" x14ac:dyDescent="0.2">
+      <c r="A32" s="5">
+        <v>44278</v>
+      </c>
+      <c r="B32" s="3">
+        <v>0.6777777777777777</v>
+      </c>
+      <c r="C32" t="s">
+        <v>26</v>
+      </c>
+      <c r="D32" t="s">
+        <v>79</v>
+      </c>
+      <c r="E32">
+        <v>0.75</v>
+      </c>
+      <c r="F32">
+        <v>0.75</v>
+      </c>
+      <c r="G32">
+        <v>1.5</v>
+      </c>
+      <c r="H32">
+        <v>1</v>
+      </c>
+      <c r="I32">
+        <v>0</v>
+      </c>
+      <c r="J32">
+        <v>0.5</v>
+      </c>
+      <c r="K32" s="4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="A33" s="5">
+        <v>44278</v>
+      </c>
+      <c r="B33" s="3">
+        <v>0.68958333333333333</v>
+      </c>
+      <c r="C33" t="s">
+        <v>9</v>
+      </c>
+      <c r="D33" t="s">
+        <v>80</v>
+      </c>
+      <c r="E33">
+        <v>1</v>
+      </c>
+      <c r="F33">
+        <v>4</v>
+      </c>
+      <c r="G33">
+        <v>2</v>
+      </c>
+      <c r="H33">
+        <v>1</v>
+      </c>
+      <c r="I33">
+        <v>0</v>
+      </c>
+      <c r="J33">
+        <v>0.5</v>
+      </c>
+      <c r="K33" s="4" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="A34" s="5">
+        <v>44278</v>
+      </c>
+      <c r="B34" s="3">
+        <v>0.69236111111111109</v>
+      </c>
+      <c r="C34" t="s">
+        <v>9</v>
+      </c>
+      <c r="D34" t="s">
+        <v>82</v>
+      </c>
+      <c r="E34">
+        <v>0.5</v>
+      </c>
+      <c r="F34">
+        <v>4</v>
+      </c>
+      <c r="G34">
+        <v>2</v>
+      </c>
+      <c r="H34">
+        <v>1</v>
+      </c>
+      <c r="I34">
+        <v>0</v>
+      </c>
+      <c r="J34">
+        <v>0.5</v>
+      </c>
+      <c r="K34" s="4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" ht="34" x14ac:dyDescent="0.2">
+      <c r="A35" s="5">
+        <v>44278</v>
+      </c>
+      <c r="B35" s="3">
+        <v>0.69930555555555562</v>
+      </c>
+      <c r="C35" t="s">
+        <v>26</v>
+      </c>
+      <c r="D35" t="s">
+        <v>81</v>
+      </c>
+      <c r="E35">
+        <v>0.5</v>
+      </c>
+      <c r="F35">
+        <v>4</v>
+      </c>
+      <c r="G35">
+        <v>2</v>
+      </c>
+      <c r="H35">
+        <v>1</v>
+      </c>
+      <c r="I35">
+        <v>0</v>
+      </c>
+      <c r="J35">
+        <v>0.5</v>
+      </c>
+      <c r="K35" s="4" t="s">
+        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Upload mission logs 2021-03-24 afternoon tests
</commit_message>
<xml_diff>
--- a/pearl_logs/PEARL_MOOS_testing_notes.xlsx
+++ b/pearl_logs/PEARL_MOOS_testing_notes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maha/moos-ivp-pearl/pearl_logs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45842B30-B207-194D-A7F6-ADF062FDFED5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC35CBCB-A42D-9B42-A7BC-A51A05565F0E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6780" yWindow="460" windowWidth="18820" windowHeight="15540" xr2:uid="{CE7898E4-CB96-184C-9C00-2CBDA86B470B}"/>
+    <workbookView xWindow="12800" yWindow="460" windowWidth="12800" windowHeight="15540" xr2:uid="{CE7898E4-CB96-184C-9C00-2CBDA86B470B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="83">
   <si>
     <t>Date</t>
   </si>
@@ -138,6 +138,192 @@
   </si>
   <si>
     <t>next Yaw to 1.0, sent to waypoint and then returned home but kept spinning round</t>
+  </si>
+  <si>
+    <t>Waypoint - Star</t>
+  </si>
+  <si>
+    <t>Yaw_Kp</t>
+  </si>
+  <si>
+    <t>Yaw_Ki</t>
+  </si>
+  <si>
+    <t>Yaw_Kd</t>
+  </si>
+  <si>
+    <t>Speed_Kp</t>
+  </si>
+  <si>
+    <t>Speed_Ki</t>
+  </si>
+  <si>
+    <t>Did a three loops, issue with the IMU heading as recorded or used by MOOS?</t>
+  </si>
+  <si>
+    <t>Again did loops… If IMU heading is trash, can try to estimate based on GPS waypoints to construct your actual velocity vector and allows you to get your heading (works even if you don't have a dedicated compass or IMU)</t>
+  </si>
+  <si>
+    <t>Tighter loops</t>
+  </si>
+  <si>
+    <t>Still looping. Maybe something wrong with the heading</t>
+  </si>
+  <si>
+    <t>Re-running experiment 4 with new printouts for heading. IMU Heading values definitely off when in MOOS mode, but seem ok when did manual RC override</t>
+  </si>
+  <si>
+    <t>Try re-running slow moving but maybe successful mission from yesterday
+- did one loop at the start… some issue with IMU reading from Arduino lagging?</t>
+  </si>
+  <si>
+    <t>Try another spin, through MOOS, 50% thrust, delay a bit more - maybe 10 seconds</t>
+  </si>
+  <si>
+    <t>GPS now for heading, tried manual square mission</t>
+  </si>
+  <si>
+    <t>GPS now used for heading, simple striahgt line - to waypoint and then returned - did pretty good, some curved pattern but no loops!</t>
+  </si>
+  <si>
+    <t>Speed (m/s)</t>
+  </si>
+  <si>
+    <t>- overshot a little on the heading - probably because we only have proportional control
+- we bumped into her about 3:27pm
+- no damped at all
+- overshoot of heading is almost 90 degrees (wants 81 but goes to 170 and back) - quite severe</t>
+  </si>
+  <si>
+    <t>- did a bit better, so we won't remove Kp in future from yaw</t>
+  </si>
+  <si>
+    <t>- kept Yaw Kp same because responsiveness looks good, now add in derivative gain
+- we don't really care how fast she goes so OK that Speed Ki not used
+- she couldn't really settle in turns</t>
+  </si>
+  <si>
+    <t>- looked better, got to her waypoint, still need some damping out with yaw Kd</t>
+  </si>
+  <si>
+    <t>- oscillated to about 20 degrees away from desired heading?
+- made it to waypoint</t>
+  </si>
+  <si>
+    <t>- still oscillated, more than before? Maybe bump up D more</t>
+  </si>
+  <si>
+    <t>- a bit better</t>
+  </si>
+  <si>
+    <t>- now trying to add in some integral control
+- no oscillations!</t>
+  </si>
+  <si>
+    <t>- did really well before, now just trying more "symmetric" Ki and Kp for Yaw
+- oscillated just slightly in beginning but did really well! Happy with these. Now try patterns?</t>
+  </si>
+  <si>
+    <t>- had not commented out desired track info, restarting next without track leads
+- she's not ready yet with PID gains to follow track well</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- now leads commented out - wait was for wrong pattern </t>
+  </si>
+  <si>
+    <t>- NOW leads commented out for STAR pattern
+- still some slight oscillation. Ok to leave gains as they are now, but they are not completely optimized yet</t>
+  </si>
+  <si>
+    <t>- let's try more derivative and integral gain, oscillated a lot, too much P?</t>
+  </si>
+  <si>
+    <t>- did pretty well! Keep these gains and try star again</t>
+  </si>
+  <si>
+    <t>- did well on straight legs, on the 180 turns she had issues and overshot, so may need some more D but let's look at theoretical model first</t>
+  </si>
+  <si>
+    <t>LOG_PEARL_SIMPLE_23_3_2021_____09_55_00</t>
+  </si>
+  <si>
+    <t>LOG_PEARL_SIMPLE_23_3_2021_____10_10_47</t>
+  </si>
+  <si>
+    <t>LOG_PEARL_SIMPLE_23_3_2021_____10_17_52</t>
+  </si>
+  <si>
+    <t>LOG_PEARL_SIMPLE_23_3_2021_____10_24_30</t>
+  </si>
+  <si>
+    <t>LOG_PEARL_SIMPLE_23_3_2021_____10_35_18</t>
+  </si>
+  <si>
+    <t>LOG_PEARL_SIMPLE_23_3_2021_____10_49_35</t>
+  </si>
+  <si>
+    <t>LOG_PEARL_SIMPLE_23_3_2021_____10_58_13</t>
+  </si>
+  <si>
+    <t>LOG_PEARL_SIMPLE_23_3_2021_____11_17_21</t>
+  </si>
+  <si>
+    <t>Bump up derivative gain a bit more
+Tried doing some RC control to spin, estimate the delay to be 5 seconds
+slow turn took about 1 minute ended around 11:07 AM
+next turn - try a bit faster, also 5 seconds delay
+tried the fast spin again, 6.8 seconds</t>
+  </si>
+  <si>
+    <t>LOG_PEARL_SIMPLE_23_3_2021_____11_24_57</t>
+  </si>
+  <si>
+    <t>LOG_PEARL_SIMPLE_23_3_2021_____11_37_55</t>
+  </si>
+  <si>
+    <t>LOG_PEARL_SIMPLE_23_3_2021_____15_25_19</t>
+  </si>
+  <si>
+    <t>LOG_PEARL_SIMPLE_23_3_2021_____15_32_32</t>
+  </si>
+  <si>
+    <t>LOG_PEARL_SIMPLE_23_3_2021_____15_36_26</t>
+  </si>
+  <si>
+    <t>LOG_PEARL_SIMPLE_23_3_2021_____15_39_06</t>
+  </si>
+  <si>
+    <t>LOG_PEARL_SIMPLE_23_3_2021_____15_42_12</t>
+  </si>
+  <si>
+    <t>LOG_PEARL_SIMPLE_23_3_2021_____15_47_16</t>
+  </si>
+  <si>
+    <t>LOG_PEARL_SIMPLE_23_3_2021_____15_51_34</t>
+  </si>
+  <si>
+    <t>LOG_PEARL_SIMPLE_23_3_2021_____15_55_01</t>
+  </si>
+  <si>
+    <t>LOG_PEARL_SIMPLE_23_3_2021_____16_00_03</t>
+  </si>
+  <si>
+    <t>LOG_PEARL_WAYPOINT_23_3_2021_____16_09_17</t>
+  </si>
+  <si>
+    <t>LOG_PEARL_WAYPOINT_23_3_2021_____16_14_09</t>
+  </si>
+  <si>
+    <t>LOG_PEARL_WAYPOINT_23_3_2021_____16_16_26</t>
+  </si>
+  <si>
+    <t>LOG_PEARL_SQUARE_23_3_2021_____16_33_09</t>
+  </si>
+  <si>
+    <t>LOG_PEARL_WAYPOINT_23_3_2021_____16_47_05</t>
+  </si>
+  <si>
+    <t>LOG_PEARL_SQUARE_23_3_2021_____16_37_43</t>
   </si>
 </sst>
 </file>
@@ -181,7 +367,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -192,6 +378,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -506,10 +693,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C322D9A-DAA8-F94B-8299-5D36BBA36BB2}">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:K35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" topLeftCell="C21" workbookViewId="0">
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -517,10 +704,16 @@
     <col min="2" max="2" width="16.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="25.83203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="55.83203125" customWidth="1"/>
-    <col min="5" max="5" width="80.1640625" customWidth="1"/>
+    <col min="5" max="5" width="7.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.83203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.83203125" customWidth="1"/>
+    <col min="11" max="11" width="80.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -534,10 +727,28 @@
         <v>1</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" ht="34" x14ac:dyDescent="0.2">
       <c r="A2" s="5">
         <v>44277</v>
       </c>
@@ -550,11 +761,29 @@
       <c r="D2" t="s">
         <v>23</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2">
+        <v>0.1</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>1</v>
+      </c>
+      <c r="I2">
+        <v>1</v>
+      </c>
+      <c r="J2">
+        <v>0.3</v>
+      </c>
+      <c r="K2" s="2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="5">
         <v>44277</v>
       </c>
@@ -567,11 +796,29 @@
       <c r="D3" t="s">
         <v>21</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
+      </c>
+      <c r="I3">
+        <v>1</v>
+      </c>
+      <c r="J3">
+        <v>0.3</v>
+      </c>
+      <c r="K3" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="85" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" ht="85" x14ac:dyDescent="0.2">
       <c r="A4" s="5">
         <v>44277</v>
       </c>
@@ -584,11 +831,29 @@
       <c r="D4" t="s">
         <v>20</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="E4">
+        <v>0.5</v>
+      </c>
+      <c r="F4">
+        <v>0.5</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>1</v>
+      </c>
+      <c r="I4">
+        <v>1</v>
+      </c>
+      <c r="J4">
+        <v>0.3</v>
+      </c>
+      <c r="K4" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="68" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" ht="68" x14ac:dyDescent="0.2">
       <c r="A5" s="5">
         <v>44277</v>
       </c>
@@ -601,11 +866,29 @@
       <c r="D5" t="s">
         <v>19</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="E5">
+        <v>0.2</v>
+      </c>
+      <c r="F5">
+        <v>0.2</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>0.2</v>
+      </c>
+      <c r="I5">
+        <v>0.2</v>
+      </c>
+      <c r="J5">
+        <v>0.3</v>
+      </c>
+      <c r="K5" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="272" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" ht="272" x14ac:dyDescent="0.2">
       <c r="A6" s="5">
         <v>44277</v>
       </c>
@@ -618,11 +901,14 @@
       <c r="D6" t="s">
         <v>18</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="J6">
+        <v>0.3</v>
+      </c>
+      <c r="K6" s="4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="102" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" ht="102" x14ac:dyDescent="0.2">
       <c r="A7" s="5">
         <v>44277</v>
       </c>
@@ -635,11 +921,29 @@
       <c r="D7" t="s">
         <v>17</v>
       </c>
-      <c r="E7" s="4" t="s">
+      <c r="E7">
+        <v>0.25</v>
+      </c>
+      <c r="F7">
+        <v>0.2</v>
+      </c>
+      <c r="G7">
+        <v>0.1</v>
+      </c>
+      <c r="H7">
+        <v>0.2</v>
+      </c>
+      <c r="I7">
+        <v>0.2</v>
+      </c>
+      <c r="J7">
+        <v>0.3</v>
+      </c>
+      <c r="K7" s="4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" ht="34" x14ac:dyDescent="0.2">
       <c r="A8" s="5">
         <v>44277</v>
       </c>
@@ -652,11 +956,29 @@
       <c r="D8" t="s">
         <v>16</v>
       </c>
-      <c r="E8" s="4" t="s">
+      <c r="E8">
+        <v>0.4</v>
+      </c>
+      <c r="F8">
+        <v>0.2</v>
+      </c>
+      <c r="G8">
+        <v>0.1</v>
+      </c>
+      <c r="H8">
+        <v>0.6</v>
+      </c>
+      <c r="I8">
+        <v>0.2</v>
+      </c>
+      <c r="J8">
+        <v>0.3</v>
+      </c>
+      <c r="K8" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="136" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" ht="136" x14ac:dyDescent="0.2">
       <c r="A9" s="5">
         <v>44277</v>
       </c>
@@ -669,11 +991,29 @@
       <c r="D9" t="s">
         <v>15</v>
       </c>
-      <c r="E9" s="4" t="s">
+      <c r="E9">
+        <v>0.3</v>
+      </c>
+      <c r="F9">
+        <v>0.2</v>
+      </c>
+      <c r="G9">
+        <v>0.1</v>
+      </c>
+      <c r="H9">
+        <v>0.5</v>
+      </c>
+      <c r="I9">
+        <v>0.2</v>
+      </c>
+      <c r="J9">
+        <v>0.3</v>
+      </c>
+      <c r="K9" s="4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" ht="51" x14ac:dyDescent="0.2">
       <c r="A10" s="5">
         <v>44277</v>
       </c>
@@ -686,8 +1026,901 @@
       <c r="D10" t="s">
         <v>14</v>
       </c>
-      <c r="E10" s="2" t="s">
+      <c r="E10">
+        <v>0.3</v>
+      </c>
+      <c r="F10">
+        <v>0.2</v>
+      </c>
+      <c r="G10">
+        <v>0.1</v>
+      </c>
+      <c r="H10">
+        <v>0.5</v>
+      </c>
+      <c r="I10">
+        <v>0.2</v>
+      </c>
+      <c r="J10">
+        <v>0.3</v>
+      </c>
+      <c r="K10" s="2" t="s">
         <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A11" s="5">
+        <v>44278</v>
+      </c>
+      <c r="B11" s="3">
+        <v>0.41319444444444442</v>
+      </c>
+      <c r="C11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D11" t="s">
+        <v>57</v>
+      </c>
+      <c r="E11">
+        <v>0.25</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>0.25</v>
+      </c>
+      <c r="H11">
+        <v>0.5</v>
+      </c>
+      <c r="I11">
+        <v>0.75</v>
+      </c>
+      <c r="J11">
+        <v>0.3</v>
+      </c>
+      <c r="K11" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A12" s="5">
+        <v>44278</v>
+      </c>
+      <c r="B12" s="3">
+        <v>0.4236111111111111</v>
+      </c>
+      <c r="C12" t="s">
+        <v>6</v>
+      </c>
+      <c r="D12" t="s">
+        <v>58</v>
+      </c>
+      <c r="E12">
+        <v>0.25</v>
+      </c>
+      <c r="F12">
+        <v>0.25</v>
+      </c>
+      <c r="G12">
+        <v>0.5</v>
+      </c>
+      <c r="H12">
+        <v>0.75</v>
+      </c>
+      <c r="I12">
+        <v>1</v>
+      </c>
+      <c r="J12">
+        <v>0.3</v>
+      </c>
+      <c r="K12" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A13" s="5">
+        <v>44278</v>
+      </c>
+      <c r="B13" s="3">
+        <v>0.4284722222222222</v>
+      </c>
+      <c r="C13" t="s">
+        <v>6</v>
+      </c>
+      <c r="D13" t="s">
+        <v>59</v>
+      </c>
+      <c r="E13">
+        <v>0.25</v>
+      </c>
+      <c r="F13">
+        <v>0.5</v>
+      </c>
+      <c r="G13">
+        <v>0.75</v>
+      </c>
+      <c r="H13">
+        <v>1</v>
+      </c>
+      <c r="I13">
+        <v>0</v>
+      </c>
+      <c r="J13">
+        <v>0.3</v>
+      </c>
+      <c r="K13" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A14" s="5">
+        <v>44278</v>
+      </c>
+      <c r="B14" s="3">
+        <v>0.43333333333333335</v>
+      </c>
+      <c r="C14" t="s">
+        <v>6</v>
+      </c>
+      <c r="D14" t="s">
+        <v>60</v>
+      </c>
+      <c r="E14">
+        <v>0.25</v>
+      </c>
+      <c r="F14">
+        <v>1</v>
+      </c>
+      <c r="G14">
+        <v>0</v>
+      </c>
+      <c r="H14">
+        <v>0.25</v>
+      </c>
+      <c r="I14">
+        <v>0.5</v>
+      </c>
+      <c r="J14">
+        <v>0.3</v>
+      </c>
+      <c r="K14" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A15" s="5">
+        <v>44278</v>
+      </c>
+      <c r="B15" s="3">
+        <v>0.44097222222222227</v>
+      </c>
+      <c r="C15" t="s">
+        <v>6</v>
+      </c>
+      <c r="D15" t="s">
+        <v>61</v>
+      </c>
+      <c r="E15">
+        <v>0.25</v>
+      </c>
+      <c r="F15">
+        <v>1</v>
+      </c>
+      <c r="G15">
+        <v>0</v>
+      </c>
+      <c r="H15">
+        <v>0.25</v>
+      </c>
+      <c r="I15">
+        <v>0.5</v>
+      </c>
+      <c r="J15">
+        <v>0.3</v>
+      </c>
+      <c r="K15" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="34" x14ac:dyDescent="0.2">
+      <c r="A16" s="5">
+        <v>44278</v>
+      </c>
+      <c r="B16" s="3">
+        <v>0.45</v>
+      </c>
+      <c r="C16" t="s">
+        <v>6</v>
+      </c>
+      <c r="D16" t="s">
+        <v>62</v>
+      </c>
+      <c r="E16">
+        <v>0.25</v>
+      </c>
+      <c r="F16">
+        <v>0.2</v>
+      </c>
+      <c r="G16">
+        <v>0.1</v>
+      </c>
+      <c r="H16">
+        <v>0.5</v>
+      </c>
+      <c r="I16">
+        <v>0.2</v>
+      </c>
+      <c r="J16">
+        <v>0.3</v>
+      </c>
+      <c r="K16" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" ht="85" x14ac:dyDescent="0.2">
+      <c r="A17" s="5">
+        <v>44278</v>
+      </c>
+      <c r="B17" s="3">
+        <v>0.45624999999999999</v>
+      </c>
+      <c r="C17" t="s">
+        <v>6</v>
+      </c>
+      <c r="D17" t="s">
+        <v>63</v>
+      </c>
+      <c r="E17">
+        <v>0.25</v>
+      </c>
+      <c r="F17">
+        <v>0.2</v>
+      </c>
+      <c r="G17">
+        <v>0.2</v>
+      </c>
+      <c r="H17">
+        <v>0.5</v>
+      </c>
+      <c r="I17">
+        <v>0.2</v>
+      </c>
+      <c r="J17">
+        <v>0.3</v>
+      </c>
+      <c r="K17" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A18" s="5">
+        <v>44278</v>
+      </c>
+      <c r="B18" s="3">
+        <v>0.47013888888888888</v>
+      </c>
+      <c r="C18" t="s">
+        <v>6</v>
+      </c>
+      <c r="D18" t="s">
+        <v>64</v>
+      </c>
+      <c r="E18">
+        <v>0.25</v>
+      </c>
+      <c r="F18">
+        <v>0.2</v>
+      </c>
+      <c r="G18">
+        <v>0.1</v>
+      </c>
+      <c r="H18">
+        <v>0.5</v>
+      </c>
+      <c r="I18">
+        <v>0.2</v>
+      </c>
+      <c r="J18">
+        <v>0.3</v>
+      </c>
+      <c r="K18" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="A19" s="5">
+        <v>44278</v>
+      </c>
+      <c r="B19" s="3">
+        <v>0.47500000000000003</v>
+      </c>
+      <c r="C19" t="s">
+        <v>6</v>
+      </c>
+      <c r="D19" t="s">
+        <v>66</v>
+      </c>
+      <c r="E19">
+        <v>0.25</v>
+      </c>
+      <c r="F19">
+        <v>0.2</v>
+      </c>
+      <c r="G19">
+        <v>0.1</v>
+      </c>
+      <c r="H19">
+        <v>0.5</v>
+      </c>
+      <c r="I19">
+        <v>0.2</v>
+      </c>
+      <c r="J19">
+        <v>0.3</v>
+      </c>
+      <c r="K19" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A20" s="5">
+        <v>44278</v>
+      </c>
+      <c r="B20" s="3">
+        <v>0.48402777777777778</v>
+      </c>
+      <c r="C20" t="s">
+        <v>6</v>
+      </c>
+      <c r="D20" t="s">
+        <v>67</v>
+      </c>
+      <c r="E20">
+        <v>0.25</v>
+      </c>
+      <c r="F20">
+        <v>0.2</v>
+      </c>
+      <c r="G20">
+        <v>0.1</v>
+      </c>
+      <c r="H20">
+        <v>0.5</v>
+      </c>
+      <c r="I20">
+        <v>0.2</v>
+      </c>
+      <c r="J20">
+        <v>0.3</v>
+      </c>
+      <c r="K20" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" ht="66" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="5">
+        <v>44278</v>
+      </c>
+      <c r="B21" s="3">
+        <v>0.64166666666666672</v>
+      </c>
+      <c r="C21" t="s">
+        <v>6</v>
+      </c>
+      <c r="D21" t="s">
+        <v>68</v>
+      </c>
+      <c r="E21">
+        <v>1</v>
+      </c>
+      <c r="F21">
+        <v>0</v>
+      </c>
+      <c r="G21">
+        <v>0</v>
+      </c>
+      <c r="H21">
+        <v>1</v>
+      </c>
+      <c r="I21">
+        <v>0</v>
+      </c>
+      <c r="J21">
+        <v>0.5</v>
+      </c>
+      <c r="K21" s="4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A22" s="5">
+        <v>44278</v>
+      </c>
+      <c r="B22" s="3">
+        <v>0.64722222222222225</v>
+      </c>
+      <c r="C22" t="s">
+        <v>6</v>
+      </c>
+      <c r="D22" t="s">
+        <v>69</v>
+      </c>
+      <c r="E22">
+        <v>0.75</v>
+      </c>
+      <c r="F22">
+        <v>0</v>
+      </c>
+      <c r="G22">
+        <v>0</v>
+      </c>
+      <c r="H22">
+        <v>1</v>
+      </c>
+      <c r="I22">
+        <v>0</v>
+      </c>
+      <c r="J22">
+        <v>0.5</v>
+      </c>
+      <c r="K22" s="6" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" ht="51" x14ac:dyDescent="0.2">
+      <c r="A23" s="5">
+        <v>44278</v>
+      </c>
+      <c r="B23" s="3">
+        <v>0.65</v>
+      </c>
+      <c r="C23" t="s">
+        <v>6</v>
+      </c>
+      <c r="D23" t="s">
+        <v>70</v>
+      </c>
+      <c r="E23">
+        <v>0.75</v>
+      </c>
+      <c r="F23">
+        <v>0</v>
+      </c>
+      <c r="G23">
+        <v>0.25</v>
+      </c>
+      <c r="H23">
+        <v>1</v>
+      </c>
+      <c r="I23">
+        <v>0</v>
+      </c>
+      <c r="J23">
+        <v>0.5</v>
+      </c>
+      <c r="K23" s="4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A24" s="5">
+        <v>44278</v>
+      </c>
+      <c r="B24" s="3">
+        <v>0.65138888888888891</v>
+      </c>
+      <c r="C24" t="s">
+        <v>6</v>
+      </c>
+      <c r="D24" t="s">
+        <v>71</v>
+      </c>
+      <c r="E24">
+        <v>0.75</v>
+      </c>
+      <c r="F24">
+        <v>0</v>
+      </c>
+      <c r="G24">
+        <v>0.5</v>
+      </c>
+      <c r="H24">
+        <v>1</v>
+      </c>
+      <c r="I24">
+        <v>0</v>
+      </c>
+      <c r="J24">
+        <v>0.5</v>
+      </c>
+      <c r="K24" s="6" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" ht="34" x14ac:dyDescent="0.2">
+      <c r="A25" s="5">
+        <v>44278</v>
+      </c>
+      <c r="B25" s="3">
+        <v>0.65347222222222223</v>
+      </c>
+      <c r="C25" t="s">
+        <v>6</v>
+      </c>
+      <c r="D25" t="s">
+        <v>72</v>
+      </c>
+      <c r="E25">
+        <v>0.75</v>
+      </c>
+      <c r="F25">
+        <v>0</v>
+      </c>
+      <c r="G25">
+        <v>0.75</v>
+      </c>
+      <c r="H25">
+        <v>1</v>
+      </c>
+      <c r="I25">
+        <v>0</v>
+      </c>
+      <c r="J25">
+        <v>0.5</v>
+      </c>
+      <c r="K25" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A26" s="5">
+        <v>44278</v>
+      </c>
+      <c r="B26" s="3">
+        <v>0.65763888888888888</v>
+      </c>
+      <c r="C26" t="s">
+        <v>6</v>
+      </c>
+      <c r="D26" t="s">
+        <v>73</v>
+      </c>
+      <c r="E26">
+        <v>0.75</v>
+      </c>
+      <c r="F26">
+        <v>0</v>
+      </c>
+      <c r="G26">
+        <v>1</v>
+      </c>
+      <c r="H26">
+        <v>1</v>
+      </c>
+      <c r="I26">
+        <v>0</v>
+      </c>
+      <c r="J26">
+        <v>0.5</v>
+      </c>
+      <c r="K26" s="6" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="A27" s="5">
+        <v>44278</v>
+      </c>
+      <c r="B27" s="3">
+        <v>0.66041666666666665</v>
+      </c>
+      <c r="C27" t="s">
+        <v>6</v>
+      </c>
+      <c r="D27" t="s">
+        <v>74</v>
+      </c>
+      <c r="E27">
+        <v>0.75</v>
+      </c>
+      <c r="F27">
+        <v>0</v>
+      </c>
+      <c r="G27">
+        <v>1.5</v>
+      </c>
+      <c r="H27">
+        <v>1</v>
+      </c>
+      <c r="I27">
+        <v>0</v>
+      </c>
+      <c r="J27">
+        <v>0.5</v>
+      </c>
+      <c r="K27" s="4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" ht="34" x14ac:dyDescent="0.2">
+      <c r="A28" s="5">
+        <v>44278</v>
+      </c>
+      <c r="B28" s="3">
+        <v>0.66249999999999998</v>
+      </c>
+      <c r="C28" t="s">
+        <v>6</v>
+      </c>
+      <c r="D28" t="s">
+        <v>75</v>
+      </c>
+      <c r="E28">
+        <v>0.75</v>
+      </c>
+      <c r="F28">
+        <v>0.5</v>
+      </c>
+      <c r="G28">
+        <v>1.5</v>
+      </c>
+      <c r="H28">
+        <v>1</v>
+      </c>
+      <c r="I28">
+        <v>0</v>
+      </c>
+      <c r="J28">
+        <v>0.5</v>
+      </c>
+      <c r="K28" s="4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" ht="34" x14ac:dyDescent="0.2">
+      <c r="A29" s="5">
+        <v>44278</v>
+      </c>
+      <c r="B29" s="3">
+        <v>0.66597222222222219</v>
+      </c>
+      <c r="C29" t="s">
+        <v>6</v>
+      </c>
+      <c r="D29" t="s">
+        <v>76</v>
+      </c>
+      <c r="E29">
+        <v>0.75</v>
+      </c>
+      <c r="F29">
+        <v>0.75</v>
+      </c>
+      <c r="G29">
+        <v>1.5</v>
+      </c>
+      <c r="H29">
+        <v>1</v>
+      </c>
+      <c r="I29">
+        <v>0</v>
+      </c>
+      <c r="J29">
+        <v>0.5</v>
+      </c>
+      <c r="K29" s="4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" ht="34" x14ac:dyDescent="0.2">
+      <c r="A30" s="5">
+        <v>44278</v>
+      </c>
+      <c r="B30" s="3">
+        <v>0.67152777777777783</v>
+      </c>
+      <c r="C30" t="s">
+        <v>26</v>
+      </c>
+      <c r="D30" t="s">
+        <v>77</v>
+      </c>
+      <c r="E30">
+        <v>0.75</v>
+      </c>
+      <c r="F30">
+        <v>0.75</v>
+      </c>
+      <c r="G30">
+        <v>1.5</v>
+      </c>
+      <c r="H30">
+        <v>1</v>
+      </c>
+      <c r="I30">
+        <v>0</v>
+      </c>
+      <c r="J30">
+        <v>0.5</v>
+      </c>
+      <c r="K30" s="4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="A31" s="5">
+        <v>44278</v>
+      </c>
+      <c r="B31" s="3">
+        <v>0.67569444444444438</v>
+      </c>
+      <c r="C31" t="s">
+        <v>26</v>
+      </c>
+      <c r="D31" t="s">
+        <v>78</v>
+      </c>
+      <c r="E31">
+        <v>0.75</v>
+      </c>
+      <c r="F31">
+        <v>0.75</v>
+      </c>
+      <c r="G31">
+        <v>1.5</v>
+      </c>
+      <c r="H31">
+        <v>1</v>
+      </c>
+      <c r="I31">
+        <v>0</v>
+      </c>
+      <c r="J31">
+        <v>0.5</v>
+      </c>
+      <c r="K31" s="4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" ht="51" x14ac:dyDescent="0.2">
+      <c r="A32" s="5">
+        <v>44278</v>
+      </c>
+      <c r="B32" s="3">
+        <v>0.6777777777777777</v>
+      </c>
+      <c r="C32" t="s">
+        <v>26</v>
+      </c>
+      <c r="D32" t="s">
+        <v>79</v>
+      </c>
+      <c r="E32">
+        <v>0.75</v>
+      </c>
+      <c r="F32">
+        <v>0.75</v>
+      </c>
+      <c r="G32">
+        <v>1.5</v>
+      </c>
+      <c r="H32">
+        <v>1</v>
+      </c>
+      <c r="I32">
+        <v>0</v>
+      </c>
+      <c r="J32">
+        <v>0.5</v>
+      </c>
+      <c r="K32" s="4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="A33" s="5">
+        <v>44278</v>
+      </c>
+      <c r="B33" s="3">
+        <v>0.68958333333333333</v>
+      </c>
+      <c r="C33" t="s">
+        <v>9</v>
+      </c>
+      <c r="D33" t="s">
+        <v>80</v>
+      </c>
+      <c r="E33">
+        <v>1</v>
+      </c>
+      <c r="F33">
+        <v>4</v>
+      </c>
+      <c r="G33">
+        <v>2</v>
+      </c>
+      <c r="H33">
+        <v>1</v>
+      </c>
+      <c r="I33">
+        <v>0</v>
+      </c>
+      <c r="J33">
+        <v>0.5</v>
+      </c>
+      <c r="K33" s="4" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="A34" s="5">
+        <v>44278</v>
+      </c>
+      <c r="B34" s="3">
+        <v>0.69236111111111109</v>
+      </c>
+      <c r="C34" t="s">
+        <v>9</v>
+      </c>
+      <c r="D34" t="s">
+        <v>82</v>
+      </c>
+      <c r="E34">
+        <v>0.5</v>
+      </c>
+      <c r="F34">
+        <v>4</v>
+      </c>
+      <c r="G34">
+        <v>2</v>
+      </c>
+      <c r="H34">
+        <v>1</v>
+      </c>
+      <c r="I34">
+        <v>0</v>
+      </c>
+      <c r="J34">
+        <v>0.5</v>
+      </c>
+      <c r="K34" s="4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" ht="34" x14ac:dyDescent="0.2">
+      <c r="A35" s="5">
+        <v>44278</v>
+      </c>
+      <c r="B35" s="3">
+        <v>0.69930555555555562</v>
+      </c>
+      <c r="C35" t="s">
+        <v>26</v>
+      </c>
+      <c r="D35" t="s">
+        <v>81</v>
+      </c>
+      <c r="E35">
+        <v>0.5</v>
+      </c>
+      <c r="F35">
+        <v>4</v>
+      </c>
+      <c r="G35">
+        <v>2</v>
+      </c>
+      <c r="H35">
+        <v>1</v>
+      </c>
+      <c r="I35">
+        <v>0</v>
+      </c>
+      <c r="J35">
+        <v>0.5</v>
+      </c>
+      <c r="K35" s="4" t="s">
+        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update notes from testing 2021-03-24
</commit_message>
<xml_diff>
--- a/pearl_logs/PEARL_MOOS_testing_notes.xlsx
+++ b/pearl_logs/PEARL_MOOS_testing_notes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maha/moos-ivp-pearl/pearl_logs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC35CBCB-A42D-9B42-A7BC-A51A05565F0E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC8D46EA-831E-B246-A957-883436FFFEFB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="12800" yWindow="460" windowWidth="12800" windowHeight="15540" xr2:uid="{CE7898E4-CB96-184C-9C00-2CBDA86B470B}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="102">
   <si>
     <t>Date</t>
   </si>
@@ -325,12 +325,73 @@
   <si>
     <t>LOG_PEARL_SQUARE_23_3_2021_____16_37_43</t>
   </si>
+  <si>
+    <t>Waypoint - Perimeter</t>
+  </si>
+  <si>
+    <t>- better than yesterday, still some overshoot initially turning 90 degrees</t>
+  </si>
+  <si>
+    <t>- did better, made more of circle than square</t>
+  </si>
+  <si>
+    <t>- redid above with leads back in, looked ok but lost GUI so can't see tracks realtime</t>
+  </si>
+  <si>
+    <t>- re run to try again with GUI not crashing, lost connection at last leg</t>
+  </si>
+  <si>
+    <t>- re run again</t>
+  </si>
+  <si>
+    <t>- trying star with new gains and lead ins - lost connection</t>
+  </si>
+  <si>
+    <t>- trying star with new gains and lead ins 
+- track points not showing up? But checked in code
+- track points showe dup
+- she did really well!
+- going to west star point, it was slow because of current? Coming back was much faster</t>
+  </si>
+  <si>
+    <t>- timed out at 2:47 PM?</t>
+  </si>
+  <si>
+    <t>- did well!</t>
+  </si>
+  <si>
+    <t>LOG_PEARL_WAYPOINT_24_3_2021_____14_49_26</t>
+  </si>
+  <si>
+    <t>LOG_PEARL_WAYPOINT_24_3_2021_____14_37_29</t>
+  </si>
+  <si>
+    <t>LOG_PEARL_WAYPOINT_24_3_2021_____14_23_34</t>
+  </si>
+  <si>
+    <t>LOG_PEARL_WAYPOINT_24_3_2021_____14_18_41</t>
+  </si>
+  <si>
+    <t>LOG_PEARL_SQUARE_24_3_2021_____13_46_33</t>
+  </si>
+  <si>
+    <t>LOG_PEARL_SQUARE_24_3_2021_____13_38_41</t>
+  </si>
+  <si>
+    <t>LOG_PEARL_SQUARE_24_3_2021_____13_31_35</t>
+  </si>
+  <si>
+    <t>LOG_PEARL_SQUARE_24_3_2021_____13_24_07</t>
+  </si>
+  <si>
+    <t>LOG_PEARL_SQUARE_24_3_2021_____13_14_36</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -342,6 +403,13 @@
       <b/>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -367,7 +435,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -379,6 +447,12 @@
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="18" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -693,10 +767,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C322D9A-DAA8-F94B-8299-5D36BBA36BB2}">
-  <dimension ref="A1:K35"/>
+  <dimension ref="A1:K44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C21" workbookViewId="0">
-      <selection activeCell="D34" sqref="D34"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="D42" sqref="D42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1923,6 +1997,321 @@
         <v>56</v>
       </c>
     </row>
+    <row r="36" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="A36" s="5">
+        <v>44279</v>
+      </c>
+      <c r="B36" s="3">
+        <v>0.55138888888888882</v>
+      </c>
+      <c r="C36" t="s">
+        <v>9</v>
+      </c>
+      <c r="D36" t="s">
+        <v>101</v>
+      </c>
+      <c r="E36">
+        <v>0.6</v>
+      </c>
+      <c r="F36">
+        <v>0.03</v>
+      </c>
+      <c r="G36">
+        <v>2.7</v>
+      </c>
+      <c r="H36">
+        <v>1</v>
+      </c>
+      <c r="I36">
+        <v>0</v>
+      </c>
+      <c r="J36">
+        <v>0.5</v>
+      </c>
+      <c r="K36" s="4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A37" s="5">
+        <v>44279</v>
+      </c>
+      <c r="B37" s="3">
+        <v>0.55763888888888891</v>
+      </c>
+      <c r="C37" t="s">
+        <v>9</v>
+      </c>
+      <c r="D37" t="s">
+        <v>100</v>
+      </c>
+      <c r="E37">
+        <v>0.4</v>
+      </c>
+      <c r="F37">
+        <v>0.04</v>
+      </c>
+      <c r="G37">
+        <v>4</v>
+      </c>
+      <c r="H37">
+        <v>1</v>
+      </c>
+      <c r="I37">
+        <v>0</v>
+      </c>
+      <c r="J37">
+        <v>0.5</v>
+      </c>
+      <c r="K37" s="6" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="A38" s="5">
+        <v>44279</v>
+      </c>
+      <c r="B38" s="3">
+        <v>0.56388888888888888</v>
+      </c>
+      <c r="C38" t="s">
+        <v>9</v>
+      </c>
+      <c r="D38" t="s">
+        <v>99</v>
+      </c>
+      <c r="E38">
+        <v>0.4</v>
+      </c>
+      <c r="F38">
+        <v>0.04</v>
+      </c>
+      <c r="G38">
+        <v>4</v>
+      </c>
+      <c r="H38">
+        <v>1</v>
+      </c>
+      <c r="I38">
+        <v>0</v>
+      </c>
+      <c r="J38">
+        <v>0.5</v>
+      </c>
+      <c r="K38" s="4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A39" s="5">
+        <v>44279</v>
+      </c>
+      <c r="B39" s="3">
+        <v>0.56805555555555554</v>
+      </c>
+      <c r="C39" t="s">
+        <v>9</v>
+      </c>
+      <c r="D39" t="s">
+        <v>98</v>
+      </c>
+      <c r="E39">
+        <v>0.4</v>
+      </c>
+      <c r="F39">
+        <v>0.04</v>
+      </c>
+      <c r="G39">
+        <v>4</v>
+      </c>
+      <c r="H39">
+        <v>1</v>
+      </c>
+      <c r="I39">
+        <v>0</v>
+      </c>
+      <c r="J39">
+        <v>0.5</v>
+      </c>
+      <c r="K39" s="6" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="A40" s="5">
+        <v>44279</v>
+      </c>
+      <c r="B40" s="3">
+        <v>0.57361111111111118</v>
+      </c>
+      <c r="C40" t="s">
+        <v>9</v>
+      </c>
+      <c r="D40" t="s">
+        <v>97</v>
+      </c>
+      <c r="E40">
+        <v>0.4</v>
+      </c>
+      <c r="F40">
+        <v>0.04</v>
+      </c>
+      <c r="G40">
+        <v>4</v>
+      </c>
+      <c r="H40">
+        <v>1</v>
+      </c>
+      <c r="I40">
+        <v>0</v>
+      </c>
+      <c r="J40">
+        <v>0.5</v>
+      </c>
+      <c r="K40" s="4" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="A41" s="5">
+        <v>44279</v>
+      </c>
+      <c r="B41" s="3">
+        <v>0.59583333333333333</v>
+      </c>
+      <c r="C41" t="s">
+        <v>26</v>
+      </c>
+      <c r="D41" t="s">
+        <v>96</v>
+      </c>
+      <c r="E41">
+        <v>0.4</v>
+      </c>
+      <c r="F41">
+        <v>0.04</v>
+      </c>
+      <c r="G41">
+        <v>4</v>
+      </c>
+      <c r="H41">
+        <v>1</v>
+      </c>
+      <c r="I41">
+        <v>0</v>
+      </c>
+      <c r="J41">
+        <v>0.5</v>
+      </c>
+      <c r="K41" s="4" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" ht="85" x14ac:dyDescent="0.2">
+      <c r="A42" s="7">
+        <v>44279</v>
+      </c>
+      <c r="B42" s="8">
+        <v>0.59930555555555554</v>
+      </c>
+      <c r="C42" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="D42" t="s">
+        <v>95</v>
+      </c>
+      <c r="E42" s="9">
+        <v>0.4</v>
+      </c>
+      <c r="F42" s="9">
+        <v>0.04</v>
+      </c>
+      <c r="G42" s="9">
+        <v>4</v>
+      </c>
+      <c r="H42" s="9">
+        <v>1</v>
+      </c>
+      <c r="I42" s="9">
+        <v>0</v>
+      </c>
+      <c r="J42" s="9">
+        <v>0.5</v>
+      </c>
+      <c r="K42" s="10" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="A43" s="7">
+        <v>44279</v>
+      </c>
+      <c r="B43" s="8">
+        <v>0.10902777777777778</v>
+      </c>
+      <c r="C43" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="D43" t="s">
+        <v>94</v>
+      </c>
+      <c r="E43" s="9">
+        <v>0.4</v>
+      </c>
+      <c r="F43" s="9">
+        <v>0.04</v>
+      </c>
+      <c r="G43" s="9">
+        <v>4</v>
+      </c>
+      <c r="H43" s="9">
+        <v>1</v>
+      </c>
+      <c r="I43" s="9">
+        <v>0</v>
+      </c>
+      <c r="J43" s="9">
+        <v>0.5</v>
+      </c>
+      <c r="K43" s="4" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="A44" s="7">
+        <v>44279</v>
+      </c>
+      <c r="B44" s="3">
+        <v>0.61736111111111114</v>
+      </c>
+      <c r="C44" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="D44" t="s">
+        <v>93</v>
+      </c>
+      <c r="E44" s="9">
+        <v>0.4</v>
+      </c>
+      <c r="F44" s="9">
+        <v>0.04</v>
+      </c>
+      <c r="G44" s="9">
+        <v>4</v>
+      </c>
+      <c r="H44" s="9">
+        <v>1</v>
+      </c>
+      <c r="I44" s="9">
+        <v>0</v>
+      </c>
+      <c r="J44" s="9">
+        <v>0.5</v>
+      </c>
+      <c r="K44" s="4" t="s">
+        <v>92</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update PEARL testing logs for 2021-03-25
</commit_message>
<xml_diff>
--- a/pearl_logs/PEARL_MOOS_testing_notes.xlsx
+++ b/pearl_logs/PEARL_MOOS_testing_notes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maha/moos-ivp-pearl/pearl_logs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC8D46EA-831E-B246-A957-883436FFFEFB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3F7FC85-784B-784F-80A4-66072D7767DB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12800" yWindow="460" windowWidth="12800" windowHeight="15540" xr2:uid="{CE7898E4-CB96-184C-9C00-2CBDA86B470B}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" xr2:uid="{CE7898E4-CB96-184C-9C00-2CBDA86B470B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="111">
   <si>
     <t>Date</t>
   </si>
@@ -385,6 +385,35 @@
   </si>
   <si>
     <t>LOG_PEARL_SQUARE_24_3_2021_____13_14_36</t>
+  </si>
+  <si>
+    <t>Waypoint - Figure 8</t>
+  </si>
+  <si>
+    <t>- PEARL bumped into edge of canoe on the way to first way point (grazed). Will it show up in log?</t>
+  </si>
+  <si>
+    <t>- did well, some overshoot/undershoot on turns but overall OK</t>
+  </si>
+  <si>
+    <t>Oops no good, kept starting wrong mission</t>
+  </si>
+  <si>
+    <t>- virtually no wind or waves now, water quite still, seems to be following path exceptionally well!
+- my anchor broke loose??</t>
+  </si>
+  <si>
+    <t>- excellent!</t>
+  </si>
+  <si>
+    <t>- redo for statistics</t>
+  </si>
+  <si>
+    <t>- redo for statistics
+- got caught on something or went stale? Hmm</t>
+  </si>
+  <si>
+    <t>- to send her home cuz lazy lol</t>
   </si>
 </sst>
 </file>
@@ -767,10 +796,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C322D9A-DAA8-F94B-8299-5D36BBA36BB2}">
-  <dimension ref="A1:K44"/>
+  <dimension ref="A1:K52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="D42" sqref="D42"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="B53" sqref="B53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2312,6 +2341,262 @@
         <v>92</v>
       </c>
     </row>
+    <row r="45" spans="1:11" ht="34" x14ac:dyDescent="0.2">
+      <c r="A45" s="7">
+        <v>44280</v>
+      </c>
+      <c r="B45" s="3">
+        <v>0.56874999999999998</v>
+      </c>
+      <c r="C45" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="E45" s="9">
+        <v>0.4</v>
+      </c>
+      <c r="F45" s="9">
+        <v>0.04</v>
+      </c>
+      <c r="G45" s="9">
+        <v>4</v>
+      </c>
+      <c r="H45" s="9">
+        <v>1</v>
+      </c>
+      <c r="I45" s="9">
+        <v>0</v>
+      </c>
+      <c r="J45" s="9">
+        <v>0.5</v>
+      </c>
+      <c r="K45" s="4" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="A46" s="7">
+        <v>44280</v>
+      </c>
+      <c r="B46" s="3">
+        <v>0.57777777777777783</v>
+      </c>
+      <c r="C46" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="E46" s="9">
+        <v>0.4</v>
+      </c>
+      <c r="F46" s="9">
+        <v>0.04</v>
+      </c>
+      <c r="G46" s="9">
+        <v>4</v>
+      </c>
+      <c r="H46" s="9">
+        <v>1</v>
+      </c>
+      <c r="I46" s="9">
+        <v>0</v>
+      </c>
+      <c r="J46" s="9">
+        <v>0.5</v>
+      </c>
+      <c r="K46" s="4" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="A47" s="7">
+        <v>44280</v>
+      </c>
+      <c r="B47" s="3">
+        <v>0.58680555555555558</v>
+      </c>
+      <c r="C47" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="E47" s="9">
+        <v>0.4</v>
+      </c>
+      <c r="F47" s="9">
+        <v>0.04</v>
+      </c>
+      <c r="G47" s="9">
+        <v>4</v>
+      </c>
+      <c r="H47" s="9">
+        <v>1</v>
+      </c>
+      <c r="I47" s="9">
+        <v>0</v>
+      </c>
+      <c r="J47" s="9">
+        <v>0.5</v>
+      </c>
+      <c r="K47" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" ht="51" x14ac:dyDescent="0.2">
+      <c r="A48" s="7">
+        <v>44280</v>
+      </c>
+      <c r="B48" s="3">
+        <v>0.58819444444444446</v>
+      </c>
+      <c r="C48" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="E48" s="9">
+        <v>0.4</v>
+      </c>
+      <c r="F48" s="9">
+        <v>0.04</v>
+      </c>
+      <c r="G48" s="9">
+        <v>4</v>
+      </c>
+      <c r="H48" s="9">
+        <v>1</v>
+      </c>
+      <c r="I48" s="9">
+        <v>0</v>
+      </c>
+      <c r="J48" s="9">
+        <v>0.5</v>
+      </c>
+      <c r="K48" s="4" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="A49" s="7">
+        <v>44280</v>
+      </c>
+      <c r="B49" s="3">
+        <v>0.59583333333333333</v>
+      </c>
+      <c r="C49" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="E49" s="9">
+        <v>0.4</v>
+      </c>
+      <c r="F49" s="9">
+        <v>0.04</v>
+      </c>
+      <c r="G49" s="9">
+        <v>4</v>
+      </c>
+      <c r="H49" s="9">
+        <v>1</v>
+      </c>
+      <c r="I49" s="9">
+        <v>0</v>
+      </c>
+      <c r="J49" s="9">
+        <v>0.5</v>
+      </c>
+      <c r="K49" s="4" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" ht="34" x14ac:dyDescent="0.2">
+      <c r="A50" s="7">
+        <v>44280</v>
+      </c>
+      <c r="B50" s="3">
+        <v>0.60555555555555551</v>
+      </c>
+      <c r="C50" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="E50" s="9">
+        <v>0.4</v>
+      </c>
+      <c r="F50" s="9">
+        <v>0.04</v>
+      </c>
+      <c r="G50" s="9">
+        <v>4</v>
+      </c>
+      <c r="H50" s="9">
+        <v>1</v>
+      </c>
+      <c r="I50" s="9">
+        <v>0</v>
+      </c>
+      <c r="J50" s="9">
+        <v>0.5</v>
+      </c>
+      <c r="K50" s="4" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="A51" s="7">
+        <v>44280</v>
+      </c>
+      <c r="B51" s="3">
+        <v>0.6069444444444444</v>
+      </c>
+      <c r="C51" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="E51" s="9">
+        <v>0.4</v>
+      </c>
+      <c r="F51" s="9">
+        <v>0.04</v>
+      </c>
+      <c r="G51" s="9">
+        <v>4</v>
+      </c>
+      <c r="H51" s="9">
+        <v>1</v>
+      </c>
+      <c r="I51" s="9">
+        <v>0</v>
+      </c>
+      <c r="J51" s="9">
+        <v>0.5</v>
+      </c>
+      <c r="K51" s="4" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="A52" s="5">
+        <v>44280</v>
+      </c>
+      <c r="B52" s="3">
+        <v>0.61736111111111114</v>
+      </c>
+      <c r="C52" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="E52" s="9">
+        <v>0.4</v>
+      </c>
+      <c r="F52" s="9">
+        <v>0.04</v>
+      </c>
+      <c r="G52" s="9">
+        <v>4</v>
+      </c>
+      <c r="H52" s="9">
+        <v>1</v>
+      </c>
+      <c r="I52" s="9">
+        <v>0</v>
+      </c>
+      <c r="J52" s="9">
+        <v>0.5</v>
+      </c>
+      <c r="K52" s="4" t="s">
+        <v>110</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Upload mission screenshots and notes from 2021-03-25 testing
</commit_message>
<xml_diff>
--- a/pearl_logs/PEARL_MOOS_testing_notes.xlsx
+++ b/pearl_logs/PEARL_MOOS_testing_notes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maha/moos-ivp-pearl/pearl_logs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3F7FC85-784B-784F-80A4-66072D7767DB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{262C397A-7A23-F147-BD71-684931DA3DB5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" xr2:uid="{CE7898E4-CB96-184C-9C00-2CBDA86B470B}"/>
+    <workbookView xWindow="12820" yWindow="460" windowWidth="12780" windowHeight="15540" xr2:uid="{CE7898E4-CB96-184C-9C00-2CBDA86B470B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="119">
   <si>
     <t>Date</t>
   </si>
@@ -414,6 +414,30 @@
   </si>
   <si>
     <t>- to send her home cuz lazy lol</t>
+  </si>
+  <si>
+    <t>LOG_PEARL_WAYPOINT_25_3_2021_____13_39_28</t>
+  </si>
+  <si>
+    <t>LOG_PEARL_WAYPOINT_25_3_2021_____13_52_14</t>
+  </si>
+  <si>
+    <t>LOG_PEARL_WAYPOINT_25_3_2021_____14_05_23</t>
+  </si>
+  <si>
+    <t>LOG_PEARL_WAYPOINT_25_3_2021_____14_07_52</t>
+  </si>
+  <si>
+    <t>LOG_PEARL_WAYPOINT_25_3_2021_____14_19_12</t>
+  </si>
+  <si>
+    <t>LOG_PEARL_WAYPOINT_25_3_2021_____14_32_25</t>
+  </si>
+  <si>
+    <t>LOG_PEARL_WAYPOINT_25_3_2021_____14_35_08</t>
+  </si>
+  <si>
+    <t>LOG_PEARL_SIMPLE_25_3_2021_____14_50_18</t>
   </si>
 </sst>
 </file>
@@ -798,8 +822,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C322D9A-DAA8-F94B-8299-5D36BBA36BB2}">
   <dimension ref="A1:K52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="B53" sqref="B53"/>
+    <sheetView tabSelected="1" topLeftCell="B37" workbookViewId="0">
+      <selection activeCell="D52" sqref="D52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2351,6 +2375,9 @@
       <c r="C45" s="9" t="s">
         <v>102</v>
       </c>
+      <c r="D45" t="s">
+        <v>111</v>
+      </c>
       <c r="E45" s="9">
         <v>0.4</v>
       </c>
@@ -2383,6 +2410,9 @@
       <c r="C46" s="9" t="s">
         <v>102</v>
       </c>
+      <c r="D46" t="s">
+        <v>112</v>
+      </c>
       <c r="E46" s="9">
         <v>0.4</v>
       </c>
@@ -2415,6 +2445,9 @@
       <c r="C47" s="9" t="s">
         <v>102</v>
       </c>
+      <c r="D47" t="s">
+        <v>113</v>
+      </c>
       <c r="E47" s="9">
         <v>0.4</v>
       </c>
@@ -2447,6 +2480,9 @@
       <c r="C48" s="9" t="s">
         <v>102</v>
       </c>
+      <c r="D48" t="s">
+        <v>114</v>
+      </c>
       <c r="E48" s="9">
         <v>0.4</v>
       </c>
@@ -2479,6 +2515,9 @@
       <c r="C49" s="9" t="s">
         <v>26</v>
       </c>
+      <c r="D49" t="s">
+        <v>115</v>
+      </c>
       <c r="E49" s="9">
         <v>0.4</v>
       </c>
@@ -2511,6 +2550,9 @@
       <c r="C50" s="9" t="s">
         <v>26</v>
       </c>
+      <c r="D50" t="s">
+        <v>116</v>
+      </c>
       <c r="E50" s="9">
         <v>0.4</v>
       </c>
@@ -2543,6 +2585,9 @@
       <c r="C51" s="9" t="s">
         <v>26</v>
       </c>
+      <c r="D51" t="s">
+        <v>117</v>
+      </c>
       <c r="E51" s="9">
         <v>0.4</v>
       </c>
@@ -2574,6 +2619,9 @@
       </c>
       <c r="C52" s="9" t="s">
         <v>6</v>
+      </c>
+      <c r="D52" t="s">
+        <v>118</v>
       </c>
       <c r="E52" s="9">
         <v>0.4</v>

</xml_diff>

<commit_message>
Upload screenshots and testing notes from 2021-03-27 testing
</commit_message>
<xml_diff>
--- a/pearl_logs/PEARL_MOOS_testing_notes.xlsx
+++ b/pearl_logs/PEARL_MOOS_testing_notes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maha/moos-ivp-pearl/pearl_logs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{262C397A-7A23-F147-BD71-684931DA3DB5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64940F8B-CD9E-FA44-9234-6F9D0412B994}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12820" yWindow="460" windowWidth="12780" windowHeight="15540" xr2:uid="{CE7898E4-CB96-184C-9C00-2CBDA86B470B}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" xr2:uid="{CE7898E4-CB96-184C-9C00-2CBDA86B470B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="157">
   <si>
     <t>Date</t>
   </si>
@@ -438,6 +438,135 @@
   </si>
   <si>
     <t>LOG_PEARL_SIMPLE_25_3_2021_____14_50_18</t>
+  </si>
+  <si>
+    <t>Pattern good for statistics?</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>- ignore, I was in her way, had to stop and restart mission</t>
+  </si>
+  <si>
+    <t>- GUI crashed but presumably she's still going? I see her still making patterns
+- check later if this worked out ok. She seemed to keep going after last waypoint?</t>
+  </si>
+  <si>
+    <t>- BIG gust of wind threw her off at the start near the initial waypoint. Let's see how that looks!
+- GUI froze again? But still updating…
+- and then stopped around 11:27 AM</t>
+  </si>
+  <si>
+    <t>- bumped into her on N to S leg - oops. Will that show up? Redo?</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>Square - stationkeep at first N corner</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- try stationkeeping for 10 minutes to check how GPS heading vs IMU heading handles it
+- did GUI stop updating?
+- time increasing but nothing else?
+- code from terminal still outputting
+- stopped at 12:05 (5 minute test) </t>
+  </si>
+  <si>
+    <t>- retry stationkeeping for 10 minutes to check GPS vs IMU heading
+- compareds to iPhone compass, both seem wrong?
+- at 12:12pm, took over RC control and moved out of watch circle
+- lost connection?</t>
+  </si>
+  <si>
+    <t>- start with stationkeep, then moved out of watch circle via manual RC, then turned back on stationkeep to see if could return
+- lost connection from my WiFi</t>
+  </si>
+  <si>
+    <t>- stationkeep for 60 seconds
+ - then moved out of watch circle via manual RC, then turned back on stationkeep to see if could return
+- wind started blowing her out of watch circle towards end
+- she turned on to correct herself and returned to watch circle</t>
+  </si>
+  <si>
+    <t>- lost connection because WiFi turned off -oops</t>
+  </si>
+  <si>
+    <t>- something wrong, was not going to right point? Returning back to center
+- could have been wind?</t>
+  </si>
+  <si>
+    <t>- windier than this morning. Pretty steady breeze coming from the SE</t>
+  </si>
+  <si>
+    <t>- fair bit of wind seen in her 3rd leg - when she was going approximately upwind</t>
+  </si>
+  <si>
+    <t>- quite windy as previous missions</t>
+  </si>
+  <si>
+    <t>- sent back towards home autonomously</t>
+  </si>
+  <si>
+    <t>LOG_PEARL_SIMPLE_27_3_2021_____15_06_52</t>
+  </si>
+  <si>
+    <t>LOG_PEARL_WAYPOINT_27_3_2021_____14_53_27</t>
+  </si>
+  <si>
+    <t>LOG_PEARL_WAYPOINT_27_3_2021_____14_41_16</t>
+  </si>
+  <si>
+    <t>LOG_PEARL_WAYPOINT_27_3_2021_____14_29_01</t>
+  </si>
+  <si>
+    <t>LOG_PEARL_WAYPOINT_27_3_2021_____14_25_21</t>
+  </si>
+  <si>
+    <t>LOG_PEARL_WAYPOINT_27_3_2021_____14_21_39</t>
+  </si>
+  <si>
+    <t>LOG_PEARL_SQUARE_27_3_2021_____12_17_03</t>
+  </si>
+  <si>
+    <t>LOG_PEARL_SQUARE_27_3_2021_____12_14_23</t>
+  </si>
+  <si>
+    <t>LOG_PEARL_SQUARE_27_3_2021_____12_06_09</t>
+  </si>
+  <si>
+    <t>LOG_PEARL_SQUARE_27_3_2021_____12_00_13</t>
+  </si>
+  <si>
+    <t>LOG_PEARL_SQUARE_27_3_2021_____11_54_10</t>
+  </si>
+  <si>
+    <t>LOG_PEARL_SQUARE_27_3_2021_____11_47_47</t>
+  </si>
+  <si>
+    <t>LOG_PEARL_SQUARE_27_3_2021_____11_41_41</t>
+  </si>
+  <si>
+    <t>LOG_PEARL_SQUARE_27_3_2021_____11_35_47</t>
+  </si>
+  <si>
+    <t>LOG_PEARL_SQUARE_27_3_2021_____11_28_22</t>
+  </si>
+  <si>
+    <t>LOG_PEARL_SQUARE_27_3_2021_____11_21_57</t>
+  </si>
+  <si>
+    <t>LOG_PEARL_SQUARE_27_3_2021_____11_15_43</t>
+  </si>
+  <si>
+    <t>LOG_PEARL_SQUARE_27_3_2021_____11_09_19</t>
+  </si>
+  <si>
+    <t>LOG_PEARL_SQUARE_27_3_2021_____11_07_00</t>
   </si>
 </sst>
 </file>
@@ -468,12 +597,42 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCCC0DA"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -488,7 +647,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -503,15 +662,62 @@
     <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="18" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="18" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="18" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="18" fontId="2" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="18" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="18" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="18" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="18" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFCCC0DA"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -820,10 +1026,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C322D9A-DAA8-F94B-8299-5D36BBA36BB2}">
-  <dimension ref="A1:K52"/>
+  <dimension ref="A1:L71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B37" workbookViewId="0">
-      <selection activeCell="D52" sqref="D52"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="D53" sqref="D53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -836,11 +1042,11 @@
     <col min="7" max="7" width="7.83203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9.33203125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="8.83203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8.83203125" customWidth="1"/>
-    <col min="11" max="11" width="80.1640625" customWidth="1"/>
+    <col min="10" max="11" width="8.83203125" customWidth="1"/>
+    <col min="12" max="12" width="80.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -872,10 +1078,13 @@
         <v>41</v>
       </c>
       <c r="K1" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="34" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" ht="34" x14ac:dyDescent="0.2">
       <c r="A2" s="5">
         <v>44277</v>
       </c>
@@ -906,11 +1115,11 @@
       <c r="J2">
         <v>0.3</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="L2" s="2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" s="5">
         <v>44277</v>
       </c>
@@ -941,11 +1150,11 @@
       <c r="J3">
         <v>0.3</v>
       </c>
-      <c r="K3" t="s">
+      <c r="L3" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="85" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" ht="85" x14ac:dyDescent="0.2">
       <c r="A4" s="5">
         <v>44277</v>
       </c>
@@ -976,11 +1185,11 @@
       <c r="J4">
         <v>0.3</v>
       </c>
-      <c r="K4" s="2" t="s">
+      <c r="L4" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="68" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12" ht="68" x14ac:dyDescent="0.2">
       <c r="A5" s="5">
         <v>44277</v>
       </c>
@@ -1011,11 +1220,11 @@
       <c r="J5">
         <v>0.3</v>
       </c>
-      <c r="K5" s="2" t="s">
+      <c r="L5" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="272" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12" ht="272" x14ac:dyDescent="0.2">
       <c r="A6" s="5">
         <v>44277</v>
       </c>
@@ -1031,11 +1240,11 @@
       <c r="J6">
         <v>0.3</v>
       </c>
-      <c r="K6" s="4" t="s">
+      <c r="L6" s="4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="102" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12" ht="102" x14ac:dyDescent="0.2">
       <c r="A7" s="5">
         <v>44277</v>
       </c>
@@ -1066,11 +1275,11 @@
       <c r="J7">
         <v>0.3</v>
       </c>
-      <c r="K7" s="4" t="s">
+      <c r="L7" s="4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="34" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12" ht="34" x14ac:dyDescent="0.2">
       <c r="A8" s="5">
         <v>44277</v>
       </c>
@@ -1101,11 +1310,11 @@
       <c r="J8">
         <v>0.3</v>
       </c>
-      <c r="K8" s="4" t="s">
+      <c r="L8" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="136" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:12" ht="136" x14ac:dyDescent="0.2">
       <c r="A9" s="5">
         <v>44277</v>
       </c>
@@ -1136,11 +1345,11 @@
       <c r="J9">
         <v>0.3</v>
       </c>
-      <c r="K9" s="4" t="s">
+      <c r="L9" s="4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="51" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:12" ht="51" x14ac:dyDescent="0.2">
       <c r="A10" s="5">
         <v>44277</v>
       </c>
@@ -1171,11 +1380,11 @@
       <c r="J10">
         <v>0.3</v>
       </c>
-      <c r="K10" s="2" t="s">
+      <c r="L10" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" s="5">
         <v>44278</v>
       </c>
@@ -1206,11 +1415,11 @@
       <c r="J11">
         <v>0.3</v>
       </c>
-      <c r="K11" t="s">
+      <c r="L11" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12" s="5">
         <v>44278</v>
       </c>
@@ -1241,11 +1450,11 @@
       <c r="J12">
         <v>0.3</v>
       </c>
-      <c r="K12" t="s">
+      <c r="L12" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13" s="5">
         <v>44278</v>
       </c>
@@ -1276,11 +1485,11 @@
       <c r="J13">
         <v>0.3</v>
       </c>
-      <c r="K13" t="s">
+      <c r="L13" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14" s="5">
         <v>44278</v>
       </c>
@@ -1311,11 +1520,11 @@
       <c r="J14">
         <v>0.3</v>
       </c>
-      <c r="K14" t="s">
+      <c r="L14" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15" s="5">
         <v>44278</v>
       </c>
@@ -1346,11 +1555,11 @@
       <c r="J15">
         <v>0.3</v>
       </c>
-      <c r="K15" t="s">
+      <c r="L15" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="34" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:12" ht="34" x14ac:dyDescent="0.2">
       <c r="A16" s="5">
         <v>44278</v>
       </c>
@@ -1381,11 +1590,11 @@
       <c r="J16">
         <v>0.3</v>
       </c>
-      <c r="K16" s="2" t="s">
+      <c r="L16" s="2" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="85" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:12" ht="85" x14ac:dyDescent="0.2">
       <c r="A17" s="5">
         <v>44278</v>
       </c>
@@ -1416,11 +1625,11 @@
       <c r="J17">
         <v>0.3</v>
       </c>
-      <c r="K17" s="2" t="s">
+      <c r="L17" s="2" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A18" s="5">
         <v>44278</v>
       </c>
@@ -1451,11 +1660,11 @@
       <c r="J18">
         <v>0.3</v>
       </c>
-      <c r="K18" t="s">
+      <c r="L18" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="19" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" s="5">
         <v>44278</v>
       </c>
@@ -1486,11 +1695,11 @@
       <c r="J19">
         <v>0.3</v>
       </c>
-      <c r="K19" s="2" t="s">
+      <c r="L19" s="2" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A20" s="5">
         <v>44278</v>
       </c>
@@ -1521,11 +1730,11 @@
       <c r="J20">
         <v>0.3</v>
       </c>
-      <c r="K20" t="s">
+      <c r="L20" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="66" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:12" ht="66" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="5">
         <v>44278</v>
       </c>
@@ -1556,11 +1765,11 @@
       <c r="J21">
         <v>0.5</v>
       </c>
-      <c r="K21" s="4" t="s">
+      <c r="L21" s="4" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A22" s="5">
         <v>44278</v>
       </c>
@@ -1591,11 +1800,11 @@
       <c r="J22">
         <v>0.5</v>
       </c>
-      <c r="K22" s="6" t="s">
+      <c r="L22" s="6" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="23" spans="1:11" ht="51" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:12" ht="51" x14ac:dyDescent="0.2">
       <c r="A23" s="5">
         <v>44278</v>
       </c>
@@ -1626,11 +1835,11 @@
       <c r="J23">
         <v>0.5</v>
       </c>
-      <c r="K23" s="4" t="s">
+      <c r="L23" s="4" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A24" s="5">
         <v>44278</v>
       </c>
@@ -1661,11 +1870,11 @@
       <c r="J24">
         <v>0.5</v>
       </c>
-      <c r="K24" s="6" t="s">
+      <c r="L24" s="6" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="25" spans="1:11" ht="34" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:12" ht="34" x14ac:dyDescent="0.2">
       <c r="A25" s="5">
         <v>44278</v>
       </c>
@@ -1696,11 +1905,11 @@
       <c r="J25">
         <v>0.5</v>
       </c>
-      <c r="K25" s="4" t="s">
+      <c r="L25" s="4" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A26" s="5">
         <v>44278</v>
       </c>
@@ -1731,11 +1940,11 @@
       <c r="J26">
         <v>0.5</v>
       </c>
-      <c r="K26" s="6" t="s">
+      <c r="L26" s="6" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="27" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A27" s="5">
         <v>44278</v>
       </c>
@@ -1766,11 +1975,11 @@
       <c r="J27">
         <v>0.5</v>
       </c>
-      <c r="K27" s="4" t="s">
+      <c r="L27" s="4" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="28" spans="1:11" ht="34" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:12" ht="34" x14ac:dyDescent="0.2">
       <c r="A28" s="5">
         <v>44278</v>
       </c>
@@ -1801,11 +2010,11 @@
       <c r="J28">
         <v>0.5</v>
       </c>
-      <c r="K28" s="4" t="s">
+      <c r="L28" s="4" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="29" spans="1:11" ht="34" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:12" ht="34" x14ac:dyDescent="0.2">
       <c r="A29" s="5">
         <v>44278</v>
       </c>
@@ -1836,11 +2045,11 @@
       <c r="J29">
         <v>0.5</v>
       </c>
-      <c r="K29" s="4" t="s">
+      <c r="L29" s="4" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="30" spans="1:11" ht="34" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:12" ht="34" x14ac:dyDescent="0.2">
       <c r="A30" s="5">
         <v>44278</v>
       </c>
@@ -1871,11 +2080,11 @@
       <c r="J30">
         <v>0.5</v>
       </c>
-      <c r="K30" s="4" t="s">
+      <c r="L30" s="4" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="31" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A31" s="5">
         <v>44278</v>
       </c>
@@ -1906,11 +2115,11 @@
       <c r="J31">
         <v>0.5</v>
       </c>
-      <c r="K31" s="4" t="s">
+      <c r="L31" s="4" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="32" spans="1:11" ht="51" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:12" ht="51" x14ac:dyDescent="0.2">
       <c r="A32" s="5">
         <v>44278</v>
       </c>
@@ -1941,11 +2150,11 @@
       <c r="J32">
         <v>0.5</v>
       </c>
-      <c r="K32" s="4" t="s">
+      <c r="L32" s="4" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="33" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A33" s="5">
         <v>44278</v>
       </c>
@@ -1976,11 +2185,11 @@
       <c r="J33">
         <v>0.5</v>
       </c>
-      <c r="K33" s="4" t="s">
+      <c r="L33" s="4" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="34" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A34" s="5">
         <v>44278</v>
       </c>
@@ -2011,11 +2220,11 @@
       <c r="J34">
         <v>0.5</v>
       </c>
-      <c r="K34" s="4" t="s">
+      <c r="L34" s="4" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="35" spans="1:11" ht="34" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:12" ht="34" x14ac:dyDescent="0.2">
       <c r="A35" s="5">
         <v>44278</v>
       </c>
@@ -2046,11 +2255,11 @@
       <c r="J35">
         <v>0.5</v>
       </c>
-      <c r="K35" s="4" t="s">
+      <c r="L35" s="4" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="36" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A36" s="5">
         <v>44279</v>
       </c>
@@ -2081,11 +2290,11 @@
       <c r="J36">
         <v>0.5</v>
       </c>
-      <c r="K36" s="4" t="s">
+      <c r="L36" s="4" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A37" s="5">
         <v>44279</v>
       </c>
@@ -2116,46 +2325,49 @@
       <c r="J37">
         <v>0.5</v>
       </c>
-      <c r="K37" s="6" t="s">
+      <c r="L37" s="6" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="38" spans="1:11" ht="17" x14ac:dyDescent="0.2">
-      <c r="A38" s="5">
+    <row r="38" spans="1:12" s="20" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A38" s="18">
         <v>44279</v>
       </c>
-      <c r="B38" s="3">
+      <c r="B38" s="19">
         <v>0.56388888888888888</v>
       </c>
-      <c r="C38" t="s">
+      <c r="C38" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="D38" t="s">
+      <c r="D38" s="20" t="s">
         <v>99</v>
       </c>
-      <c r="E38">
+      <c r="E38" s="20">
         <v>0.4</v>
       </c>
-      <c r="F38">
+      <c r="F38" s="20">
         <v>0.04</v>
       </c>
-      <c r="G38">
-        <v>4</v>
-      </c>
-      <c r="H38">
-        <v>1</v>
-      </c>
-      <c r="I38">
-        <v>0</v>
-      </c>
-      <c r="J38">
-        <v>0.5</v>
-      </c>
-      <c r="K38" s="4" t="s">
+      <c r="G38" s="20">
+        <v>4</v>
+      </c>
+      <c r="H38" s="20">
+        <v>1</v>
+      </c>
+      <c r="I38" s="20">
+        <v>0</v>
+      </c>
+      <c r="J38" s="20">
+        <v>0.5</v>
+      </c>
+      <c r="K38" s="20" t="s">
+        <v>120</v>
+      </c>
+      <c r="L38" s="21" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A39" s="5">
         <v>44279</v>
       </c>
@@ -2186,46 +2398,52 @@
       <c r="J39">
         <v>0.5</v>
       </c>
-      <c r="K39" s="6" t="s">
+      <c r="K39" t="s">
+        <v>121</v>
+      </c>
+      <c r="L39" s="6" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="40" spans="1:11" ht="17" x14ac:dyDescent="0.2">
-      <c r="A40" s="5">
+    <row r="40" spans="1:12" s="20" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A40" s="18">
         <v>44279</v>
       </c>
-      <c r="B40" s="3">
+      <c r="B40" s="19">
         <v>0.57361111111111118</v>
       </c>
-      <c r="C40" t="s">
+      <c r="C40" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="D40" t="s">
+      <c r="D40" s="20" t="s">
         <v>97</v>
       </c>
-      <c r="E40">
+      <c r="E40" s="20">
         <v>0.4</v>
       </c>
-      <c r="F40">
+      <c r="F40" s="20">
         <v>0.04</v>
       </c>
-      <c r="G40">
-        <v>4</v>
-      </c>
-      <c r="H40">
-        <v>1</v>
-      </c>
-      <c r="I40">
-        <v>0</v>
-      </c>
-      <c r="J40">
-        <v>0.5</v>
-      </c>
-      <c r="K40" s="4" t="s">
+      <c r="G40" s="20">
+        <v>4</v>
+      </c>
+      <c r="H40" s="20">
+        <v>1</v>
+      </c>
+      <c r="I40" s="20">
+        <v>0</v>
+      </c>
+      <c r="J40" s="20">
+        <v>0.5</v>
+      </c>
+      <c r="K40" s="20" t="s">
+        <v>120</v>
+      </c>
+      <c r="L40" s="21" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="41" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A41" s="5">
         <v>44279</v>
       </c>
@@ -2256,46 +2474,52 @@
       <c r="J41">
         <v>0.5</v>
       </c>
-      <c r="K41" s="4" t="s">
+      <c r="K41" t="s">
+        <v>121</v>
+      </c>
+      <c r="L41" s="4" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="42" spans="1:11" ht="85" x14ac:dyDescent="0.2">
-      <c r="A42" s="7">
+    <row r="42" spans="1:12" s="25" customFormat="1" ht="85" x14ac:dyDescent="0.2">
+      <c r="A42" s="22">
         <v>44279</v>
       </c>
-      <c r="B42" s="8">
+      <c r="B42" s="23">
         <v>0.59930555555555554</v>
       </c>
-      <c r="C42" s="9" t="s">
+      <c r="C42" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="D42" t="s">
+      <c r="D42" s="25" t="s">
         <v>95</v>
       </c>
-      <c r="E42" s="9">
+      <c r="E42" s="24">
         <v>0.4</v>
       </c>
-      <c r="F42" s="9">
+      <c r="F42" s="24">
         <v>0.04</v>
       </c>
-      <c r="G42" s="9">
-        <v>4</v>
-      </c>
-      <c r="H42" s="9">
-        <v>1</v>
-      </c>
-      <c r="I42" s="9">
-        <v>0</v>
-      </c>
-      <c r="J42" s="9">
-        <v>0.5</v>
-      </c>
-      <c r="K42" s="10" t="s">
+      <c r="G42" s="24">
+        <v>4</v>
+      </c>
+      <c r="H42" s="24">
+        <v>1</v>
+      </c>
+      <c r="I42" s="24">
+        <v>0</v>
+      </c>
+      <c r="J42" s="24">
+        <v>0.5</v>
+      </c>
+      <c r="K42" s="24" t="s">
+        <v>120</v>
+      </c>
+      <c r="L42" s="26" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="43" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A43" s="7">
         <v>44279</v>
       </c>
@@ -2326,46 +2550,52 @@
       <c r="J43" s="9">
         <v>0.5</v>
       </c>
-      <c r="K43" s="4" t="s">
+      <c r="K43" s="9" t="s">
+        <v>121</v>
+      </c>
+      <c r="L43" s="4" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="44" spans="1:11" ht="17" x14ac:dyDescent="0.2">
-      <c r="A44" s="7">
+    <row r="44" spans="1:12" s="11" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A44" s="13">
         <v>44279</v>
       </c>
-      <c r="B44" s="3">
+      <c r="B44" s="10">
         <v>0.61736111111111114</v>
       </c>
-      <c r="C44" s="9" t="s">
+      <c r="C44" s="14" t="s">
         <v>83</v>
       </c>
-      <c r="D44" t="s">
+      <c r="D44" s="11" t="s">
         <v>93</v>
       </c>
-      <c r="E44" s="9">
+      <c r="E44" s="14">
         <v>0.4</v>
       </c>
-      <c r="F44" s="9">
+      <c r="F44" s="14">
         <v>0.04</v>
       </c>
-      <c r="G44" s="9">
-        <v>4</v>
-      </c>
-      <c r="H44" s="9">
-        <v>1</v>
-      </c>
-      <c r="I44" s="9">
-        <v>0</v>
-      </c>
-      <c r="J44" s="9">
-        <v>0.5</v>
-      </c>
-      <c r="K44" s="4" t="s">
+      <c r="G44" s="14">
+        <v>4</v>
+      </c>
+      <c r="H44" s="14">
+        <v>1</v>
+      </c>
+      <c r="I44" s="14">
+        <v>0</v>
+      </c>
+      <c r="J44" s="14">
+        <v>0.5</v>
+      </c>
+      <c r="K44" s="14" t="s">
+        <v>120</v>
+      </c>
+      <c r="L44" s="12" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="45" spans="1:11" ht="34" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:12" ht="34" x14ac:dyDescent="0.2">
       <c r="A45" s="7">
         <v>44280</v>
       </c>
@@ -2396,46 +2626,52 @@
       <c r="J45" s="9">
         <v>0.5</v>
       </c>
-      <c r="K45" s="4" t="s">
+      <c r="K45" s="9" t="s">
+        <v>121</v>
+      </c>
+      <c r="L45" s="4" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="46" spans="1:11" ht="17" x14ac:dyDescent="0.2">
-      <c r="A46" s="7">
+    <row r="46" spans="1:12" s="17" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A46" s="15">
         <v>44280</v>
       </c>
-      <c r="B46" s="3">
+      <c r="B46" s="29">
         <v>0.57777777777777783</v>
       </c>
-      <c r="C46" s="9" t="s">
+      <c r="C46" s="16" t="s">
         <v>102</v>
       </c>
-      <c r="D46" t="s">
+      <c r="D46" s="17" t="s">
         <v>112</v>
       </c>
-      <c r="E46" s="9">
+      <c r="E46" s="16">
         <v>0.4</v>
       </c>
-      <c r="F46" s="9">
+      <c r="F46" s="16">
         <v>0.04</v>
       </c>
-      <c r="G46" s="9">
-        <v>4</v>
-      </c>
-      <c r="H46" s="9">
-        <v>1</v>
-      </c>
-      <c r="I46" s="9">
-        <v>0</v>
-      </c>
-      <c r="J46" s="9">
-        <v>0.5</v>
-      </c>
-      <c r="K46" s="4" t="s">
+      <c r="G46" s="16">
+        <v>4</v>
+      </c>
+      <c r="H46" s="16">
+        <v>1</v>
+      </c>
+      <c r="I46" s="16">
+        <v>0</v>
+      </c>
+      <c r="J46" s="16">
+        <v>0.5</v>
+      </c>
+      <c r="K46" s="16" t="s">
+        <v>120</v>
+      </c>
+      <c r="L46" s="30" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="47" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A47" s="7">
         <v>44280</v>
       </c>
@@ -2466,81 +2702,90 @@
       <c r="J47" s="9">
         <v>0.5</v>
       </c>
-      <c r="K47" s="2" t="s">
+      <c r="K47" s="9" t="s">
+        <v>121</v>
+      </c>
+      <c r="L47" s="2" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="48" spans="1:11" ht="51" x14ac:dyDescent="0.2">
-      <c r="A48" s="7">
+    <row r="48" spans="1:12" s="17" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+      <c r="A48" s="15">
         <v>44280</v>
       </c>
-      <c r="B48" s="3">
+      <c r="B48" s="29">
         <v>0.58819444444444446</v>
       </c>
-      <c r="C48" s="9" t="s">
+      <c r="C48" s="16" t="s">
         <v>102</v>
       </c>
-      <c r="D48" t="s">
+      <c r="D48" s="17" t="s">
         <v>114</v>
       </c>
-      <c r="E48" s="9">
+      <c r="E48" s="16">
         <v>0.4</v>
       </c>
-      <c r="F48" s="9">
+      <c r="F48" s="16">
         <v>0.04</v>
       </c>
-      <c r="G48" s="9">
-        <v>4</v>
-      </c>
-      <c r="H48" s="9">
-        <v>1</v>
-      </c>
-      <c r="I48" s="9">
-        <v>0</v>
-      </c>
-      <c r="J48" s="9">
-        <v>0.5</v>
-      </c>
-      <c r="K48" s="4" t="s">
+      <c r="G48" s="16">
+        <v>4</v>
+      </c>
+      <c r="H48" s="16">
+        <v>1</v>
+      </c>
+      <c r="I48" s="16">
+        <v>0</v>
+      </c>
+      <c r="J48" s="16">
+        <v>0.5</v>
+      </c>
+      <c r="K48" s="16" t="s">
+        <v>120</v>
+      </c>
+      <c r="L48" s="30" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="49" spans="1:11" ht="17" x14ac:dyDescent="0.2">
-      <c r="A49" s="7">
+    <row r="49" spans="1:12" s="25" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A49" s="22">
         <v>44280</v>
       </c>
-      <c r="B49" s="3">
+      <c r="B49" s="27">
         <v>0.59583333333333333</v>
       </c>
-      <c r="C49" s="9" t="s">
+      <c r="C49" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="D49" t="s">
+      <c r="D49" s="25" t="s">
         <v>115</v>
       </c>
-      <c r="E49" s="9">
+      <c r="E49" s="24">
         <v>0.4</v>
       </c>
-      <c r="F49" s="9">
+      <c r="F49" s="24">
         <v>0.04</v>
       </c>
-      <c r="G49" s="9">
-        <v>4</v>
-      </c>
-      <c r="H49" s="9">
-        <v>1</v>
-      </c>
-      <c r="I49" s="9">
-        <v>0</v>
-      </c>
-      <c r="J49" s="9">
-        <v>0.5</v>
-      </c>
-      <c r="K49" s="4" t="s">
+      <c r="G49" s="24">
+        <v>4</v>
+      </c>
+      <c r="H49" s="24">
+        <v>1</v>
+      </c>
+      <c r="I49" s="24">
+        <v>0</v>
+      </c>
+      <c r="J49" s="24">
+        <v>0.5</v>
+      </c>
+      <c r="K49" s="24" t="s">
+        <v>120</v>
+      </c>
+      <c r="L49" s="28" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="50" spans="1:11" ht="34" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:12" ht="34" x14ac:dyDescent="0.2">
       <c r="A50" s="7">
         <v>44280</v>
       </c>
@@ -2571,46 +2816,52 @@
       <c r="J50" s="9">
         <v>0.5</v>
       </c>
-      <c r="K50" s="4" t="s">
+      <c r="K50" s="9" t="s">
+        <v>121</v>
+      </c>
+      <c r="L50" s="4" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="51" spans="1:11" ht="17" x14ac:dyDescent="0.2">
-      <c r="A51" s="7">
+    <row r="51" spans="1:12" s="25" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A51" s="22">
         <v>44280</v>
       </c>
-      <c r="B51" s="3">
+      <c r="B51" s="27">
         <v>0.6069444444444444</v>
       </c>
-      <c r="C51" s="9" t="s">
+      <c r="C51" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="D51" t="s">
+      <c r="D51" s="25" t="s">
         <v>117</v>
       </c>
-      <c r="E51" s="9">
+      <c r="E51" s="24">
         <v>0.4</v>
       </c>
-      <c r="F51" s="9">
+      <c r="F51" s="24">
         <v>0.04</v>
       </c>
-      <c r="G51" s="9">
-        <v>4</v>
-      </c>
-      <c r="H51" s="9">
-        <v>1</v>
-      </c>
-      <c r="I51" s="9">
-        <v>0</v>
-      </c>
-      <c r="J51" s="9">
-        <v>0.5</v>
-      </c>
-      <c r="K51" s="4" t="s">
+      <c r="G51" s="24">
+        <v>4</v>
+      </c>
+      <c r="H51" s="24">
+        <v>1</v>
+      </c>
+      <c r="I51" s="24">
+        <v>0</v>
+      </c>
+      <c r="J51" s="24">
+        <v>0.5</v>
+      </c>
+      <c r="K51" s="24" t="s">
+        <v>120</v>
+      </c>
+      <c r="L51" s="28" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="52" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A52" s="5">
         <v>44280</v>
       </c>
@@ -2641,11 +2892,716 @@
       <c r="J52" s="9">
         <v>0.5</v>
       </c>
-      <c r="K52" s="4" t="s">
+      <c r="K52" s="9" t="s">
+        <v>121</v>
+      </c>
+      <c r="L52" s="4" t="s">
         <v>110</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A53" s="5">
+        <v>44282</v>
+      </c>
+      <c r="B53" s="3">
+        <v>0.46319444444444446</v>
+      </c>
+      <c r="C53" t="s">
+        <v>9</v>
+      </c>
+      <c r="D53" t="s">
+        <v>156</v>
+      </c>
+      <c r="E53">
+        <v>0.4</v>
+      </c>
+      <c r="F53">
+        <v>0.04</v>
+      </c>
+      <c r="G53">
+        <v>4</v>
+      </c>
+      <c r="H53">
+        <v>1</v>
+      </c>
+      <c r="I53">
+        <v>0</v>
+      </c>
+      <c r="J53">
+        <v>0.5</v>
+      </c>
+      <c r="K53" t="s">
+        <v>121</v>
+      </c>
+      <c r="L53" s="6" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A54" s="18">
+        <v>44282</v>
+      </c>
+      <c r="B54" s="19">
+        <v>0.46458333333333335</v>
+      </c>
+      <c r="C54" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="D54" s="20" t="s">
+        <v>155</v>
+      </c>
+      <c r="E54" s="20">
+        <v>0.4</v>
+      </c>
+      <c r="F54" s="20">
+        <v>0.04</v>
+      </c>
+      <c r="G54" s="20">
+        <v>4</v>
+      </c>
+      <c r="H54" s="20">
+        <v>1</v>
+      </c>
+      <c r="I54" s="20">
+        <v>0</v>
+      </c>
+      <c r="J54" s="20">
+        <v>0.5</v>
+      </c>
+      <c r="K54" s="20" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12" ht="34" x14ac:dyDescent="0.2">
+      <c r="A55" s="5">
+        <v>44282</v>
+      </c>
+      <c r="B55" s="3">
+        <v>0.46875</v>
+      </c>
+      <c r="C55" t="s">
+        <v>9</v>
+      </c>
+      <c r="D55" t="s">
+        <v>154</v>
+      </c>
+      <c r="E55">
+        <v>0.4</v>
+      </c>
+      <c r="F55">
+        <v>0.04</v>
+      </c>
+      <c r="G55">
+        <v>4</v>
+      </c>
+      <c r="H55">
+        <v>1</v>
+      </c>
+      <c r="I55">
+        <v>0</v>
+      </c>
+      <c r="J55">
+        <v>0.5</v>
+      </c>
+      <c r="K55" t="s">
+        <v>126</v>
+      </c>
+      <c r="L55" s="4" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12" ht="68" x14ac:dyDescent="0.2">
+      <c r="A56" s="5">
+        <v>44282</v>
+      </c>
+      <c r="B56" s="3">
+        <v>0.47361111111111115</v>
+      </c>
+      <c r="C56" t="s">
+        <v>9</v>
+      </c>
+      <c r="D56" t="s">
+        <v>153</v>
+      </c>
+      <c r="E56">
+        <v>0.4</v>
+      </c>
+      <c r="F56">
+        <v>0.04</v>
+      </c>
+      <c r="G56">
+        <v>4</v>
+      </c>
+      <c r="H56">
+        <v>1</v>
+      </c>
+      <c r="I56">
+        <v>0</v>
+      </c>
+      <c r="J56">
+        <v>0.5</v>
+      </c>
+      <c r="K56" t="s">
+        <v>126</v>
+      </c>
+      <c r="L56" s="4" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="57" spans="1:12" ht="17" x14ac:dyDescent="0.2">
+      <c r="A57" s="5">
+        <v>44282</v>
+      </c>
+      <c r="B57" s="3">
+        <v>0.4777777777777778</v>
+      </c>
+      <c r="C57" t="s">
+        <v>9</v>
+      </c>
+      <c r="D57" t="s">
+        <v>152</v>
+      </c>
+      <c r="E57">
+        <v>0.4</v>
+      </c>
+      <c r="F57">
+        <v>0.04</v>
+      </c>
+      <c r="G57">
+        <v>4</v>
+      </c>
+      <c r="H57">
+        <v>1</v>
+      </c>
+      <c r="I57">
+        <v>0</v>
+      </c>
+      <c r="J57">
+        <v>0.5</v>
+      </c>
+      <c r="K57" t="s">
+        <v>126</v>
+      </c>
+      <c r="L57" s="4" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="58" spans="1:12" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A58" s="18">
+        <v>44282</v>
+      </c>
+      <c r="B58" s="19">
+        <v>0.4826388888888889</v>
+      </c>
+      <c r="C58" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="D58" s="20" t="s">
+        <v>151</v>
+      </c>
+      <c r="E58" s="20">
+        <v>0.4</v>
+      </c>
+      <c r="F58" s="20">
+        <v>0.04</v>
+      </c>
+      <c r="G58" s="20">
+        <v>4</v>
+      </c>
+      <c r="H58" s="20">
+        <v>1</v>
+      </c>
+      <c r="I58" s="20">
+        <v>0</v>
+      </c>
+      <c r="J58" s="20">
+        <v>0.5</v>
+      </c>
+      <c r="K58" s="20" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="59" spans="1:12" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A59" s="18">
+        <v>44282</v>
+      </c>
+      <c r="B59" s="19">
+        <v>0.48680555555555555</v>
+      </c>
+      <c r="C59" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="D59" s="20" t="s">
+        <v>150</v>
+      </c>
+      <c r="E59" s="20">
+        <v>0.4</v>
+      </c>
+      <c r="F59" s="20">
+        <v>0.04</v>
+      </c>
+      <c r="G59" s="20">
+        <v>4</v>
+      </c>
+      <c r="H59" s="20">
+        <v>1</v>
+      </c>
+      <c r="I59" s="20">
+        <v>0</v>
+      </c>
+      <c r="J59" s="20">
+        <v>0.5</v>
+      </c>
+      <c r="K59" s="20" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="60" spans="1:12" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A60" s="18">
+        <v>44282</v>
+      </c>
+      <c r="B60" s="19">
+        <v>0.4909722222222222</v>
+      </c>
+      <c r="C60" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="D60" s="20" t="s">
+        <v>149</v>
+      </c>
+      <c r="E60" s="20">
+        <v>0.4</v>
+      </c>
+      <c r="F60" s="20">
+        <v>0.04</v>
+      </c>
+      <c r="G60" s="20">
+        <v>4</v>
+      </c>
+      <c r="H60" s="20">
+        <v>1</v>
+      </c>
+      <c r="I60" s="20">
+        <v>0</v>
+      </c>
+      <c r="J60" s="20">
+        <v>0.5</v>
+      </c>
+      <c r="K60" s="20" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="61" spans="1:12" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A61" s="18">
+        <v>44282</v>
+      </c>
+      <c r="B61" s="19">
+        <v>0.49583333333333335</v>
+      </c>
+      <c r="C61" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="D61" s="20" t="s">
+        <v>148</v>
+      </c>
+      <c r="E61" s="20">
+        <v>0.4</v>
+      </c>
+      <c r="F61" s="20">
+        <v>0.04</v>
+      </c>
+      <c r="G61" s="20">
+        <v>4</v>
+      </c>
+      <c r="H61" s="20">
+        <v>1</v>
+      </c>
+      <c r="I61" s="20">
+        <v>0</v>
+      </c>
+      <c r="J61" s="20">
+        <v>0.5</v>
+      </c>
+      <c r="K61" s="20" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="62" spans="1:12" s="33" customFormat="1" ht="85" x14ac:dyDescent="0.2">
+      <c r="A62" s="31">
+        <v>44282</v>
+      </c>
+      <c r="B62" s="32">
+        <v>0.5</v>
+      </c>
+      <c r="C62" s="33" t="s">
+        <v>127</v>
+      </c>
+      <c r="D62" s="33" t="s">
+        <v>147</v>
+      </c>
+      <c r="E62" s="33">
+        <v>0.4</v>
+      </c>
+      <c r="F62" s="33">
+        <v>0.04</v>
+      </c>
+      <c r="G62" s="33">
+        <v>4</v>
+      </c>
+      <c r="H62" s="33">
+        <v>1</v>
+      </c>
+      <c r="I62" s="33">
+        <v>0</v>
+      </c>
+      <c r="J62" s="33">
+        <v>0.5</v>
+      </c>
+      <c r="K62" s="33" t="s">
+        <v>120</v>
+      </c>
+      <c r="L62" s="34" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="63" spans="1:12" ht="68" x14ac:dyDescent="0.2">
+      <c r="A63" s="5">
+        <v>44282</v>
+      </c>
+      <c r="B63" s="3">
+        <v>0.50416666666666665</v>
+      </c>
+      <c r="C63" t="s">
+        <v>127</v>
+      </c>
+      <c r="D63" t="s">
+        <v>146</v>
+      </c>
+      <c r="E63">
+        <v>0.4</v>
+      </c>
+      <c r="F63">
+        <v>0.04</v>
+      </c>
+      <c r="G63">
+        <v>4</v>
+      </c>
+      <c r="H63">
+        <v>1</v>
+      </c>
+      <c r="I63">
+        <v>0</v>
+      </c>
+      <c r="J63">
+        <v>0.5</v>
+      </c>
+      <c r="L63" s="4" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="64" spans="1:12" ht="51" x14ac:dyDescent="0.2">
+      <c r="A64" s="5">
+        <v>44282</v>
+      </c>
+      <c r="B64" s="3">
+        <v>0.50902777777777775</v>
+      </c>
+      <c r="C64" t="s">
+        <v>127</v>
+      </c>
+      <c r="D64" t="s">
+        <v>145</v>
+      </c>
+      <c r="E64">
+        <v>0.4</v>
+      </c>
+      <c r="F64">
+        <v>0.04</v>
+      </c>
+      <c r="G64">
+        <v>4</v>
+      </c>
+      <c r="H64">
+        <v>1</v>
+      </c>
+      <c r="I64">
+        <v>0</v>
+      </c>
+      <c r="J64">
+        <v>0.5</v>
+      </c>
+      <c r="L64" s="4" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="65" spans="1:12" s="33" customFormat="1" ht="85" x14ac:dyDescent="0.2">
+      <c r="A65" s="31">
+        <v>44282</v>
+      </c>
+      <c r="B65" s="32">
+        <v>0.51180555555555551</v>
+      </c>
+      <c r="C65" s="33" t="s">
+        <v>127</v>
+      </c>
+      <c r="D65" s="33" t="s">
+        <v>144</v>
+      </c>
+      <c r="E65" s="33">
+        <v>0.4</v>
+      </c>
+      <c r="F65" s="33">
+        <v>0.04</v>
+      </c>
+      <c r="G65" s="33">
+        <v>4</v>
+      </c>
+      <c r="H65" s="33">
+        <v>1</v>
+      </c>
+      <c r="I65" s="33">
+        <v>0</v>
+      </c>
+      <c r="J65" s="33">
+        <v>0.5</v>
+      </c>
+      <c r="K65" s="33" t="s">
+        <v>120</v>
+      </c>
+      <c r="L65" s="34" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="66" spans="1:12" s="38" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A66" s="35">
+        <v>44280</v>
+      </c>
+      <c r="B66" s="36">
+        <v>0.59791666666666665</v>
+      </c>
+      <c r="C66" s="37" t="s">
+        <v>26</v>
+      </c>
+      <c r="D66" s="38" t="s">
+        <v>143</v>
+      </c>
+      <c r="E66" s="37">
+        <v>0.4</v>
+      </c>
+      <c r="F66" s="37">
+        <v>0.04</v>
+      </c>
+      <c r="G66" s="37">
+        <v>4</v>
+      </c>
+      <c r="H66" s="37">
+        <v>1</v>
+      </c>
+      <c r="I66" s="37">
+        <v>0</v>
+      </c>
+      <c r="J66" s="37">
+        <v>0.5</v>
+      </c>
+      <c r="K66" s="37" t="s">
+        <v>121</v>
+      </c>
+      <c r="L66" s="39" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="67" spans="1:12" s="38" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A67" s="35">
+        <v>44280</v>
+      </c>
+      <c r="B67" s="36">
+        <v>0.60069444444444442</v>
+      </c>
+      <c r="C67" s="37" t="s">
+        <v>26</v>
+      </c>
+      <c r="D67" s="38" t="s">
+        <v>142</v>
+      </c>
+      <c r="E67" s="37">
+        <v>0.4</v>
+      </c>
+      <c r="F67" s="37">
+        <v>0.04</v>
+      </c>
+      <c r="G67" s="37">
+        <v>4</v>
+      </c>
+      <c r="H67" s="37">
+        <v>1</v>
+      </c>
+      <c r="I67" s="37">
+        <v>0</v>
+      </c>
+      <c r="J67" s="37">
+        <v>0.5</v>
+      </c>
+      <c r="K67" s="37" t="s">
+        <v>121</v>
+      </c>
+      <c r="L67" s="39" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="68" spans="1:12" s="25" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A68" s="22">
+        <v>44280</v>
+      </c>
+      <c r="B68" s="27">
+        <v>0.60277777777777775</v>
+      </c>
+      <c r="C68" s="24" t="s">
+        <v>26</v>
+      </c>
+      <c r="D68" s="25" t="s">
+        <v>141</v>
+      </c>
+      <c r="E68" s="24">
+        <v>0.4</v>
+      </c>
+      <c r="F68" s="24">
+        <v>0.04</v>
+      </c>
+      <c r="G68" s="24">
+        <v>4</v>
+      </c>
+      <c r="H68" s="24">
+        <v>1</v>
+      </c>
+      <c r="I68" s="24">
+        <v>0</v>
+      </c>
+      <c r="J68" s="24">
+        <v>0.5</v>
+      </c>
+      <c r="K68" s="24" t="s">
+        <v>120</v>
+      </c>
+      <c r="L68" s="28" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="69" spans="1:12" s="25" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A69" s="22">
+        <v>44280</v>
+      </c>
+      <c r="B69" s="27">
+        <v>0.6118055555555556</v>
+      </c>
+      <c r="C69" s="24" t="s">
+        <v>26</v>
+      </c>
+      <c r="D69" s="25" t="s">
+        <v>140</v>
+      </c>
+      <c r="E69" s="24">
+        <v>0.4</v>
+      </c>
+      <c r="F69" s="24">
+        <v>0.04</v>
+      </c>
+      <c r="G69" s="24">
+        <v>4</v>
+      </c>
+      <c r="H69" s="24">
+        <v>1</v>
+      </c>
+      <c r="I69" s="24">
+        <v>0</v>
+      </c>
+      <c r="J69" s="24">
+        <v>0.5</v>
+      </c>
+      <c r="K69" s="24" t="s">
+        <v>120</v>
+      </c>
+      <c r="L69" s="28" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="70" spans="1:12" s="25" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A70" s="22">
+        <v>44280</v>
+      </c>
+      <c r="B70" s="27">
+        <v>0.62013888888888891</v>
+      </c>
+      <c r="C70" s="24" t="s">
+        <v>26</v>
+      </c>
+      <c r="D70" s="25" t="s">
+        <v>139</v>
+      </c>
+      <c r="E70" s="24">
+        <v>0.4</v>
+      </c>
+      <c r="F70" s="24">
+        <v>0.04</v>
+      </c>
+      <c r="G70" s="24">
+        <v>4</v>
+      </c>
+      <c r="H70" s="24">
+        <v>1</v>
+      </c>
+      <c r="I70" s="24">
+        <v>0</v>
+      </c>
+      <c r="J70" s="24">
+        <v>0.5</v>
+      </c>
+      <c r="K70" s="24" t="s">
+        <v>120</v>
+      </c>
+      <c r="L70" s="40" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="71" spans="1:12" ht="17" x14ac:dyDescent="0.2">
+      <c r="A71" s="5">
+        <v>44280</v>
+      </c>
+      <c r="B71" s="3">
+        <v>0.62986111111111109</v>
+      </c>
+      <c r="C71" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D71" t="s">
+        <v>138</v>
+      </c>
+      <c r="E71" s="9">
+        <v>0.4</v>
+      </c>
+      <c r="F71" s="9">
+        <v>0.04</v>
+      </c>
+      <c r="G71" s="9">
+        <v>4</v>
+      </c>
+      <c r="H71" s="9">
+        <v>1</v>
+      </c>
+      <c r="I71" s="9">
+        <v>0</v>
+      </c>
+      <c r="J71" s="9">
+        <v>0.5</v>
+      </c>
+      <c r="K71" s="9" t="s">
+        <v>121</v>
+      </c>
+      <c r="L71" s="4" t="s">
+        <v>137</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update mission logs and testing log file
</commit_message>
<xml_diff>
--- a/pearl_logs/PEARL_MOOS_testing_notes.xlsx
+++ b/pearl_logs/PEARL_MOOS_testing_notes.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maha/moos-ivp-pearl/pearl_logs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64940F8B-CD9E-FA44-9234-6F9D0412B994}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{107840C7-357B-1F46-81B8-024BD23A1629}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" xr2:uid="{CE7898E4-CB96-184C-9C00-2CBDA86B470B}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Testing Log" sheetId="1" r:id="rId1"/>
+    <sheet name="Pattern Testing" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="182">
   <si>
     <t>Date</t>
   </si>
@@ -567,6 +568,88 @@
   </si>
   <si>
     <t>LOG_PEARL_SQUARE_27_3_2021_____11_07_00</t>
+  </si>
+  <si>
+    <t>LOG_PEARL_SIMPLE_29_3_2021_____16_16_44</t>
+  </si>
+  <si>
+    <t>LOG_PEARL_SIMPLE_29_3_2021_____16_10_39</t>
+  </si>
+  <si>
+    <t>LOG_PEARL_SIMPLE_29_3_2021_____15_30_11</t>
+  </si>
+  <si>
+    <t>LOG_PEARL_SIMPLE_29_3_2021_____14_54_09</t>
+  </si>
+  <si>
+    <t>- lost gui at some point, but data still logging…</t>
+  </si>
+  <si>
+    <t>- wind got stronger around 3:53 PM ? Or just one big long gust?</t>
+  </si>
+  <si>
+    <t>Pattern Name</t>
+  </si>
+  <si>
+    <t>Test Log File Name</t>
+  </si>
+  <si>
+    <t>Good Test #</t>
+  </si>
+  <si>
+    <t>Star</t>
+  </si>
+  <si>
+    <t>Figure 8</t>
+  </si>
+  <si>
+    <t>Perimeter</t>
+  </si>
+  <si>
+    <t>LOG_PEARL_WAYPOINT_30_3_2021_____16_22_51</t>
+  </si>
+  <si>
+    <t>LOG_PEARL_WAYPOINT_30_3_2021_____16_11_26</t>
+  </si>
+  <si>
+    <t>LOG_PEARL_WAYPOINT_30_3_2021_____15_59_22</t>
+  </si>
+  <si>
+    <t>LOG_PEARL_WAYPOINT_30_3_2021_____15_45_20</t>
+  </si>
+  <si>
+    <t>LOG_PEARL_WAYPOINT_30_3_2021_____15_32_04</t>
+  </si>
+  <si>
+    <t>LOG_PEARL_WAYPOINT_30_3_2021_____15_18_35</t>
+  </si>
+  <si>
+    <t>- did really well!
+- slight wind, steady from the SW and some small gusts
+- did not make complete circuit…</t>
+  </si>
+  <si>
+    <t>- did not make complete circuit?</t>
+  </si>
+  <si>
+    <t>- CW rotation incremental thrust
+- followed by CCW rotation incremental thrust</t>
+  </si>
+  <si>
+    <t>Simple - Stationkeeping</t>
+  </si>
+  <si>
+    <t>- Stationkeeping with IMU heading used
+- Kept station for 2 mins, then used RC control to move out of watch circle, allowed to return to station, left there for remainder of 5-6 min mission</t>
+  </si>
+  <si>
+    <t>- Stationkeeping with GPS heading used
+- Kept station for 2 mins, then used RC control to move out of watch circle, allowed to return to station, left there for remainder of 5-6 min mission</t>
+  </si>
+  <si>
+    <t>- Forward incremental thrust
+- Backward incremental thrust
+- Then fast rotation with RC control</t>
   </si>
 </sst>
 </file>
@@ -597,7 +680,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -634,6 +717,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -647,7 +736,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -707,6 +796,10 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1026,10 +1119,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C322D9A-DAA8-F94B-8299-5D36BBA36BB2}">
-  <dimension ref="A1:L71"/>
+  <dimension ref="A1:L81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="D53" sqref="D53"/>
+    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="A76" sqref="A76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3600,8 +3693,685 @@
         <v>137</v>
       </c>
     </row>
+    <row r="72" spans="1:12" ht="34" x14ac:dyDescent="0.2">
+      <c r="A72" s="5">
+        <v>44284</v>
+      </c>
+      <c r="B72" s="3">
+        <v>0.62083333333333335</v>
+      </c>
+      <c r="C72" s="37" t="s">
+        <v>13</v>
+      </c>
+      <c r="D72" t="s">
+        <v>160</v>
+      </c>
+      <c r="E72" s="9">
+        <v>0.4</v>
+      </c>
+      <c r="F72" s="9">
+        <v>0.04</v>
+      </c>
+      <c r="G72" s="9">
+        <v>4</v>
+      </c>
+      <c r="H72" s="9">
+        <v>1</v>
+      </c>
+      <c r="I72" s="9">
+        <v>0</v>
+      </c>
+      <c r="J72" s="9">
+        <v>0.5</v>
+      </c>
+      <c r="L72" s="4" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="73" spans="1:12" ht="51" x14ac:dyDescent="0.2">
+      <c r="A73" s="5">
+        <v>44284</v>
+      </c>
+      <c r="B73" s="3">
+        <v>0.64583333333333337</v>
+      </c>
+      <c r="C73" s="37" t="s">
+        <v>13</v>
+      </c>
+      <c r="D73" t="s">
+        <v>159</v>
+      </c>
+      <c r="E73" s="9">
+        <v>0.4</v>
+      </c>
+      <c r="F73" s="9">
+        <v>0.04</v>
+      </c>
+      <c r="G73" s="9">
+        <v>4</v>
+      </c>
+      <c r="H73" s="9">
+        <v>1</v>
+      </c>
+      <c r="I73" s="9">
+        <v>0</v>
+      </c>
+      <c r="J73" s="9">
+        <v>0.5</v>
+      </c>
+      <c r="L73" s="4" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="74" spans="1:12" ht="51" x14ac:dyDescent="0.2">
+      <c r="A74" s="5">
+        <v>44284</v>
+      </c>
+      <c r="B74" s="3">
+        <v>0.67361111111111116</v>
+      </c>
+      <c r="C74" s="37" t="s">
+        <v>178</v>
+      </c>
+      <c r="D74" t="s">
+        <v>158</v>
+      </c>
+      <c r="E74" s="9">
+        <v>0.4</v>
+      </c>
+      <c r="F74" s="9">
+        <v>0.04</v>
+      </c>
+      <c r="G74" s="9">
+        <v>4</v>
+      </c>
+      <c r="H74" s="9">
+        <v>1</v>
+      </c>
+      <c r="I74" s="9">
+        <v>0</v>
+      </c>
+      <c r="J74" s="9">
+        <v>0.5</v>
+      </c>
+      <c r="L74" s="4" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="75" spans="1:12" ht="51" x14ac:dyDescent="0.2">
+      <c r="A75" s="5">
+        <v>44284</v>
+      </c>
+      <c r="B75" s="3">
+        <v>0.6777777777777777</v>
+      </c>
+      <c r="C75" s="37" t="s">
+        <v>178</v>
+      </c>
+      <c r="D75" t="s">
+        <v>157</v>
+      </c>
+      <c r="E75" s="9">
+        <v>0.4</v>
+      </c>
+      <c r="F75" s="9">
+        <v>0.04</v>
+      </c>
+      <c r="G75" s="9">
+        <v>4</v>
+      </c>
+      <c r="H75" s="9">
+        <v>1</v>
+      </c>
+      <c r="I75" s="9">
+        <v>0</v>
+      </c>
+      <c r="J75" s="9">
+        <v>0.5</v>
+      </c>
+      <c r="L75" s="4" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="76" spans="1:12" ht="51" x14ac:dyDescent="0.2">
+      <c r="A76" s="5">
+        <v>44285</v>
+      </c>
+      <c r="B76" s="3">
+        <v>0.63888888888888895</v>
+      </c>
+      <c r="C76" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="D76" t="s">
+        <v>174</v>
+      </c>
+      <c r="E76" s="9">
+        <v>0.4</v>
+      </c>
+      <c r="F76" s="9">
+        <v>0.04</v>
+      </c>
+      <c r="G76" s="9">
+        <v>4</v>
+      </c>
+      <c r="H76" s="9">
+        <v>1</v>
+      </c>
+      <c r="I76" s="9">
+        <v>0</v>
+      </c>
+      <c r="J76" s="9">
+        <v>0.5</v>
+      </c>
+      <c r="K76" t="s">
+        <v>121</v>
+      </c>
+      <c r="L76" s="4" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="77" spans="1:12" s="11" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A77" s="41">
+        <v>44285</v>
+      </c>
+      <c r="B77" s="10">
+        <v>0.64652777777777781</v>
+      </c>
+      <c r="C77" s="14" t="s">
+        <v>83</v>
+      </c>
+      <c r="D77" s="11" t="s">
+        <v>173</v>
+      </c>
+      <c r="E77" s="14">
+        <v>0.4</v>
+      </c>
+      <c r="F77" s="14">
+        <v>0.04</v>
+      </c>
+      <c r="G77" s="14">
+        <v>4</v>
+      </c>
+      <c r="H77" s="14">
+        <v>1</v>
+      </c>
+      <c r="I77" s="14">
+        <v>0</v>
+      </c>
+      <c r="J77" s="14">
+        <v>0.5</v>
+      </c>
+      <c r="K77" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="L77" s="12" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="78" spans="1:12" s="11" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A78" s="41">
+        <v>44285</v>
+      </c>
+      <c r="B78" s="10">
+        <v>0.65555555555555556</v>
+      </c>
+      <c r="C78" s="14" t="s">
+        <v>83</v>
+      </c>
+      <c r="D78" s="11" t="s">
+        <v>172</v>
+      </c>
+      <c r="E78" s="14">
+        <v>0.4</v>
+      </c>
+      <c r="F78" s="14">
+        <v>0.04</v>
+      </c>
+      <c r="G78" s="14">
+        <v>4</v>
+      </c>
+      <c r="H78" s="14">
+        <v>1</v>
+      </c>
+      <c r="I78" s="14">
+        <v>0</v>
+      </c>
+      <c r="J78" s="14">
+        <v>0.5</v>
+      </c>
+      <c r="K78" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="L78" s="12" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="79" spans="1:12" s="38" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A79" s="43">
+        <v>44285</v>
+      </c>
+      <c r="B79" s="36">
+        <v>0.66597222222222219</v>
+      </c>
+      <c r="C79" s="37" t="s">
+        <v>83</v>
+      </c>
+      <c r="D79" s="38" t="s">
+        <v>171</v>
+      </c>
+      <c r="E79" s="37">
+        <v>0.4</v>
+      </c>
+      <c r="F79" s="37">
+        <v>0.04</v>
+      </c>
+      <c r="G79" s="37">
+        <v>4</v>
+      </c>
+      <c r="H79" s="37">
+        <v>1</v>
+      </c>
+      <c r="I79" s="37">
+        <v>0</v>
+      </c>
+      <c r="J79" s="37">
+        <v>0.5</v>
+      </c>
+      <c r="K79" s="38" t="s">
+        <v>121</v>
+      </c>
+      <c r="L79" s="44" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="80" spans="1:12" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A80" s="41">
+        <v>44285</v>
+      </c>
+      <c r="B80" s="10">
+        <v>0.6743055555555556</v>
+      </c>
+      <c r="C80" s="14" t="s">
+        <v>83</v>
+      </c>
+      <c r="D80" s="11" t="s">
+        <v>170</v>
+      </c>
+      <c r="E80" s="14">
+        <v>0.4</v>
+      </c>
+      <c r="F80" s="14">
+        <v>0.04</v>
+      </c>
+      <c r="G80" s="14">
+        <v>4</v>
+      </c>
+      <c r="H80" s="14">
+        <v>1</v>
+      </c>
+      <c r="I80" s="14">
+        <v>0</v>
+      </c>
+      <c r="J80" s="14">
+        <v>0.5</v>
+      </c>
+      <c r="K80" s="11" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="81" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A81" s="41">
+        <v>44285</v>
+      </c>
+      <c r="B81" s="10">
+        <v>0.68263888888888891</v>
+      </c>
+      <c r="C81" s="14" t="s">
+        <v>83</v>
+      </c>
+      <c r="D81" s="11" t="s">
+        <v>169</v>
+      </c>
+      <c r="E81" s="14">
+        <v>0.4</v>
+      </c>
+      <c r="F81" s="14">
+        <v>0.04</v>
+      </c>
+      <c r="G81" s="14">
+        <v>4</v>
+      </c>
+      <c r="H81" s="14">
+        <v>1</v>
+      </c>
+      <c r="I81" s="14">
+        <v>0</v>
+      </c>
+      <c r="J81" s="14">
+        <v>0.5</v>
+      </c>
+      <c r="K81" s="11" t="s">
+        <v>120</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A800C2D-7086-3649-85CB-0A56FEC6D735}">
+  <dimension ref="A1:C29"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="45" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="20">
+        <v>1</v>
+      </c>
+      <c r="C2" s="20" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="20">
+        <v>2</v>
+      </c>
+      <c r="C3" s="20" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="20">
+        <v>3</v>
+      </c>
+      <c r="C4" s="20" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="20">
+        <v>4</v>
+      </c>
+      <c r="C5" s="20" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="20">
+        <v>5</v>
+      </c>
+      <c r="C6" s="20" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="20">
+        <v>6</v>
+      </c>
+      <c r="C7" s="20" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="20">
+        <v>7</v>
+      </c>
+      <c r="C8" s="20" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" s="25" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="25" t="s">
+        <v>166</v>
+      </c>
+      <c r="B9" s="25">
+        <v>1</v>
+      </c>
+      <c r="C9" s="25" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" s="25" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="25" t="s">
+        <v>166</v>
+      </c>
+      <c r="B10" s="25">
+        <v>2</v>
+      </c>
+      <c r="C10" s="25" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" s="25" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="25" t="s">
+        <v>166</v>
+      </c>
+      <c r="B11" s="25">
+        <v>3</v>
+      </c>
+      <c r="C11" s="25" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" s="25" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="25" t="s">
+        <v>166</v>
+      </c>
+      <c r="B12" s="25">
+        <v>4</v>
+      </c>
+      <c r="C12" s="25" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" s="25" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="25" t="s">
+        <v>166</v>
+      </c>
+      <c r="B13" s="25">
+        <v>5</v>
+      </c>
+      <c r="C13" s="25" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" s="25" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="25" t="s">
+        <v>166</v>
+      </c>
+      <c r="B14" s="25">
+        <v>6</v>
+      </c>
+      <c r="C14" s="25" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>166</v>
+      </c>
+      <c r="B15">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" s="17" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="17" t="s">
+        <v>167</v>
+      </c>
+      <c r="B16" s="17">
+        <v>1</v>
+      </c>
+      <c r="C16" s="17" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" s="17" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="17" t="s">
+        <v>167</v>
+      </c>
+      <c r="B17" s="17">
+        <v>2</v>
+      </c>
+      <c r="C17" s="17" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>167</v>
+      </c>
+      <c r="B18">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>167</v>
+      </c>
+      <c r="B19">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>167</v>
+      </c>
+      <c r="B20">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>167</v>
+      </c>
+      <c r="B21">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>167</v>
+      </c>
+      <c r="B22">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="11" t="s">
+        <v>168</v>
+      </c>
+      <c r="B23" s="11">
+        <v>1</v>
+      </c>
+      <c r="C23" s="42" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="11" t="s">
+        <v>168</v>
+      </c>
+      <c r="B24" s="11">
+        <v>2</v>
+      </c>
+      <c r="C24" s="11" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="11" t="s">
+        <v>168</v>
+      </c>
+      <c r="B25" s="11">
+        <v>3</v>
+      </c>
+      <c r="C25" s="11" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="11" t="s">
+        <v>168</v>
+      </c>
+      <c r="B26" s="11">
+        <v>4</v>
+      </c>
+      <c r="C26" s="11" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="11" t="s">
+        <v>168</v>
+      </c>
+      <c r="B27" s="11">
+        <v>5</v>
+      </c>
+      <c r="C27" s="11" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>168</v>
+      </c>
+      <c r="B28">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>168</v>
+      </c>
+      <c r="B29">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Upload mission screenshots and testing log for 2021-03-31
</commit_message>
<xml_diff>
--- a/pearl_logs/PEARL_MOOS_testing_notes.xlsx
+++ b/pearl_logs/PEARL_MOOS_testing_notes.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maha/moos-ivp-pearl/pearl_logs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{107840C7-357B-1F46-81B8-024BD23A1629}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71007550-24EA-814B-9A84-039B50814863}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" xr2:uid="{CE7898E4-CB96-184C-9C00-2CBDA86B470B}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" activeTab="1" xr2:uid="{CE7898E4-CB96-184C-9C00-2CBDA86B470B}"/>
   </bookViews>
   <sheets>
     <sheet name="Testing Log" sheetId="1" r:id="rId1"/>
     <sheet name="Pattern Testing" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="389" uniqueCount="214">
   <si>
     <t>Date</t>
   </si>
@@ -348,13 +349,6 @@
     <t>- trying star with new gains and lead ins - lost connection</t>
   </si>
   <si>
-    <t>- trying star with new gains and lead ins 
-- track points not showing up? But checked in code
-- track points showe dup
-- she did really well!
-- going to west star point, it was slow because of current? Coming back was much faster</t>
-  </si>
-  <si>
     <t>- timed out at 2:47 PM?</t>
   </si>
   <si>
@@ -501,9 +495,6 @@
 - could have been wind?</t>
   </si>
   <si>
-    <t>- windier than this morning. Pretty steady breeze coming from the SE</t>
-  </si>
-  <si>
     <t>- fair bit of wind seen in her 3rd leg - when she was going approximately upwind</t>
   </si>
   <si>
@@ -650,13 +641,126 @@
     <t>- Forward incremental thrust
 - Backward incremental thrust
 - Then fast rotation with RC control</t>
+  </si>
+  <si>
+    <t>- lost GUI almost right away?
+- Need to check if completed mission and all data logged
+- visually, seemed to shift pretty far north. Check in logged mission data</t>
+  </si>
+  <si>
+    <t>- got quite windy by 3:15 PM?</t>
+  </si>
+  <si>
+    <t>- complete the remaining patterns like figure 8 pattern</t>
+  </si>
+  <si>
+    <t>- add a new pattern which would be a “search pattern" that combines many elements of the other missions and would be useful in a realistic mission (like search and rescue or fishfarm monitoring), see attached PPT chart</t>
+  </si>
+  <si>
+    <t>- do a long term mission that lasts about 2-3 hours and could be done with the laptop from shore (so on the Westside of the pond) including extensive station-keeping and no “babysitting” of PEARL from the canoe</t>
+  </si>
+  <si>
+    <t>- do a nighttime mission. Equip PEARL with some LED lights (could be battery powered, separate from the main electronics) and do nightime operation when no charging and sunlight are available and observe the net power drain at night (and take some cool nightime time lapse video)</t>
+  </si>
+  <si>
+    <t>- repeat patterns a few more times (e.g. square pattern) to get some statistics on how well executes its missions after PID tuning has been completed</t>
+  </si>
+  <si>
+    <t>- some “stress testing” of PEARL at maximum thrust and doing step inputs, impulse function, using manual control to characterize her mass, CG location, dragt coefficient, dynamic behavior etc both in translational and rotational mode</t>
+  </si>
+  <si>
+    <t>- as you suggested on a sunny day enable sun tracking mode and operate say 30 min in sun-tracking mode, and then 30 minute in drift mode to characterize net energy generated with sun tracking and without to see if it is actually worth it.</t>
+  </si>
+  <si>
+    <t>- try starting and stopping a mission via Iridium, by having the “shoreside” MOOS-IVP running on PEARL and logging in remotely via Iridium (this would be a stretch goal). </t>
+  </si>
+  <si>
+    <t>DONE</t>
+  </si>
+  <si>
+    <t>PLAN FOR MONDAY/TUESDAY WITH OLI - CHECK WHEN LIGHTS ARRIVE</t>
+  </si>
+  <si>
+    <t>ALMOST DONE</t>
+  </si>
+  <si>
+    <t>DO FRIDAY/SATURDAY/SUNDAY ?</t>
+  </si>
+  <si>
+    <t>CHECK WITH ETHAN WHEN THIS CAN BE DONE</t>
+  </si>
+  <si>
+    <t>ASK ETHAN WHEN READY - FRIDAY/SATURDAY/SUNDAY?</t>
+  </si>
+  <si>
+    <t>- GUI stopped halfway through. 
+- need to check if completed mission and all data logged</t>
+  </si>
+  <si>
+    <t>- completed circuit no problem, but was getting windy…</t>
+  </si>
+  <si>
+    <t>- can't see data in terminal log? - OOPS caps lock was on. All OK
+- went stale? Lost connection? Was spinning in place near last half…. Got stuck doing last action (turning)</t>
+  </si>
+  <si>
+    <t>- west side of pond much less windy than right side today</t>
+  </si>
+  <si>
+    <t>POST PROCESS DATA FROM MONDAY TEST WITH ETHAN TO SEE IF THESE ARE DONE</t>
+  </si>
+  <si>
+    <t>- to send her home cuz lazy lol
+- lost connection to WiFi network as she went to south of pond</t>
+  </si>
+  <si>
+    <t>LOG_PEARL_SIMPLE_31_3_2021_____16_39_13</t>
+  </si>
+  <si>
+    <t>LOG_PEARL_WAYPOINT_31_3_2021_____16_26_50</t>
+  </si>
+  <si>
+    <t>LOG_PEARL_WAYPOINT_31_3_2021_____16_13_05</t>
+  </si>
+  <si>
+    <t>LOG_PEARL_WAYPOINT_31_3_2021_____16_04_11</t>
+  </si>
+  <si>
+    <t>LOG_PEARL_WAYPOINT_31_3_2021_____14_50_14</t>
+  </si>
+  <si>
+    <t>LOG_PEARL_WAYPOINT_31_3_2021_____15_03_50</t>
+  </si>
+  <si>
+    <t>LOG_PEARL_WAYPOINT_31_3_2021_____15_16_48</t>
+  </si>
+  <si>
+    <t>LOG_PEARL_WAYPOINT_31_3_2021_____15_30_19</t>
+  </si>
+  <si>
+    <t>LOG_PEARL_WAYPOINT_31_3_2021_____15_46_20</t>
+  </si>
+  <si>
+    <t>- trying star with new gains and lead ins 
+- track points not showing up? But checked in code
+- track points showe dup
+- she did really well!
+- going to west star point, it was slow because of current? Coming back was much faster
+- not quite complete?</t>
+  </si>
+  <si>
+    <t>- windier than this morning. Pretty steady breeze coming from the SE
+- not quite complete?</t>
+  </si>
+  <si>
+    <t>- not full pattern?</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -678,6 +782,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Helvetica"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="8">
@@ -736,7 +846,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -768,12 +878,8 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="2" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="18" fontId="2" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="18" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -800,6 +906,14 @@
     <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="18" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
+    <xf numFmtId="18" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1119,10 +1233,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C322D9A-DAA8-F94B-8299-5D36BBA36BB2}">
-  <dimension ref="A1:L81"/>
+  <dimension ref="A1:L90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="A76" sqref="A76"/>
+    <sheetView topLeftCell="D76" workbookViewId="0">
+      <selection activeCell="L87" sqref="L87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1171,7 +1285,7 @@
         <v>41</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>2</v>
@@ -2363,7 +2477,7 @@
         <v>9</v>
       </c>
       <c r="D36" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E36">
         <v>0.6</v>
@@ -2398,7 +2512,7 @@
         <v>9</v>
       </c>
       <c r="D37" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E37">
         <v>0.4</v>
@@ -2433,7 +2547,7 @@
         <v>9</v>
       </c>
       <c r="D38" s="20" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E38" s="20">
         <v>0.4</v>
@@ -2454,7 +2568,7 @@
         <v>0.5</v>
       </c>
       <c r="K38" s="20" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="L38" s="21" t="s">
         <v>86</v>
@@ -2471,7 +2585,7 @@
         <v>9</v>
       </c>
       <c r="D39" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E39">
         <v>0.4</v>
@@ -2492,7 +2606,7 @@
         <v>0.5</v>
       </c>
       <c r="K39" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="L39" s="6" t="s">
         <v>87</v>
@@ -2509,7 +2623,7 @@
         <v>9</v>
       </c>
       <c r="D40" s="20" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E40" s="20">
         <v>0.4</v>
@@ -2530,7 +2644,7 @@
         <v>0.5</v>
       </c>
       <c r="K40" s="20" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="L40" s="21" t="s">
         <v>88</v>
@@ -2547,7 +2661,7 @@
         <v>26</v>
       </c>
       <c r="D41" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E41">
         <v>0.4</v>
@@ -2568,48 +2682,48 @@
         <v>0.5</v>
       </c>
       <c r="K41" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="L41" s="4" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="42" spans="1:12" s="25" customFormat="1" ht="85" x14ac:dyDescent="0.2">
-      <c r="A42" s="22">
+    <row r="42" spans="1:12" s="36" customFormat="1" ht="102" x14ac:dyDescent="0.2">
+      <c r="A42" s="33">
         <v>44279</v>
       </c>
-      <c r="B42" s="23">
+      <c r="B42" s="47">
         <v>0.59930555555555554</v>
       </c>
-      <c r="C42" s="24" t="s">
+      <c r="C42" s="35" t="s">
         <v>26</v>
       </c>
-      <c r="D42" s="25" t="s">
-        <v>95</v>
-      </c>
-      <c r="E42" s="24">
-        <v>0.4</v>
-      </c>
-      <c r="F42" s="24">
-        <v>0.04</v>
-      </c>
-      <c r="G42" s="24">
-        <v>4</v>
-      </c>
-      <c r="H42" s="24">
-        <v>1</v>
-      </c>
-      <c r="I42" s="24">
-        <v>0</v>
-      </c>
-      <c r="J42" s="24">
-        <v>0.5</v>
-      </c>
-      <c r="K42" s="24" t="s">
-        <v>120</v>
-      </c>
-      <c r="L42" s="26" t="s">
-        <v>90</v>
+      <c r="D42" s="36" t="s">
+        <v>94</v>
+      </c>
+      <c r="E42" s="35">
+        <v>0.4</v>
+      </c>
+      <c r="F42" s="35">
+        <v>0.04</v>
+      </c>
+      <c r="G42" s="35">
+        <v>4</v>
+      </c>
+      <c r="H42" s="35">
+        <v>1</v>
+      </c>
+      <c r="I42" s="35">
+        <v>0</v>
+      </c>
+      <c r="J42" s="35">
+        <v>0.5</v>
+      </c>
+      <c r="K42" s="35" t="s">
+        <v>125</v>
+      </c>
+      <c r="L42" s="48" t="s">
+        <v>211</v>
       </c>
     </row>
     <row r="43" spans="1:12" ht="17" x14ac:dyDescent="0.2">
@@ -2623,7 +2737,7 @@
         <v>83</v>
       </c>
       <c r="D43" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E43" s="9">
         <v>0.4</v>
@@ -2644,10 +2758,10 @@
         <v>0.5</v>
       </c>
       <c r="K43" s="9" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="L43" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="44" spans="1:12" s="11" customFormat="1" ht="17" x14ac:dyDescent="0.2">
@@ -2661,7 +2775,7 @@
         <v>83</v>
       </c>
       <c r="D44" s="11" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E44" s="14">
         <v>0.4</v>
@@ -2682,10 +2796,10 @@
         <v>0.5</v>
       </c>
       <c r="K44" s="14" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="L44" s="12" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="45" spans="1:12" ht="34" x14ac:dyDescent="0.2">
@@ -2696,48 +2810,48 @@
         <v>0.56874999999999998</v>
       </c>
       <c r="C45" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="D45" t="s">
+        <v>110</v>
+      </c>
+      <c r="E45" s="9">
+        <v>0.4</v>
+      </c>
+      <c r="F45" s="9">
+        <v>0.04</v>
+      </c>
+      <c r="G45" s="9">
+        <v>4</v>
+      </c>
+      <c r="H45" s="9">
+        <v>1</v>
+      </c>
+      <c r="I45" s="9">
+        <v>0</v>
+      </c>
+      <c r="J45" s="9">
+        <v>0.5</v>
+      </c>
+      <c r="K45" s="9" t="s">
+        <v>120</v>
+      </c>
+      <c r="L45" s="4" t="s">
         <v>102</v>
-      </c>
-      <c r="D45" t="s">
-        <v>111</v>
-      </c>
-      <c r="E45" s="9">
-        <v>0.4</v>
-      </c>
-      <c r="F45" s="9">
-        <v>0.04</v>
-      </c>
-      <c r="G45" s="9">
-        <v>4</v>
-      </c>
-      <c r="H45" s="9">
-        <v>1</v>
-      </c>
-      <c r="I45" s="9">
-        <v>0</v>
-      </c>
-      <c r="J45" s="9">
-        <v>0.5</v>
-      </c>
-      <c r="K45" s="9" t="s">
-        <v>121</v>
-      </c>
-      <c r="L45" s="4" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="46" spans="1:12" s="17" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A46" s="15">
         <v>44280</v>
       </c>
-      <c r="B46" s="29">
+      <c r="B46" s="27">
         <v>0.57777777777777783</v>
       </c>
       <c r="C46" s="16" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D46" s="17" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E46" s="16">
         <v>0.4</v>
@@ -2758,10 +2872,10 @@
         <v>0.5</v>
       </c>
       <c r="K46" s="16" t="s">
-        <v>120</v>
-      </c>
-      <c r="L46" s="30" t="s">
-        <v>104</v>
+        <v>119</v>
+      </c>
+      <c r="L46" s="28" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="47" spans="1:12" ht="17" x14ac:dyDescent="0.2">
@@ -2772,10 +2886,10 @@
         <v>0.58680555555555558</v>
       </c>
       <c r="C47" s="9" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D47" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E47" s="9">
         <v>0.4</v>
@@ -2796,24 +2910,24 @@
         <v>0.5</v>
       </c>
       <c r="K47" s="9" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="L47" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="48" spans="1:12" s="17" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A48" s="15">
         <v>44280</v>
       </c>
-      <c r="B48" s="29">
+      <c r="B48" s="27">
         <v>0.58819444444444446</v>
       </c>
       <c r="C48" s="16" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D48" s="17" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E48" s="16">
         <v>0.4</v>
@@ -2834,48 +2948,48 @@
         <v>0.5</v>
       </c>
       <c r="K48" s="16" t="s">
-        <v>120</v>
-      </c>
-      <c r="L48" s="30" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="49" spans="1:12" s="25" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+        <v>119</v>
+      </c>
+      <c r="L48" s="28" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12" s="24" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A49" s="22">
         <v>44280</v>
       </c>
-      <c r="B49" s="27">
+      <c r="B49" s="25">
         <v>0.59583333333333333</v>
       </c>
-      <c r="C49" s="24" t="s">
+      <c r="C49" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="D49" s="25" t="s">
-        <v>115</v>
-      </c>
-      <c r="E49" s="24">
-        <v>0.4</v>
-      </c>
-      <c r="F49" s="24">
-        <v>0.04</v>
-      </c>
-      <c r="G49" s="24">
-        <v>4</v>
-      </c>
-      <c r="H49" s="24">
-        <v>1</v>
-      </c>
-      <c r="I49" s="24">
-        <v>0</v>
-      </c>
-      <c r="J49" s="24">
-        <v>0.5</v>
-      </c>
-      <c r="K49" s="24" t="s">
-        <v>120</v>
-      </c>
-      <c r="L49" s="28" t="s">
-        <v>107</v>
+      <c r="D49" s="24" t="s">
+        <v>114</v>
+      </c>
+      <c r="E49" s="23">
+        <v>0.4</v>
+      </c>
+      <c r="F49" s="23">
+        <v>0.04</v>
+      </c>
+      <c r="G49" s="23">
+        <v>4</v>
+      </c>
+      <c r="H49" s="23">
+        <v>1</v>
+      </c>
+      <c r="I49" s="23">
+        <v>0</v>
+      </c>
+      <c r="J49" s="23">
+        <v>0.5</v>
+      </c>
+      <c r="K49" s="23" t="s">
+        <v>119</v>
+      </c>
+      <c r="L49" s="26" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="50" spans="1:12" ht="34" x14ac:dyDescent="0.2">
@@ -2889,7 +3003,7 @@
         <v>26</v>
       </c>
       <c r="D50" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E50" s="9">
         <v>0.4</v>
@@ -2910,48 +3024,48 @@
         <v>0.5</v>
       </c>
       <c r="K50" s="9" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="L50" s="4" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="51" spans="1:12" s="25" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12" s="24" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A51" s="22">
         <v>44280</v>
       </c>
-      <c r="B51" s="27">
+      <c r="B51" s="25">
         <v>0.6069444444444444</v>
       </c>
-      <c r="C51" s="24" t="s">
+      <c r="C51" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="D51" s="25" t="s">
-        <v>117</v>
-      </c>
-      <c r="E51" s="24">
-        <v>0.4</v>
-      </c>
-      <c r="F51" s="24">
-        <v>0.04</v>
-      </c>
-      <c r="G51" s="24">
-        <v>4</v>
-      </c>
-      <c r="H51" s="24">
-        <v>1</v>
-      </c>
-      <c r="I51" s="24">
-        <v>0</v>
-      </c>
-      <c r="J51" s="24">
-        <v>0.5</v>
-      </c>
-      <c r="K51" s="24" t="s">
-        <v>120</v>
-      </c>
-      <c r="L51" s="28" t="s">
-        <v>108</v>
+      <c r="D51" s="24" t="s">
+        <v>116</v>
+      </c>
+      <c r="E51" s="23">
+        <v>0.4</v>
+      </c>
+      <c r="F51" s="23">
+        <v>0.04</v>
+      </c>
+      <c r="G51" s="23">
+        <v>4</v>
+      </c>
+      <c r="H51" s="23">
+        <v>1</v>
+      </c>
+      <c r="I51" s="23">
+        <v>0</v>
+      </c>
+      <c r="J51" s="23">
+        <v>0.5</v>
+      </c>
+      <c r="K51" s="23" t="s">
+        <v>119</v>
+      </c>
+      <c r="L51" s="26" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="52" spans="1:12" ht="17" x14ac:dyDescent="0.2">
@@ -2965,7 +3079,7 @@
         <v>6</v>
       </c>
       <c r="D52" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E52" s="9">
         <v>0.4</v>
@@ -2986,10 +3100,10 @@
         <v>0.5</v>
       </c>
       <c r="K52" s="9" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="L52" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="53" spans="1:12" x14ac:dyDescent="0.2">
@@ -3003,7 +3117,7 @@
         <v>9</v>
       </c>
       <c r="D53" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E53">
         <v>0.4</v>
@@ -3024,10 +3138,10 @@
         <v>0.5</v>
       </c>
       <c r="K53" t="s">
+        <v>120</v>
+      </c>
+      <c r="L53" s="6" t="s">
         <v>121</v>
-      </c>
-      <c r="L53" s="6" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="54" spans="1:12" s="20" customFormat="1" x14ac:dyDescent="0.2">
@@ -3041,7 +3155,7 @@
         <v>9</v>
       </c>
       <c r="D54" s="20" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="E54" s="20">
         <v>0.4</v>
@@ -3062,7 +3176,7 @@
         <v>0.5</v>
       </c>
       <c r="K54" s="20" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="55" spans="1:12" ht="34" x14ac:dyDescent="0.2">
@@ -3076,7 +3190,7 @@
         <v>9</v>
       </c>
       <c r="D55" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="E55">
         <v>0.4</v>
@@ -3097,10 +3211,10 @@
         <v>0.5</v>
       </c>
       <c r="K55" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="L55" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="56" spans="1:12" ht="68" x14ac:dyDescent="0.2">
@@ -3114,7 +3228,7 @@
         <v>9</v>
       </c>
       <c r="D56" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="E56">
         <v>0.4</v>
@@ -3135,10 +3249,10 @@
         <v>0.5</v>
       </c>
       <c r="K56" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="L56" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="57" spans="1:12" ht="17" x14ac:dyDescent="0.2">
@@ -3152,7 +3266,7 @@
         <v>9</v>
       </c>
       <c r="D57" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="E57">
         <v>0.4</v>
@@ -3173,10 +3287,10 @@
         <v>0.5</v>
       </c>
       <c r="K57" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="L57" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="58" spans="1:12" s="20" customFormat="1" x14ac:dyDescent="0.2">
@@ -3190,7 +3304,7 @@
         <v>9</v>
       </c>
       <c r="D58" s="20" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="E58" s="20">
         <v>0.4</v>
@@ -3211,7 +3325,7 @@
         <v>0.5</v>
       </c>
       <c r="K58" s="20" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="59" spans="1:12" s="20" customFormat="1" x14ac:dyDescent="0.2">
@@ -3225,7 +3339,7 @@
         <v>9</v>
       </c>
       <c r="D59" s="20" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="E59" s="20">
         <v>0.4</v>
@@ -3246,7 +3360,7 @@
         <v>0.5</v>
       </c>
       <c r="K59" s="20" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="60" spans="1:12" s="20" customFormat="1" x14ac:dyDescent="0.2">
@@ -3260,7 +3374,7 @@
         <v>9</v>
       </c>
       <c r="D60" s="20" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="E60" s="20">
         <v>0.4</v>
@@ -3281,7 +3395,7 @@
         <v>0.5</v>
       </c>
       <c r="K60" s="20" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="61" spans="1:12" s="20" customFormat="1" x14ac:dyDescent="0.2">
@@ -3295,7 +3409,7 @@
         <v>9</v>
       </c>
       <c r="D61" s="20" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="E61" s="20">
         <v>0.4</v>
@@ -3316,45 +3430,45 @@
         <v>0.5</v>
       </c>
       <c r="K61" s="20" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="62" spans="1:12" s="33" customFormat="1" ht="85" x14ac:dyDescent="0.2">
-      <c r="A62" s="31">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="62" spans="1:12" s="31" customFormat="1" ht="85" x14ac:dyDescent="0.2">
+      <c r="A62" s="29">
         <v>44282</v>
       </c>
-      <c r="B62" s="32">
-        <v>0.5</v>
-      </c>
-      <c r="C62" s="33" t="s">
+      <c r="B62" s="30">
+        <v>0.5</v>
+      </c>
+      <c r="C62" s="31" t="s">
+        <v>126</v>
+      </c>
+      <c r="D62" s="31" t="s">
+        <v>145</v>
+      </c>
+      <c r="E62" s="31">
+        <v>0.4</v>
+      </c>
+      <c r="F62" s="31">
+        <v>0.04</v>
+      </c>
+      <c r="G62" s="31">
+        <v>4</v>
+      </c>
+      <c r="H62" s="31">
+        <v>1</v>
+      </c>
+      <c r="I62" s="31">
+        <v>0</v>
+      </c>
+      <c r="J62" s="31">
+        <v>0.5</v>
+      </c>
+      <c r="K62" s="31" t="s">
+        <v>119</v>
+      </c>
+      <c r="L62" s="32" t="s">
         <v>127</v>
-      </c>
-      <c r="D62" s="33" t="s">
-        <v>147</v>
-      </c>
-      <c r="E62" s="33">
-        <v>0.4</v>
-      </c>
-      <c r="F62" s="33">
-        <v>0.04</v>
-      </c>
-      <c r="G62" s="33">
-        <v>4</v>
-      </c>
-      <c r="H62" s="33">
-        <v>1</v>
-      </c>
-      <c r="I62" s="33">
-        <v>0</v>
-      </c>
-      <c r="J62" s="33">
-        <v>0.5</v>
-      </c>
-      <c r="K62" s="33" t="s">
-        <v>120</v>
-      </c>
-      <c r="L62" s="34" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="63" spans="1:12" ht="68" x14ac:dyDescent="0.2">
@@ -3365,10 +3479,10 @@
         <v>0.50416666666666665</v>
       </c>
       <c r="C63" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D63" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="E63">
         <v>0.4</v>
@@ -3389,7 +3503,7 @@
         <v>0.5</v>
       </c>
       <c r="L63" s="4" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="64" spans="1:12" ht="51" x14ac:dyDescent="0.2">
@@ -3400,10 +3514,10 @@
         <v>0.50902777777777775</v>
       </c>
       <c r="C64" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D64" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="E64">
         <v>0.4</v>
@@ -3424,235 +3538,235 @@
         <v>0.5</v>
       </c>
       <c r="L64" s="4" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="65" spans="1:12" s="31" customFormat="1" ht="85" x14ac:dyDescent="0.2">
+      <c r="A65" s="29">
+        <v>44282</v>
+      </c>
+      <c r="B65" s="30">
+        <v>0.51180555555555551</v>
+      </c>
+      <c r="C65" s="31" t="s">
+        <v>126</v>
+      </c>
+      <c r="D65" s="31" t="s">
+        <v>142</v>
+      </c>
+      <c r="E65" s="31">
+        <v>0.4</v>
+      </c>
+      <c r="F65" s="31">
+        <v>0.04</v>
+      </c>
+      <c r="G65" s="31">
+        <v>4</v>
+      </c>
+      <c r="H65" s="31">
+        <v>1</v>
+      </c>
+      <c r="I65" s="31">
+        <v>0</v>
+      </c>
+      <c r="J65" s="31">
+        <v>0.5</v>
+      </c>
+      <c r="K65" s="31" t="s">
+        <v>119</v>
+      </c>
+      <c r="L65" s="32" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="65" spans="1:12" s="33" customFormat="1" ht="85" x14ac:dyDescent="0.2">
-      <c r="A65" s="31">
-        <v>44282</v>
-      </c>
-      <c r="B65" s="32">
-        <v>0.51180555555555551</v>
-      </c>
-      <c r="C65" s="33" t="s">
-        <v>127</v>
-      </c>
-      <c r="D65" s="33" t="s">
-        <v>144</v>
-      </c>
-      <c r="E65" s="33">
-        <v>0.4</v>
-      </c>
-      <c r="F65" s="33">
-        <v>0.04</v>
-      </c>
-      <c r="G65" s="33">
-        <v>4</v>
-      </c>
-      <c r="H65" s="33">
-        <v>1</v>
-      </c>
-      <c r="I65" s="33">
-        <v>0</v>
-      </c>
-      <c r="J65" s="33">
-        <v>0.5</v>
-      </c>
-      <c r="K65" s="33" t="s">
+    <row r="66" spans="1:12" s="36" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A66" s="33">
+        <v>44280</v>
+      </c>
+      <c r="B66" s="34">
+        <v>0.59791666666666665</v>
+      </c>
+      <c r="C66" s="35" t="s">
+        <v>26</v>
+      </c>
+      <c r="D66" s="36" t="s">
+        <v>141</v>
+      </c>
+      <c r="E66" s="35">
+        <v>0.4</v>
+      </c>
+      <c r="F66" s="35">
+        <v>0.04</v>
+      </c>
+      <c r="G66" s="35">
+        <v>4</v>
+      </c>
+      <c r="H66" s="35">
+        <v>1</v>
+      </c>
+      <c r="I66" s="35">
+        <v>0</v>
+      </c>
+      <c r="J66" s="35">
+        <v>0.5</v>
+      </c>
+      <c r="K66" s="35" t="s">
         <v>120</v>
       </c>
-      <c r="L65" s="34" t="s">
+      <c r="L66" s="37" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="66" spans="1:12" s="38" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A66" s="35">
+    <row r="67" spans="1:12" s="36" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A67" s="33">
         <v>44280</v>
       </c>
-      <c r="B66" s="36">
-        <v>0.59791666666666665</v>
-      </c>
-      <c r="C66" s="37" t="s">
+      <c r="B67" s="34">
+        <v>0.60069444444444442</v>
+      </c>
+      <c r="C67" s="35" t="s">
         <v>26</v>
       </c>
-      <c r="D66" s="38" t="s">
-        <v>143</v>
-      </c>
-      <c r="E66" s="37">
-        <v>0.4</v>
-      </c>
-      <c r="F66" s="37">
-        <v>0.04</v>
-      </c>
-      <c r="G66" s="37">
-        <v>4</v>
-      </c>
-      <c r="H66" s="37">
-        <v>1</v>
-      </c>
-      <c r="I66" s="37">
-        <v>0</v>
-      </c>
-      <c r="J66" s="37">
-        <v>0.5</v>
-      </c>
-      <c r="K66" s="37" t="s">
-        <v>121</v>
-      </c>
-      <c r="L66" s="39" t="s">
+      <c r="D67" s="36" t="s">
+        <v>140</v>
+      </c>
+      <c r="E67" s="35">
+        <v>0.4</v>
+      </c>
+      <c r="F67" s="35">
+        <v>0.04</v>
+      </c>
+      <c r="G67" s="35">
+        <v>4</v>
+      </c>
+      <c r="H67" s="35">
+        <v>1</v>
+      </c>
+      <c r="I67" s="35">
+        <v>0</v>
+      </c>
+      <c r="J67" s="35">
+        <v>0.5</v>
+      </c>
+      <c r="K67" s="35" t="s">
+        <v>120</v>
+      </c>
+      <c r="L67" s="37" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="67" spans="1:12" s="38" customFormat="1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A67" s="35">
+    <row r="68" spans="1:12" s="36" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A68" s="33">
         <v>44280</v>
       </c>
-      <c r="B67" s="36">
-        <v>0.60069444444444442</v>
-      </c>
-      <c r="C67" s="37" t="s">
+      <c r="B68" s="34">
+        <v>0.60277777777777775</v>
+      </c>
+      <c r="C68" s="35" t="s">
         <v>26</v>
       </c>
-      <c r="D67" s="38" t="s">
-        <v>142</v>
-      </c>
-      <c r="E67" s="37">
-        <v>0.4</v>
-      </c>
-      <c r="F67" s="37">
-        <v>0.04</v>
-      </c>
-      <c r="G67" s="37">
-        <v>4</v>
-      </c>
-      <c r="H67" s="37">
-        <v>1</v>
-      </c>
-      <c r="I67" s="37">
-        <v>0</v>
-      </c>
-      <c r="J67" s="37">
-        <v>0.5</v>
-      </c>
-      <c r="K67" s="37" t="s">
-        <v>121</v>
-      </c>
-      <c r="L67" s="39" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="68" spans="1:12" s="25" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A68" s="22">
-        <v>44280</v>
-      </c>
-      <c r="B68" s="27">
-        <v>0.60277777777777775</v>
-      </c>
-      <c r="C68" s="24" t="s">
-        <v>26</v>
-      </c>
-      <c r="D68" s="25" t="s">
-        <v>141</v>
-      </c>
-      <c r="E68" s="24">
-        <v>0.4</v>
-      </c>
-      <c r="F68" s="24">
-        <v>0.04</v>
-      </c>
-      <c r="G68" s="24">
-        <v>4</v>
-      </c>
-      <c r="H68" s="24">
-        <v>1</v>
-      </c>
-      <c r="I68" s="24">
-        <v>0</v>
-      </c>
-      <c r="J68" s="24">
-        <v>0.5</v>
-      </c>
-      <c r="K68" s="24" t="s">
-        <v>120</v>
-      </c>
-      <c r="L68" s="28" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="69" spans="1:12" s="25" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="D68" s="36" t="s">
+        <v>139</v>
+      </c>
+      <c r="E68" s="35">
+        <v>0.4</v>
+      </c>
+      <c r="F68" s="35">
+        <v>0.04</v>
+      </c>
+      <c r="G68" s="35">
+        <v>4</v>
+      </c>
+      <c r="H68" s="35">
+        <v>1</v>
+      </c>
+      <c r="I68" s="35">
+        <v>0</v>
+      </c>
+      <c r="J68" s="35">
+        <v>0.5</v>
+      </c>
+      <c r="K68" s="35" t="s">
+        <v>125</v>
+      </c>
+      <c r="L68" s="37" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="69" spans="1:12" s="24" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A69" s="22">
         <v>44280</v>
       </c>
-      <c r="B69" s="27">
+      <c r="B69" s="25">
         <v>0.6118055555555556</v>
       </c>
-      <c r="C69" s="24" t="s">
+      <c r="C69" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="D69" s="25" t="s">
-        <v>140</v>
-      </c>
-      <c r="E69" s="24">
-        <v>0.4</v>
-      </c>
-      <c r="F69" s="24">
-        <v>0.04</v>
-      </c>
-      <c r="G69" s="24">
-        <v>4</v>
-      </c>
-      <c r="H69" s="24">
-        <v>1</v>
-      </c>
-      <c r="I69" s="24">
-        <v>0</v>
-      </c>
-      <c r="J69" s="24">
-        <v>0.5</v>
-      </c>
-      <c r="K69" s="24" t="s">
-        <v>120</v>
-      </c>
-      <c r="L69" s="28" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="70" spans="1:12" s="25" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="D69" s="24" t="s">
+        <v>138</v>
+      </c>
+      <c r="E69" s="23">
+        <v>0.4</v>
+      </c>
+      <c r="F69" s="23">
+        <v>0.04</v>
+      </c>
+      <c r="G69" s="23">
+        <v>4</v>
+      </c>
+      <c r="H69" s="23">
+        <v>1</v>
+      </c>
+      <c r="I69" s="23">
+        <v>0</v>
+      </c>
+      <c r="J69" s="23">
+        <v>0.5</v>
+      </c>
+      <c r="K69" s="23" t="s">
+        <v>119</v>
+      </c>
+      <c r="L69" s="26" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="70" spans="1:12" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A70" s="22">
         <v>44280</v>
       </c>
-      <c r="B70" s="27">
+      <c r="B70" s="25">
         <v>0.62013888888888891</v>
       </c>
-      <c r="C70" s="24" t="s">
+      <c r="C70" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="D70" s="25" t="s">
-        <v>139</v>
-      </c>
-      <c r="E70" s="24">
-        <v>0.4</v>
-      </c>
-      <c r="F70" s="24">
-        <v>0.04</v>
-      </c>
-      <c r="G70" s="24">
-        <v>4</v>
-      </c>
-      <c r="H70" s="24">
-        <v>1</v>
-      </c>
-      <c r="I70" s="24">
-        <v>0</v>
-      </c>
-      <c r="J70" s="24">
-        <v>0.5</v>
-      </c>
-      <c r="K70" s="24" t="s">
-        <v>120</v>
-      </c>
-      <c r="L70" s="40" t="s">
-        <v>136</v>
+      <c r="D70" s="24" t="s">
+        <v>137</v>
+      </c>
+      <c r="E70" s="23">
+        <v>0.4</v>
+      </c>
+      <c r="F70" s="23">
+        <v>0.04</v>
+      </c>
+      <c r="G70" s="23">
+        <v>4</v>
+      </c>
+      <c r="H70" s="23">
+        <v>1</v>
+      </c>
+      <c r="I70" s="23">
+        <v>0</v>
+      </c>
+      <c r="J70" s="23">
+        <v>0.5</v>
+      </c>
+      <c r="K70" s="23" t="s">
+        <v>119</v>
+      </c>
+      <c r="L70" s="38" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="71" spans="1:12" ht="17" x14ac:dyDescent="0.2">
@@ -3666,7 +3780,7 @@
         <v>6</v>
       </c>
       <c r="D71" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="E71" s="9">
         <v>0.4</v>
@@ -3687,10 +3801,10 @@
         <v>0.5</v>
       </c>
       <c r="K71" s="9" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="L71" s="4" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="72" spans="1:12" ht="34" x14ac:dyDescent="0.2">
@@ -3700,11 +3814,11 @@
       <c r="B72" s="3">
         <v>0.62083333333333335</v>
       </c>
-      <c r="C72" s="37" t="s">
+      <c r="C72" s="35" t="s">
         <v>13</v>
       </c>
       <c r="D72" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="E72" s="9">
         <v>0.4</v>
@@ -3725,7 +3839,7 @@
         <v>0.5</v>
       </c>
       <c r="L72" s="4" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="73" spans="1:12" ht="51" x14ac:dyDescent="0.2">
@@ -3735,11 +3849,11 @@
       <c r="B73" s="3">
         <v>0.64583333333333337</v>
       </c>
-      <c r="C73" s="37" t="s">
+      <c r="C73" s="35" t="s">
         <v>13</v>
       </c>
       <c r="D73" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="E73" s="9">
         <v>0.4</v>
@@ -3760,7 +3874,7 @@
         <v>0.5</v>
       </c>
       <c r="L73" s="4" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="74" spans="1:12" ht="51" x14ac:dyDescent="0.2">
@@ -3770,32 +3884,32 @@
       <c r="B74" s="3">
         <v>0.67361111111111116</v>
       </c>
-      <c r="C74" s="37" t="s">
+      <c r="C74" s="35" t="s">
+        <v>176</v>
+      </c>
+      <c r="D74" t="s">
+        <v>156</v>
+      </c>
+      <c r="E74" s="9">
+        <v>0.4</v>
+      </c>
+      <c r="F74" s="9">
+        <v>0.04</v>
+      </c>
+      <c r="G74" s="9">
+        <v>4</v>
+      </c>
+      <c r="H74" s="9">
+        <v>1</v>
+      </c>
+      <c r="I74" s="9">
+        <v>0</v>
+      </c>
+      <c r="J74" s="9">
+        <v>0.5</v>
+      </c>
+      <c r="L74" s="4" t="s">
         <v>178</v>
-      </c>
-      <c r="D74" t="s">
-        <v>158</v>
-      </c>
-      <c r="E74" s="9">
-        <v>0.4</v>
-      </c>
-      <c r="F74" s="9">
-        <v>0.04</v>
-      </c>
-      <c r="G74" s="9">
-        <v>4</v>
-      </c>
-      <c r="H74" s="9">
-        <v>1</v>
-      </c>
-      <c r="I74" s="9">
-        <v>0</v>
-      </c>
-      <c r="J74" s="9">
-        <v>0.5</v>
-      </c>
-      <c r="L74" s="4" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="75" spans="1:12" ht="51" x14ac:dyDescent="0.2">
@@ -3805,11 +3919,11 @@
       <c r="B75" s="3">
         <v>0.6777777777777777</v>
       </c>
-      <c r="C75" s="37" t="s">
-        <v>178</v>
+      <c r="C75" s="35" t="s">
+        <v>176</v>
       </c>
       <c r="D75" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="E75" s="9">
         <v>0.4</v>
@@ -3830,7 +3944,7 @@
         <v>0.5</v>
       </c>
       <c r="L75" s="4" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="76" spans="1:12" ht="51" x14ac:dyDescent="0.2">
@@ -3844,7 +3958,7 @@
         <v>83</v>
       </c>
       <c r="D76" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="E76" s="9">
         <v>0.4</v>
@@ -3865,14 +3979,14 @@
         <v>0.5</v>
       </c>
       <c r="K76" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="L76" s="4" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="77" spans="1:12" s="11" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A77" s="41">
+      <c r="A77" s="39">
         <v>44285</v>
       </c>
       <c r="B77" s="10">
@@ -3882,7 +3996,7 @@
         <v>83</v>
       </c>
       <c r="D77" s="11" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="E77" s="14">
         <v>0.4</v>
@@ -3903,14 +4017,14 @@
         <v>0.5</v>
       </c>
       <c r="K77" s="11" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="L77" s="12" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="78" spans="1:12" s="11" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A78" s="41">
+      <c r="A78" s="39">
         <v>44285</v>
       </c>
       <c r="B78" s="10">
@@ -3920,7 +4034,7 @@
         <v>83</v>
       </c>
       <c r="D78" s="11" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="E78" s="14">
         <v>0.4</v>
@@ -3941,52 +4055,52 @@
         <v>0.5</v>
       </c>
       <c r="K78" s="11" t="s">
+        <v>119</v>
+      </c>
+      <c r="L78" s="12" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="79" spans="1:12" s="36" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A79" s="41">
+        <v>44285</v>
+      </c>
+      <c r="B79" s="34">
+        <v>0.66597222222222219</v>
+      </c>
+      <c r="C79" s="35" t="s">
+        <v>83</v>
+      </c>
+      <c r="D79" s="36" t="s">
+        <v>169</v>
+      </c>
+      <c r="E79" s="35">
+        <v>0.4</v>
+      </c>
+      <c r="F79" s="35">
+        <v>0.04</v>
+      </c>
+      <c r="G79" s="35">
+        <v>4</v>
+      </c>
+      <c r="H79" s="35">
+        <v>1</v>
+      </c>
+      <c r="I79" s="35">
+        <v>0</v>
+      </c>
+      <c r="J79" s="35">
+        <v>0.5</v>
+      </c>
+      <c r="K79" s="36" t="s">
         <v>120</v>
       </c>
-      <c r="L78" s="12" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="79" spans="1:12" s="38" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A79" s="43">
-        <v>44285</v>
-      </c>
-      <c r="B79" s="36">
-        <v>0.66597222222222219</v>
-      </c>
-      <c r="C79" s="37" t="s">
-        <v>83</v>
-      </c>
-      <c r="D79" s="38" t="s">
-        <v>171</v>
-      </c>
-      <c r="E79" s="37">
-        <v>0.4</v>
-      </c>
-      <c r="F79" s="37">
-        <v>0.04</v>
-      </c>
-      <c r="G79" s="37">
-        <v>4</v>
-      </c>
-      <c r="H79" s="37">
-        <v>1</v>
-      </c>
-      <c r="I79" s="37">
-        <v>0</v>
-      </c>
-      <c r="J79" s="37">
-        <v>0.5</v>
-      </c>
-      <c r="K79" s="38" t="s">
-        <v>121</v>
-      </c>
-      <c r="L79" s="44" t="s">
-        <v>176</v>
+      <c r="L79" s="42" t="s">
+        <v>174</v>
       </c>
     </row>
     <row r="80" spans="1:12" s="11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A80" s="41">
+      <c r="A80" s="39">
         <v>44285</v>
       </c>
       <c r="B80" s="10">
@@ -3996,7 +4110,7 @@
         <v>83</v>
       </c>
       <c r="D80" s="11" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="E80" s="14">
         <v>0.4</v>
@@ -4017,11 +4131,11 @@
         <v>0.5</v>
       </c>
       <c r="K80" s="11" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="81" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A81" s="41">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="81" spans="1:12" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A81" s="39">
         <v>44285</v>
       </c>
       <c r="B81" s="10">
@@ -4031,7 +4145,7 @@
         <v>83</v>
       </c>
       <c r="D81" s="11" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="E81" s="14">
         <v>0.4</v>
@@ -4052,7 +4166,346 @@
         <v>0.5</v>
       </c>
       <c r="K81" s="11" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="82" spans="1:12" s="11" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+      <c r="A82" s="39">
+        <v>44286</v>
+      </c>
+      <c r="B82" s="10">
+        <v>0.61805555555555558</v>
+      </c>
+      <c r="C82" s="14" t="s">
+        <v>83</v>
+      </c>
+      <c r="D82" s="11" t="s">
+        <v>206</v>
+      </c>
+      <c r="E82" s="14">
+        <v>0.4</v>
+      </c>
+      <c r="F82" s="14">
+        <v>0.04</v>
+      </c>
+      <c r="G82" s="14">
+        <v>4</v>
+      </c>
+      <c r="H82" s="14">
+        <v>1</v>
+      </c>
+      <c r="I82" s="14">
+        <v>0</v>
+      </c>
+      <c r="J82" s="14">
+        <v>0.5</v>
+      </c>
+      <c r="K82" s="11" t="s">
+        <v>119</v>
+      </c>
+      <c r="L82" s="12" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="83" spans="1:12" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A83" s="39">
+        <v>44286</v>
+      </c>
+      <c r="B83" s="10">
+        <v>0.62708333333333333</v>
+      </c>
+      <c r="C83" s="14" t="s">
+        <v>83</v>
+      </c>
+      <c r="D83" s="11" t="s">
+        <v>207</v>
+      </c>
+      <c r="E83" s="14">
+        <v>0.4</v>
+      </c>
+      <c r="F83" s="14">
+        <v>0.04</v>
+      </c>
+      <c r="G83" s="14">
+        <v>4</v>
+      </c>
+      <c r="H83" s="14">
+        <v>1</v>
+      </c>
+      <c r="I83" s="14">
+        <v>0</v>
+      </c>
+      <c r="J83" s="14">
+        <v>0.5</v>
+      </c>
+      <c r="K83" s="11" t="s">
+        <v>119</v>
+      </c>
+      <c r="L83" s="43" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="84" spans="1:12" s="11" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A84" s="39">
+        <v>44286</v>
+      </c>
+      <c r="B84" s="10">
+        <v>0.63611111111111118</v>
+      </c>
+      <c r="C84" s="14" t="s">
+        <v>83</v>
+      </c>
+      <c r="D84" s="11" t="s">
+        <v>208</v>
+      </c>
+      <c r="E84" s="14">
+        <v>0.4</v>
+      </c>
+      <c r="F84" s="14">
+        <v>0.04</v>
+      </c>
+      <c r="G84" s="14">
+        <v>4</v>
+      </c>
+      <c r="H84" s="14">
+        <v>1</v>
+      </c>
+      <c r="I84" s="14">
+        <v>0</v>
+      </c>
+      <c r="J84" s="14">
+        <v>0.5</v>
+      </c>
+      <c r="K84" s="11" t="s">
+        <v>119</v>
+      </c>
+      <c r="L84" s="12" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="85" spans="1:12" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A85" s="39">
+        <v>44286</v>
+      </c>
+      <c r="B85" s="10">
+        <v>0.64583333333333337</v>
+      </c>
+      <c r="C85" s="14" t="s">
+        <v>83</v>
+      </c>
+      <c r="D85" s="11" t="s">
+        <v>209</v>
+      </c>
+      <c r="E85" s="14">
+        <v>0.4</v>
+      </c>
+      <c r="F85" s="14">
+        <v>0.04</v>
+      </c>
+      <c r="G85" s="14">
+        <v>4</v>
+      </c>
+      <c r="H85" s="14">
+        <v>1</v>
+      </c>
+      <c r="I85" s="14">
+        <v>0</v>
+      </c>
+      <c r="J85" s="14">
+        <v>0.5</v>
+      </c>
+      <c r="K85" s="11" t="s">
+        <v>119</v>
+      </c>
+      <c r="L85" s="43" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="86" spans="1:12" s="36" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A86" s="41">
+        <v>44286</v>
+      </c>
+      <c r="B86" s="34">
+        <v>0.65625</v>
+      </c>
+      <c r="C86" s="35" t="s">
+        <v>26</v>
+      </c>
+      <c r="D86" s="36" t="s">
+        <v>210</v>
+      </c>
+      <c r="E86" s="35">
+        <v>0.4</v>
+      </c>
+      <c r="F86" s="35">
+        <v>0.04</v>
+      </c>
+      <c r="G86" s="35">
+        <v>4</v>
+      </c>
+      <c r="H86" s="35">
+        <v>1</v>
+      </c>
+      <c r="I86" s="35">
+        <v>0</v>
+      </c>
+      <c r="J86" s="35">
+        <v>0.5</v>
+      </c>
+      <c r="K86" s="36" t="s">
+        <v>125</v>
+      </c>
+      <c r="L86" s="42" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="87" spans="1:12" ht="51" x14ac:dyDescent="0.2">
+      <c r="A87" s="5">
+        <v>44286</v>
+      </c>
+      <c r="B87" s="3">
+        <v>0.6694444444444444</v>
+      </c>
+      <c r="C87" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="D87" t="s">
+        <v>205</v>
+      </c>
+      <c r="E87" s="35">
+        <v>0.4</v>
+      </c>
+      <c r="F87" s="35">
+        <v>0.04</v>
+      </c>
+      <c r="G87" s="35">
+        <v>4</v>
+      </c>
+      <c r="H87" s="35">
+        <v>1</v>
+      </c>
+      <c r="I87" s="35">
+        <v>0</v>
+      </c>
+      <c r="J87" s="35">
+        <v>0.5</v>
+      </c>
+      <c r="K87" s="36" t="s">
         <v>120</v>
+      </c>
+      <c r="L87" s="4" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="88" spans="1:12" s="17" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A88" s="15">
+        <v>44286</v>
+      </c>
+      <c r="B88" s="45">
+        <v>0.67569444444444438</v>
+      </c>
+      <c r="C88" s="16" t="s">
+        <v>101</v>
+      </c>
+      <c r="D88" s="16" t="s">
+        <v>204</v>
+      </c>
+      <c r="E88" s="16">
+        <v>0.4</v>
+      </c>
+      <c r="F88" s="16">
+        <v>0.04</v>
+      </c>
+      <c r="G88" s="16">
+        <v>4</v>
+      </c>
+      <c r="H88" s="16">
+        <v>1</v>
+      </c>
+      <c r="I88" s="16">
+        <v>0</v>
+      </c>
+      <c r="J88" s="16">
+        <v>0.5</v>
+      </c>
+      <c r="K88" s="17" t="s">
+        <v>119</v>
+      </c>
+      <c r="L88" s="46" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="89" spans="1:12" s="17" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A89" s="15">
+        <v>44286</v>
+      </c>
+      <c r="B89" s="45">
+        <v>0.68472222222222223</v>
+      </c>
+      <c r="C89" s="16" t="s">
+        <v>101</v>
+      </c>
+      <c r="D89" s="16" t="s">
+        <v>203</v>
+      </c>
+      <c r="E89" s="16">
+        <v>0.4</v>
+      </c>
+      <c r="F89" s="16">
+        <v>0.04</v>
+      </c>
+      <c r="G89" s="16">
+        <v>4</v>
+      </c>
+      <c r="H89" s="16">
+        <v>1</v>
+      </c>
+      <c r="I89" s="16">
+        <v>0</v>
+      </c>
+      <c r="J89" s="16">
+        <v>0.5</v>
+      </c>
+      <c r="K89" s="17" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="90" spans="1:12" ht="34" x14ac:dyDescent="0.2">
+      <c r="A90" s="5">
+        <v>44286</v>
+      </c>
+      <c r="B90" s="3">
+        <v>0.69374999999999998</v>
+      </c>
+      <c r="C90" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D90" t="s">
+        <v>202</v>
+      </c>
+      <c r="E90" s="9">
+        <v>0.4</v>
+      </c>
+      <c r="F90" s="9">
+        <v>0.04</v>
+      </c>
+      <c r="G90" s="9">
+        <v>4</v>
+      </c>
+      <c r="H90" s="9">
+        <v>1</v>
+      </c>
+      <c r="I90" s="9">
+        <v>0</v>
+      </c>
+      <c r="J90" s="9">
+        <v>0.5</v>
+      </c>
+      <c r="K90" s="9" t="s">
+        <v>120</v>
+      </c>
+      <c r="L90" s="4" t="s">
+        <v>201</v>
       </c>
     </row>
   </sheetData>
@@ -4063,10 +4516,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A800C2D-7086-3649-85CB-0A56FEC6D735}">
-  <dimension ref="A1:C29"/>
+  <dimension ref="A1:C30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4078,13 +4531,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>165</v>
-      </c>
       <c r="C1" s="1" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="2" spans="1:3" s="20" customFormat="1" x14ac:dyDescent="0.2">
@@ -4095,7 +4548,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="20" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="3" spans="1:3" s="20" customFormat="1" x14ac:dyDescent="0.2">
@@ -4106,7 +4559,7 @@
         <v>2</v>
       </c>
       <c r="C3" s="20" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="4" spans="1:3" s="20" customFormat="1" x14ac:dyDescent="0.2">
@@ -4117,7 +4570,7 @@
         <v>3</v>
       </c>
       <c r="C4" s="20" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="5" spans="1:3" s="20" customFormat="1" x14ac:dyDescent="0.2">
@@ -4128,7 +4581,7 @@
         <v>4</v>
       </c>
       <c r="C5" s="20" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="6" spans="1:3" s="20" customFormat="1" x14ac:dyDescent="0.2">
@@ -4139,7 +4592,7 @@
         <v>5</v>
       </c>
       <c r="C6" s="20" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="7" spans="1:3" s="20" customFormat="1" x14ac:dyDescent="0.2">
@@ -4150,7 +4603,7 @@
         <v>6</v>
       </c>
       <c r="C7" s="20" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="8" spans="1:3" s="20" customFormat="1" x14ac:dyDescent="0.2">
@@ -4161,124 +4614,124 @@
         <v>7</v>
       </c>
       <c r="C8" s="20" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" s="25" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="25" t="s">
-        <v>166</v>
-      </c>
-      <c r="B9" s="25">
-        <v>1</v>
-      </c>
-      <c r="C9" s="25" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" s="25" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="25" t="s">
-        <v>166</v>
-      </c>
-      <c r="B10" s="25">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="24" t="s">
+        <v>164</v>
+      </c>
+      <c r="B9" s="24">
+        <v>1</v>
+      </c>
+      <c r="C9" s="24" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="24" t="s">
+        <v>164</v>
+      </c>
+      <c r="B10" s="24">
         <v>2</v>
       </c>
-      <c r="C10" s="25" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" s="25" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="25" t="s">
-        <v>166</v>
-      </c>
-      <c r="B11" s="25">
+      <c r="C10" s="24" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="24" t="s">
+        <v>164</v>
+      </c>
+      <c r="B11" s="24">
         <v>3</v>
       </c>
-      <c r="C11" s="25" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" s="25" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="25" t="s">
-        <v>166</v>
-      </c>
-      <c r="B12" s="25">
-        <v>4</v>
-      </c>
-      <c r="C12" s="25" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" s="25" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="25" t="s">
-        <v>166</v>
-      </c>
-      <c r="B13" s="25">
+      <c r="C11" s="24" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="24" t="s">
+        <v>164</v>
+      </c>
+      <c r="B12" s="24">
+        <v>4</v>
+      </c>
+      <c r="C12" s="24" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" s="36" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="36" t="s">
+        <v>164</v>
+      </c>
+      <c r="B13" s="36">
         <v>5</v>
       </c>
-      <c r="C13" s="25" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" s="25" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="25" t="s">
-        <v>166</v>
-      </c>
-      <c r="B14" s="25">
+    </row>
+    <row r="14" spans="1:3" s="36" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="36" t="s">
+        <v>164</v>
+      </c>
+      <c r="B14" s="36">
         <v>6</v>
       </c>
-      <c r="C14" s="25" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>166</v>
-      </c>
-      <c r="B15">
+    </row>
+    <row r="15" spans="1:3" s="36" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="36" t="s">
+        <v>164</v>
+      </c>
+      <c r="B15" s="36">
         <v>7</v>
       </c>
     </row>
     <row r="16" spans="1:3" s="17" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="17" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B16" s="17">
         <v>1</v>
       </c>
       <c r="C16" s="17" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="17" spans="1:3" s="17" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="17" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B17" s="17">
         <v>2</v>
       </c>
       <c r="C17" s="17" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>167</v>
-      </c>
-      <c r="B18">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" s="17" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="17" t="s">
+        <v>165</v>
+      </c>
+      <c r="B18" s="17">
         <v>3</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>167</v>
-      </c>
-      <c r="B19">
-        <v>4</v>
+      <c r="C18" s="16" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" s="17" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="17" t="s">
+        <v>165</v>
+      </c>
+      <c r="B19" s="17">
+        <v>4</v>
+      </c>
+      <c r="C19" s="16" t="s">
+        <v>203</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B20">
         <v>5</v>
@@ -4286,7 +4739,7 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B21">
         <v>6</v>
@@ -4294,7 +4747,7 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B22">
         <v>7</v>
@@ -4302,73 +4755,185 @@
     </row>
     <row r="23" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A23" s="11" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B23" s="11">
         <v>1</v>
       </c>
-      <c r="C23" s="42" t="s">
-        <v>93</v>
+      <c r="C23" s="40" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="24" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A24" s="11" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B24" s="11">
         <v>2</v>
       </c>
       <c r="C24" s="11" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="25" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A25" s="11" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B25" s="11">
         <v>3</v>
       </c>
       <c r="C25" s="11" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="26" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A26" s="11" t="s">
+        <v>166</v>
+      </c>
+      <c r="B26" s="11">
+        <v>4</v>
+      </c>
+      <c r="C26" s="11" t="s">
         <v>168</v>
-      </c>
-      <c r="B26" s="11">
-        <v>4</v>
-      </c>
-      <c r="C26" s="11" t="s">
-        <v>170</v>
       </c>
     </row>
     <row r="27" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A27" s="11" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B27" s="11">
         <v>5</v>
       </c>
       <c r="C27" s="11" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
-        <v>168</v>
-      </c>
-      <c r="B28">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="11" t="s">
+        <v>166</v>
+      </c>
+      <c r="B28" s="11">
         <v>6</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
-        <v>168</v>
-      </c>
-      <c r="B29">
+      <c r="C28" s="11" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="11" t="s">
+        <v>166</v>
+      </c>
+      <c r="B29" s="11">
         <v>7</v>
+      </c>
+      <c r="C29" s="11" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="11" t="s">
+        <v>166</v>
+      </c>
+      <c r="B30" s="11">
+        <v>8</v>
+      </c>
+      <c r="C30" s="11" t="s">
+        <v>208</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9DEFB68-FA96-CD44-92BB-68B17CEA3E86}">
+  <dimension ref="A1:B16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="44" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B2" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="44" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B4" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="44" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B6" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="44" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B8" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" s="44" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B10" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" s="44" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B12" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" s="44" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B14" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" s="44" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B16" t="s">
+        <v>194</v>
       </c>
     </row>
   </sheetData>

</xml_diff>